<commit_message>
Agrego posición de solicitaciones máximas
</commit_message>
<xml_diff>
--- a/Tarea 06/Vigas.xlsx
+++ b/Tarea 06/Vigas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ramos Ingenieria\12° Semestre\Proyecto de Hormigón Armado\Tarea 06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2C6F29-7649-4F1F-AF02-D950616A40E5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159EC714-E9CB-477E-82FB-E91EE8BB57F9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{B94BBB90-C174-4AC8-BDFB-4A9825C26EEC}"/>
   </bookViews>
@@ -72,35 +72,41 @@
     <t>$L^{-} [m]$</t>
   </si>
   <si>
-    <t>$L^{+} [m]$</t>
+    <t>${q^{-}}_{PP} [kgf/cm]$</t>
   </si>
   <si>
-    <t>${q^{-}}_{PP} [kgf/m]$</t>
+    <t>${q^{-}}_{SC} [kgf/cm]$</t>
   </si>
   <si>
-    <t>${q^{-}}_{SC} [kgf/m]$</t>
+    <t>$L^{+} [cm]$</t>
   </si>
   <si>
-    <t>${q^{+}}_{PP} [kgf/m]$</t>
+    <t>${q^{+}}_{PP} [kgf/cm]$</t>
   </si>
   <si>
-    <t>${q^{+}}_{SC} [kgf/m]$</t>
+    <t>${q^{+}}_{SC} [kgf/cm]$</t>
   </si>
   <si>
-    <t>$PP_{total} [kgf/m]$</t>
+    <t>posición [cm]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -119,26 +125,346 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1612,7 +1938,7 @@
         </row>
         <row r="65">
           <cell r="B65" t="str">
-            <v>$PP_l{osa} [kgf/m^2]$</v>
+            <v>PP_losa [kgf/m2]</v>
           </cell>
           <cell r="C65">
             <v>425.00000000000006</v>
@@ -2063,7 +2389,7 @@
       <sheetData sheetId="3">
         <row r="64">
           <cell r="B64" t="str">
-            <v>$SC [kgf/m^2]$</v>
+            <v>SC [kgf/m2]</v>
           </cell>
         </row>
       </sheetData>
@@ -2381,504 +2707,499 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F51FF3-724F-45F5-8F3F-FC55661E6BD0}">
-  <dimension ref="B2:O18"/>
+  <dimension ref="B1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="20.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
+    <col min="2" max="6" width="16.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="2" customWidth="1"/>
+    <col min="8" max="14" width="16.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" style="2" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" s="8" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="str">
+      <c r="C2" s="4" t="str">
+        <f>'[1]-1'!$B$65</f>
+        <v>PP_losa [kgf/m2]</v>
+      </c>
+      <c r="D2" s="4" t="str">
         <f>'[1]1'!$B$64</f>
-        <v>$SC [kgf/m^2]$</v>
-      </c>
-      <c r="D2" s="1" t="str">
+        <v>SC [kgf/m2]</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="4" t="str">
         <f>'[1]-1'!$B$65</f>
-        <v>$PP_l{osa} [kgf/m^2]$</v>
-      </c>
-      <c r="E2" s="3" t="s">
+        <v>PP_losa [kgf/m2]</v>
+      </c>
+      <c r="K2" s="4" t="str">
+        <f>'[1]1'!$B$64</f>
+        <v>SC [kgf/m2]</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="1" t="str">
-        <f>'[1]1'!$B$64</f>
-        <v>$SC [kgf/m^2]$</v>
-      </c>
-      <c r="K2" s="1" t="str">
-        <f>'[1]-1'!$B$65</f>
-        <v>$PP_l{osa} [kgf/m^2]$</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="10">
+        <f>HLOOKUP($B3,'[1]-1'!$C$46:$AE$69,D$13)</f>
+        <v>425.00000000000006</v>
+      </c>
+      <c r="D3" s="10">
         <f>HLOOKUP($B3,'[1]-1'!$C$46:$AE$69,C$13)</f>
         <v>500</v>
       </c>
-      <c r="D3" s="1">
-        <f>HLOOKUP($B3,'[1]-1'!$C$46:$AE$69,D$13)</f>
+      <c r="E3" s="10">
+        <v>1.77</v>
+      </c>
+      <c r="F3" s="10">
+        <v>178</v>
+      </c>
+      <c r="G3" s="11">
+        <f>C3*$E3/100</f>
+        <v>7.5225000000000009</v>
+      </c>
+      <c r="H3" s="12">
+        <f>D3*$E3/100</f>
+        <v>8.85</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="10">
+        <f>HLOOKUP($I3,'[1]-1'!$C$46:$AE$69,D$13)</f>
         <v>425.00000000000006</v>
       </c>
-      <c r="E3" s="3">
-        <f>D3</f>
-        <v>425.00000000000006</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1.77</v>
-      </c>
-      <c r="G3" s="1">
-        <f>$E3*F3</f>
-        <v>752.25000000000011</v>
-      </c>
-      <c r="H3" s="3">
-        <f>$C3*F3</f>
-        <v>885</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="K3" s="10">
         <f>HLOOKUP($I3,'[1]-1'!$C$46:$AE$69,C$13)</f>
         <v>500</v>
       </c>
-      <c r="K3" s="1">
-        <f>HLOOKUP($I3,'[1]-1'!$C$46:$AE$69,D$13)</f>
-        <v>425.00000000000006</v>
-      </c>
-      <c r="L3" s="3">
-        <f>K3</f>
-        <v>425.00000000000006</v>
-      </c>
-      <c r="M3" s="1">
+      <c r="L3" s="10">
         <v>2.77</v>
       </c>
-      <c r="N3" s="1">
-        <f>$L3*M3</f>
-        <v>1177.2500000000002</v>
-      </c>
-      <c r="O3" s="3">
-        <f>$J3*M3</f>
-        <v>1385</v>
+      <c r="M3" s="10">
+        <v>176</v>
+      </c>
+      <c r="N3" s="11">
+        <f>J3*$L3/100</f>
+        <v>11.772500000000003</v>
+      </c>
+      <c r="O3" s="12">
+        <f>K3*$L3/100</f>
+        <v>13.85</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="14">
+        <f>HLOOKUP($B4,'[1]-1'!$C$46:$AE$69,D$13)</f>
+        <v>425.00000000000006</v>
+      </c>
+      <c r="D4" s="14">
         <f>HLOOKUP($B4,'[1]-1'!$C$46:$AE$69,C$13)</f>
         <v>500</v>
       </c>
-      <c r="D4" s="1">
-        <f>HLOOKUP($B4,'[1]-1'!$C$46:$AE$69,D$13)</f>
+      <c r="E4" s="14">
+        <v>2.19</v>
+      </c>
+      <c r="F4" s="14">
+        <v>220</v>
+      </c>
+      <c r="G4" s="15">
+        <f>C4*$E4/100</f>
+        <v>9.307500000000001</v>
+      </c>
+      <c r="H4" s="16">
+        <f>D4*$E4/100</f>
+        <v>10.95</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="14">
+        <f>HLOOKUP($I4,'[1]-1'!$C$46:$AE$69,D$13)</f>
         <v>425.00000000000006</v>
       </c>
-      <c r="E4" s="3">
-        <f>D4</f>
-        <v>425.00000000000006</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2.19</v>
-      </c>
-      <c r="G4" s="1">
-        <f>$E4*F4</f>
-        <v>930.75000000000011</v>
-      </c>
-      <c r="H4" s="3">
-        <f>$C4*F4</f>
-        <v>1095</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="1">
+      <c r="K4" s="14">
         <f>HLOOKUP($I4,'[1]-1'!$C$46:$AE$69,C$13)</f>
         <v>500</v>
       </c>
-      <c r="K4" s="1">
-        <f>HLOOKUP($I4,'[1]-1'!$C$46:$AE$69,D$13)</f>
-        <v>425.00000000000006</v>
-      </c>
-      <c r="L4" s="3">
-        <f>K4</f>
-        <v>425.00000000000006</v>
-      </c>
-      <c r="M4" s="1">
+      <c r="L4" s="14">
         <v>2.85</v>
       </c>
-      <c r="N4" s="1">
-        <f>$L4*M4</f>
-        <v>1211.2500000000002</v>
-      </c>
-      <c r="O4" s="3">
-        <f>$J4*M4</f>
-        <v>1425</v>
+      <c r="M4" s="14">
+        <v>285</v>
+      </c>
+      <c r="N4" s="15">
+        <f t="shared" ref="N4:N5" si="0">J4*$L4/100</f>
+        <v>12.112500000000002</v>
+      </c>
+      <c r="O4" s="16">
+        <f t="shared" ref="O4:O5" si="1">K4*$L4/100</f>
+        <v>14.25</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="18">
+        <f>HLOOKUP($B5,'[1]-1'!$C$46:$AE$69,D$13)</f>
+        <v>425.00000000000006</v>
+      </c>
+      <c r="D5" s="18">
         <f>HLOOKUP($B5,'[1]-1'!$C$46:$AE$69,C$13)</f>
         <v>500</v>
       </c>
-      <c r="D5" s="4">
-        <f>HLOOKUP($B5,'[1]-1'!$C$46:$AE$69,D$13)</f>
+      <c r="E5" s="19">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="F5" s="19">
+        <v>498</v>
+      </c>
+      <c r="G5" s="20">
+        <f>C5*$E5/100</f>
+        <v>10.8375</v>
+      </c>
+      <c r="H5" s="21">
+        <f>D5*$E5/100</f>
+        <v>12.75</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="18">
+        <f>HLOOKUP($I5,'[1]-1'!$C$46:$AE$69,D$13)</f>
         <v>425.00000000000006</v>
       </c>
-      <c r="E5" s="4">
-        <f>D5</f>
-        <v>425.00000000000006</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="G5" s="1">
-        <f>$E5*F5</f>
-        <v>1083.75</v>
-      </c>
-      <c r="H5" s="3">
-        <f t="shared" ref="H5" si="0">$C5*F5</f>
-        <v>1275</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="4">
+      <c r="K5" s="18">
         <f>HLOOKUP($I5,'[1]-1'!$C$46:$AE$69,C$13)</f>
         <v>500</v>
       </c>
-      <c r="K5" s="4">
-        <f>HLOOKUP($I5,'[1]-1'!$C$46:$AE$69,D$13)</f>
-        <v>425.00000000000006</v>
-      </c>
-      <c r="L5" s="5">
-        <f>K5</f>
-        <v>425.00000000000006</v>
-      </c>
-      <c r="M5" s="1">
+      <c r="L5" s="19">
         <v>2.85</v>
       </c>
-      <c r="N5" s="1">
-        <f>$L5*M5</f>
-        <v>1211.2500000000002</v>
-      </c>
-      <c r="O5" s="3">
-        <f>$J5*M5</f>
-        <v>1425</v>
+      <c r="M5" s="19">
+        <v>750</v>
+      </c>
+      <c r="N5" s="20">
+        <f t="shared" si="0"/>
+        <v>12.112500000000002</v>
+      </c>
+      <c r="O5" s="21">
+        <f t="shared" si="1"/>
+        <v>14.25</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="1">
+      <c r="B6" s="22"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="24">
         <v>2.5</v>
       </c>
-      <c r="G6" s="2">
-        <f>$E5*F6</f>
-        <v>1062.5000000000002</v>
-      </c>
-      <c r="H6" s="2">
-        <f>$C5*F6</f>
-        <v>1250</v>
-      </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="1">
+      <c r="F6" s="24">
+        <v>252</v>
+      </c>
+      <c r="G6" s="25">
+        <f>C5*$E6/100</f>
+        <v>10.625000000000002</v>
+      </c>
+      <c r="H6" s="26">
+        <f>D5*$E6/100</f>
+        <v>12.5</v>
+      </c>
+      <c r="I6" s="22"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="24">
         <v>2.84</v>
       </c>
-      <c r="N6" s="1">
-        <f>$L5*M6</f>
-        <v>1207</v>
-      </c>
-      <c r="O6" s="2">
-        <f>$J5*M6</f>
-        <v>1420</v>
+      <c r="M6" s="24">
+        <v>273</v>
+      </c>
+      <c r="N6" s="25">
+        <f>J5*$L6/100</f>
+        <v>12.07</v>
+      </c>
+      <c r="O6" s="26">
+        <f>K5*$L6/100</f>
+        <v>14.2</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="18">
+        <f>HLOOKUP($B7,'[1]-1'!$C$46:$AE$69,D$13)</f>
+        <v>425.00000000000006</v>
+      </c>
+      <c r="D7" s="18">
         <f>HLOOKUP($B7,'[1]-1'!$C$46:$AE$69,C$13)</f>
         <v>500</v>
       </c>
-      <c r="D7" s="4">
-        <f>HLOOKUP($B7,'[1]-1'!$C$46:$AE$69,D$13)</f>
+      <c r="E7" s="19">
+        <v>2.54</v>
+      </c>
+      <c r="F7" s="19">
+        <v>500</v>
+      </c>
+      <c r="G7" s="20">
+        <f>C7*$E7/100</f>
+        <v>10.795000000000002</v>
+      </c>
+      <c r="H7" s="21">
+        <f>D7*$E7/100</f>
+        <v>12.7</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="18">
+        <f>HLOOKUP($I7,'[1]-1'!$C$46:$AE$69,D$13)</f>
         <v>425.00000000000006</v>
       </c>
-      <c r="E7" s="4">
-        <f>D7</f>
-        <v>425.00000000000006</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2.54</v>
-      </c>
-      <c r="G7" s="1">
-        <f>$E7*F7</f>
-        <v>1079.5000000000002</v>
-      </c>
-      <c r="H7" s="3">
-        <f t="shared" ref="H7" si="1">$C7*F7</f>
-        <v>1270</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" s="4">
+      <c r="K7" s="18">
         <f>HLOOKUP($I7,'[1]-1'!$C$46:$AE$69,C$13)</f>
         <v>500</v>
       </c>
-      <c r="K7" s="4">
-        <f>HLOOKUP($I7,'[1]-1'!$C$46:$AE$69,D$13)</f>
-        <v>425.00000000000006</v>
-      </c>
-      <c r="L7" s="4">
-        <f>K7</f>
-        <v>425.00000000000006</v>
-      </c>
-      <c r="M7" s="1">
+      <c r="L7" s="19">
         <v>3.04</v>
       </c>
-      <c r="N7" s="1">
-        <f>$L7*M7</f>
-        <v>1292.0000000000002</v>
-      </c>
-      <c r="O7" s="3">
-        <f>$J7*M7</f>
-        <v>1520</v>
+      <c r="M7" s="19">
+        <v>442</v>
+      </c>
+      <c r="N7" s="20">
+        <f>J7*$L7/100</f>
+        <v>12.920000000000002</v>
+      </c>
+      <c r="O7" s="21">
+        <f>K7*$L7/100</f>
+        <v>15.2</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="1">
+      <c r="B8" s="22"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="24">
         <v>2.48</v>
       </c>
-      <c r="G8" s="2">
-        <f>$E7*F8</f>
-        <v>1054.0000000000002</v>
-      </c>
-      <c r="H8" s="2">
-        <f>$C7*F8</f>
-        <v>1240</v>
-      </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="1">
+      <c r="F8" s="24">
+        <v>250</v>
+      </c>
+      <c r="G8" s="25">
+        <f>C7*$E8/100</f>
+        <v>10.540000000000003</v>
+      </c>
+      <c r="H8" s="26">
+        <f>D7*$E8/100</f>
+        <v>12.4</v>
+      </c>
+      <c r="I8" s="22"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="24">
         <v>2.84</v>
       </c>
-      <c r="N8" s="2">
-        <f>$L7*M8</f>
-        <v>1207</v>
-      </c>
-      <c r="O8" s="2">
-        <f>$J7*M8</f>
-        <v>1420</v>
+      <c r="M8" s="24">
+        <v>280</v>
+      </c>
+      <c r="N8" s="25">
+        <f>J7*$L8/100</f>
+        <v>12.07</v>
+      </c>
+      <c r="O8" s="26">
+        <f>K7*$L8/100</f>
+        <v>14.2</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="18">
+        <f>HLOOKUP($B9,'[1]-1'!$C$46:$AE$69,D$13)</f>
+        <v>425.00000000000006</v>
+      </c>
+      <c r="D9" s="18">
         <f>HLOOKUP($B9,'[1]-1'!$C$46:$AE$69,C$13)</f>
         <v>500</v>
       </c>
-      <c r="D9" s="4">
-        <f>HLOOKUP($B9,'[1]-1'!$C$46:$AE$69,D$13)</f>
+      <c r="E9" s="19">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="F9" s="19">
+        <v>501</v>
+      </c>
+      <c r="G9" s="20">
+        <f>C9*$E9/100</f>
+        <v>10.6675</v>
+      </c>
+      <c r="H9" s="21">
+        <f>D9*$E9/100</f>
+        <v>12.55</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="18">
+        <f>HLOOKUP($I9,'[1]-1'!$C$46:$AE$69,D$13)</f>
         <v>425.00000000000006</v>
       </c>
-      <c r="E9" s="4">
-        <f>D9</f>
-        <v>425.00000000000006</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2.5099999999999998</v>
-      </c>
-      <c r="G9" s="1">
-        <f>$E9*F9</f>
-        <v>1066.75</v>
-      </c>
-      <c r="H9" s="3">
-        <f t="shared" ref="H9" si="2">$C9*F9</f>
-        <v>1255</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="4">
+      <c r="K9" s="18">
         <f>HLOOKUP($I9,'[1]-1'!$C$46:$AE$69,C$13)</f>
         <v>500</v>
       </c>
-      <c r="K9" s="4">
-        <f>HLOOKUP($I9,'[1]-1'!$C$46:$AE$69,D$13)</f>
-        <v>425.00000000000006</v>
-      </c>
-      <c r="L9" s="4">
-        <f>K9</f>
-        <v>425.00000000000006</v>
-      </c>
-      <c r="M9" s="1">
+      <c r="L9" s="19">
         <v>2.87</v>
       </c>
-      <c r="N9" s="1">
-        <f>$L9*M9</f>
-        <v>1219.7500000000002</v>
-      </c>
-      <c r="O9" s="3">
-        <f>$J9*M9</f>
-        <v>1435</v>
+      <c r="M9" s="19">
+        <v>459</v>
+      </c>
+      <c r="N9" s="20">
+        <f>J9*$L9/100</f>
+        <v>12.197500000000002</v>
+      </c>
+      <c r="O9" s="21">
+        <f>K9*$L9/100</f>
+        <v>14.35</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="1">
+      <c r="B10" s="22"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="24">
         <v>2.4700000000000002</v>
       </c>
-      <c r="G10" s="2">
-        <f>$E9*F10</f>
-        <v>1049.7500000000002</v>
-      </c>
-      <c r="H10" s="2">
-        <f>$C9*F10</f>
-        <v>1235</v>
-      </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="1">
+      <c r="F10" s="24">
+        <v>251</v>
+      </c>
+      <c r="G10" s="25">
+        <f>C9*$E10/100</f>
+        <v>10.497500000000002</v>
+      </c>
+      <c r="H10" s="26">
+        <f>D9*$E10/100</f>
+        <v>12.35</v>
+      </c>
+      <c r="I10" s="22"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="24">
         <v>2.98</v>
       </c>
-      <c r="N10" s="2">
-        <f>$L9*M10</f>
-        <v>1266.5000000000002</v>
-      </c>
-      <c r="O10" s="2">
-        <f>$J9*M10</f>
-        <v>1490</v>
+      <c r="M10" s="24">
+        <v>293</v>
+      </c>
+      <c r="N10" s="25">
+        <f>J9*$L10/100</f>
+        <v>12.665000000000003</v>
+      </c>
+      <c r="O10" s="26">
+        <f>K9*$L10/100</f>
+        <v>14.9</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+    <row r="11" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="28">
+        <f>HLOOKUP($B11,'[1]-1'!$C$46:$AE$69,D$13)</f>
+        <v>425.00000000000006</v>
+      </c>
+      <c r="D11" s="28">
         <f>HLOOKUP($B11,'[1]-1'!$C$46:$AE$69,C$13)</f>
         <v>500</v>
       </c>
-      <c r="D11" s="1">
-        <f>HLOOKUP($B11,'[1]-1'!$C$46:$AE$69,D$13)</f>
+      <c r="E11" s="28">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="F11" s="28">
+        <v>255</v>
+      </c>
+      <c r="G11" s="29">
+        <f>C11*$E11/100</f>
+        <v>10.497500000000002</v>
+      </c>
+      <c r="H11" s="30">
+        <f>D11*$E11/100</f>
+        <v>12.35</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="28">
+        <f>HLOOKUP($I11,'[1]-1'!$C$46:$AE$69,D$13)</f>
         <v>425.00000000000006</v>
       </c>
-      <c r="E11" s="3">
-        <f>D11</f>
-        <v>425.00000000000006</v>
-      </c>
-      <c r="F11" s="1">
-        <v>2.4700000000000002</v>
-      </c>
-      <c r="G11" s="1">
-        <f>$E11*F11</f>
-        <v>1049.7500000000002</v>
-      </c>
-      <c r="H11" s="3">
-        <f>$C11*F11</f>
-        <v>1235</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" s="1">
+      <c r="K11" s="28">
         <f>HLOOKUP($I11,'[1]-1'!$C$46:$AE$69,C$13)</f>
         <v>500</v>
       </c>
-      <c r="K11" s="1">
-        <f>HLOOKUP($I11,'[1]-1'!$C$46:$AE$69,D$13)</f>
-        <v>425.00000000000006</v>
-      </c>
-      <c r="L11" s="3">
-        <f>K11</f>
-        <v>425.00000000000006</v>
-      </c>
-      <c r="M11" s="1">
+      <c r="L11" s="28">
         <v>2.5499999999999998</v>
       </c>
-      <c r="N11" s="1">
-        <f>$L11*M11</f>
-        <v>1083.75</v>
-      </c>
-      <c r="O11" s="3">
-        <f>$J11*M11</f>
-        <v>1275</v>
+      <c r="M11" s="28">
+        <v>252</v>
+      </c>
+      <c r="N11" s="29">
+        <f>J11*$L11/100</f>
+        <v>10.8375</v>
+      </c>
+      <c r="O11" s="30">
+        <f>K11*$L11/100</f>
+        <v>12.75</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="2"/>
-      <c r="O12" s="3"/>
+    <row r="12" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="31"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="31"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="1">
         <v>19</v>
       </c>
@@ -2886,48 +3207,40 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C16" s="1" t="s">
+    <row r="14" spans="2:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="33" t="s">
         <v>12</v>
+      </c>
+      <c r="C14" s="34">
+        <f>0.3*0.5*'[1]-1'!L$7</f>
+        <v>375</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="4">
-        <f>0.3*0.5*'[1]-1'!L$7</f>
-        <v>375</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="4"/>
+      <c r="C17" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
+  <mergeCells count="18">
     <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D5:D6"/>
     <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="C9:C10"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="I7:I8"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
     <mergeCell ref="I9:I10"/>
+    <mergeCell ref="K9:K10"/>
     <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="J7:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agrega tablas con esfuerzos de viga estatica SAP
</commit_message>
<xml_diff>
--- a/Tarea 06/Vigas.xlsx
+++ b/Tarea 06/Vigas.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ramos Ingenieria\12° Semestre\Proyecto de Hormigón Armado\Tarea 06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159EC714-E9CB-477E-82FB-E91EE8BB57F9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCCC278-FDE6-4436-B9F7-3009DE656639}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{B94BBB90-C174-4AC8-BDFB-4A9825C26EEC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" activeTab="1" xr2:uid="{B94BBB90-C174-4AC8-BDFB-4A9825C26EEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Esfuerzos Viga Estática" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="35">
   <si>
     <t>0101</t>
   </si>
@@ -89,12 +90,57 @@
   <si>
     <t>posición [cm]</t>
   </si>
+  <si>
+    <t>TABLE:  Element Forces - Frames</t>
+  </si>
+  <si>
+    <t>Frame</t>
+  </si>
+  <si>
+    <t>Station</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>Kgf</t>
+  </si>
+  <si>
+    <t>Kgf-cm</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,16 +154,36 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="49"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="41"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -355,11 +421,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -466,6 +560,23 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2709,8 +2820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F51FF3-724F-45F5-8F3F-FC55661E6BD0}">
   <dimension ref="B1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -2865,7 +2976,7 @@
         <v>2.85</v>
       </c>
       <c r="M4" s="14">
-        <v>285</v>
+        <v>149</v>
       </c>
       <c r="N4" s="15">
         <f t="shared" ref="N4:N5" si="0">J4*$L4/100</f>
@@ -3243,4 +3354,1133 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA457D5-97E1-45EE-9640-8E8A35FB636C}">
+  <dimension ref="A1:D80"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="36">
+        <v>0</v>
+      </c>
+      <c r="C4" s="36">
+        <v>-4770.4399999999996</v>
+      </c>
+      <c r="D4" s="44">
+        <v>1.1640000000000001E-10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="36">
+        <v>50</v>
+      </c>
+      <c r="C5" s="36">
+        <v>-4229.8500000000004</v>
+      </c>
+      <c r="D5" s="36">
+        <v>227710.28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="36">
+        <v>100</v>
+      </c>
+      <c r="C6" s="36">
+        <v>-3040.58</v>
+      </c>
+      <c r="D6" s="36">
+        <v>412173.92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="36">
+        <v>150</v>
+      </c>
+      <c r="C7" s="36">
+        <v>-1202.6199999999999</v>
+      </c>
+      <c r="D7" s="36">
+        <v>520956.74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="36">
+        <v>200</v>
+      </c>
+      <c r="C8" s="36">
+        <v>1284.02</v>
+      </c>
+      <c r="D8" s="36">
+        <v>521624.59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="36">
+        <v>250</v>
+      </c>
+      <c r="C9" s="36">
+        <v>4419.3500000000004</v>
+      </c>
+      <c r="D9" s="36">
+        <v>381743.27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="36">
+        <v>300</v>
+      </c>
+      <c r="C10" s="36">
+        <v>7633.23</v>
+      </c>
+      <c r="D10" s="36">
+        <v>77738.47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="36">
+        <v>350</v>
+      </c>
+      <c r="C11" s="36">
+        <v>10183.9</v>
+      </c>
+      <c r="D11" s="36">
+        <v>-370468.71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="36">
+        <v>400</v>
+      </c>
+      <c r="C12" s="36">
+        <v>12067.59</v>
+      </c>
+      <c r="D12" s="36">
+        <v>-929535.09</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="36">
+        <v>450</v>
+      </c>
+      <c r="C13" s="36">
+        <v>13284.31</v>
+      </c>
+      <c r="D13" s="36">
+        <v>-1566111.76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="36">
+        <v>500</v>
+      </c>
+      <c r="C14" s="36">
+        <v>13834.05</v>
+      </c>
+      <c r="D14" s="36">
+        <v>-2246849.7999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="36">
+        <v>0</v>
+      </c>
+      <c r="C15" s="36">
+        <v>-17845.16</v>
+      </c>
+      <c r="D15" s="36">
+        <v>-2246849.7999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="36">
+        <v>50</v>
+      </c>
+      <c r="C16" s="36">
+        <v>-17301.189999999999</v>
+      </c>
+      <c r="D16" s="36">
+        <v>-1365460.12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="36">
+        <v>100</v>
+      </c>
+      <c r="C17" s="36">
+        <v>-16101.76</v>
+      </c>
+      <c r="D17" s="36">
+        <v>-527655.43999999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="36">
+        <v>150</v>
+      </c>
+      <c r="C18" s="36">
+        <v>-14246.88</v>
+      </c>
+      <c r="D18" s="36">
+        <v>233791.71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="36">
+        <v>200</v>
+      </c>
+      <c r="C19" s="36">
+        <v>-11736.56</v>
+      </c>
+      <c r="D19" s="36">
+        <v>886108.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="36">
+        <v>250</v>
+      </c>
+      <c r="C20" s="36">
+        <v>-8570.7800000000007</v>
+      </c>
+      <c r="D20" s="36">
+        <v>1396523.28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="36">
+        <v>300</v>
+      </c>
+      <c r="C21" s="36">
+        <v>-4895.6099999999997</v>
+      </c>
+      <c r="D21" s="36">
+        <v>1734599.49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="36">
+        <v>350</v>
+      </c>
+      <c r="C22" s="36">
+        <v>-1085.48</v>
+      </c>
+      <c r="D22" s="36">
+        <v>1884141.96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="36">
+        <v>400</v>
+      </c>
+      <c r="C23" s="36">
+        <v>2728.29</v>
+      </c>
+      <c r="D23" s="36">
+        <v>1843086.94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="36">
+        <v>450</v>
+      </c>
+      <c r="C24" s="36">
+        <v>6545.72</v>
+      </c>
+      <c r="D24" s="36">
+        <v>1611251.78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="36">
+        <v>500</v>
+      </c>
+      <c r="C25" s="36">
+        <v>10265.52</v>
+      </c>
+      <c r="D25" s="36">
+        <v>1189838.1299999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="36">
+        <v>550</v>
+      </c>
+      <c r="C26" s="36">
+        <v>13512.1</v>
+      </c>
+      <c r="D26" s="36">
+        <v>592593.55000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="36">
+        <v>600</v>
+      </c>
+      <c r="C27" s="36">
+        <v>16085.34</v>
+      </c>
+      <c r="D27" s="36">
+        <v>-150148.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="36">
+        <v>650</v>
+      </c>
+      <c r="C28" s="36">
+        <v>17985.16</v>
+      </c>
+      <c r="D28" s="36">
+        <v>-1004717.06</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="36">
+        <v>700</v>
+      </c>
+      <c r="C29" s="36">
+        <v>19211.54</v>
+      </c>
+      <c r="D29" s="36">
+        <v>-1937440.55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="36">
+        <v>750</v>
+      </c>
+      <c r="C30" s="36">
+        <v>19764.509999999998</v>
+      </c>
+      <c r="D30" s="36">
+        <v>-2914647.79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="36">
+        <v>0</v>
+      </c>
+      <c r="C31" s="36">
+        <v>-18392.66</v>
+      </c>
+      <c r="D31" s="36">
+        <v>-2914647.79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="36">
+        <v>50</v>
+      </c>
+      <c r="C32" s="36">
+        <v>-17847.88</v>
+      </c>
+      <c r="D32" s="36">
+        <v>-2005896.43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="36">
+        <v>100</v>
+      </c>
+      <c r="C33" s="36">
+        <v>-16646.05</v>
+      </c>
+      <c r="D33" s="36">
+        <v>-1140810.47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="36">
+        <v>150</v>
+      </c>
+      <c r="C34" s="36">
+        <v>-14787.15</v>
+      </c>
+      <c r="D34" s="36">
+        <v>-352242.82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="36">
+        <v>200</v>
+      </c>
+      <c r="C35" s="36">
+        <v>-12271.2</v>
+      </c>
+      <c r="D35" s="36">
+        <v>326953.57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="36">
+        <v>250</v>
+      </c>
+      <c r="C36" s="36">
+        <v>-9098.18</v>
+      </c>
+      <c r="D36" s="36">
+        <v>863925.79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="36">
+        <v>300</v>
+      </c>
+      <c r="C37" s="36">
+        <v>-5449.93</v>
+      </c>
+      <c r="D37" s="36">
+        <v>1228617.83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="36">
+        <v>350</v>
+      </c>
+      <c r="C38" s="36">
+        <v>-1700.81</v>
+      </c>
+      <c r="D38" s="36">
+        <v>1407587.91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="36">
+        <v>400</v>
+      </c>
+      <c r="C39" s="36">
+        <v>2096.66</v>
+      </c>
+      <c r="D39" s="36">
+        <v>1397893.28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="36">
+        <v>450</v>
+      </c>
+      <c r="C40" s="36">
+        <v>5937.82</v>
+      </c>
+      <c r="D40" s="36">
+        <v>1197128.75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="36">
+        <v>500</v>
+      </c>
+      <c r="C41" s="36">
+        <v>9591.9699999999993</v>
+      </c>
+      <c r="D41" s="36">
+        <v>807570.01</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="36">
+        <v>550</v>
+      </c>
+      <c r="C42" s="36">
+        <v>12760.43</v>
+      </c>
+      <c r="D42" s="36">
+        <v>246026.46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="36">
+        <v>600</v>
+      </c>
+      <c r="C43" s="36">
+        <v>15272.84</v>
+      </c>
+      <c r="D43" s="36">
+        <v>-457538.92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="36">
+        <v>650</v>
+      </c>
+      <c r="C44" s="36">
+        <v>17129.21</v>
+      </c>
+      <c r="D44" s="36">
+        <v>-1270323.76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="36">
+        <v>700</v>
+      </c>
+      <c r="C45" s="36">
+        <v>18329.53</v>
+      </c>
+      <c r="D45" s="36">
+        <v>-2159525.75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46" s="36">
+        <v>750</v>
+      </c>
+      <c r="C46" s="36">
+        <v>18873.8</v>
+      </c>
+      <c r="D46" s="36">
+        <v>-3092342.54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="36">
+        <v>0</v>
+      </c>
+      <c r="C47" s="36">
+        <v>-20219.28</v>
+      </c>
+      <c r="D47" s="36">
+        <v>-3092342.54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48" s="36">
+        <v>50</v>
+      </c>
+      <c r="C48" s="36">
+        <v>-19750.099999999999</v>
+      </c>
+      <c r="D48" s="36">
+        <v>-2091000.44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" s="36">
+        <v>100</v>
+      </c>
+      <c r="C49" s="36">
+        <v>-18775.05</v>
+      </c>
+      <c r="D49" s="36">
+        <v>-1125764.1200000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50" s="36">
+        <v>150</v>
+      </c>
+      <c r="C50" s="36">
+        <v>-17294.13</v>
+      </c>
+      <c r="D50" s="36">
+        <v>-221926.9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" s="36">
+        <v>200</v>
+      </c>
+      <c r="C51" s="36">
+        <v>-15307.35</v>
+      </c>
+      <c r="D51" s="36">
+        <v>595217.92000000004</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" s="36">
+        <v>250</v>
+      </c>
+      <c r="C52" s="36">
+        <v>-12814.7</v>
+      </c>
+      <c r="D52" s="36">
+        <v>1300377</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" s="36">
+        <v>300</v>
+      </c>
+      <c r="C53" s="36">
+        <v>-8339.69</v>
+      </c>
+      <c r="D53" s="36">
+        <v>1831455.76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" s="36">
+        <v>350</v>
+      </c>
+      <c r="C54" s="36">
+        <v>-3765.03</v>
+      </c>
+      <c r="D54" s="36">
+        <v>2134059.37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55" s="36">
+        <v>400</v>
+      </c>
+      <c r="C55" s="36">
+        <v>806.19</v>
+      </c>
+      <c r="D55" s="36">
+        <v>2208015.88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B56" s="36">
+        <v>450</v>
+      </c>
+      <c r="C56" s="36">
+        <v>5373.97</v>
+      </c>
+      <c r="D56" s="36">
+        <v>2053497.33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B57" s="36">
+        <v>500</v>
+      </c>
+      <c r="C57" s="36">
+        <v>9872.67</v>
+      </c>
+      <c r="D57" s="36">
+        <v>1670741.37</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B58" s="36">
+        <v>550</v>
+      </c>
+      <c r="C58" s="36">
+        <v>12706.97</v>
+      </c>
+      <c r="D58" s="36">
+        <v>1105550.75</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B59" s="36">
+        <v>600</v>
+      </c>
+      <c r="C59" s="36">
+        <v>15373.4</v>
+      </c>
+      <c r="D59" s="36">
+        <v>402841.96</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B60" s="36">
+        <v>650</v>
+      </c>
+      <c r="C60" s="36">
+        <v>17871.939999999999</v>
+      </c>
+      <c r="D60" s="36">
+        <v>-428991.08</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61" s="36">
+        <v>700</v>
+      </c>
+      <c r="C61" s="36">
+        <v>20202.61</v>
+      </c>
+      <c r="D61" s="36">
+        <v>-1381554.44</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B62" s="36">
+        <v>750</v>
+      </c>
+      <c r="C62" s="36">
+        <v>22365.4</v>
+      </c>
+      <c r="D62" s="36">
+        <v>-2446454.19</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" s="36">
+        <v>0</v>
+      </c>
+      <c r="C63" s="36">
+        <v>-14560.05</v>
+      </c>
+      <c r="D63" s="36">
+        <v>-2446454.19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B64" s="36">
+        <v>48.555999999999997</v>
+      </c>
+      <c r="C64" s="36">
+        <v>-13900.95</v>
+      </c>
+      <c r="D64" s="36">
+        <v>-1751849.93</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B65" s="36">
+        <v>97.111000000000004</v>
+      </c>
+      <c r="C65" s="36">
+        <v>-12343.67</v>
+      </c>
+      <c r="D65" s="36">
+        <v>-1111054.42</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B66" s="36">
+        <v>145.667</v>
+      </c>
+      <c r="C66" s="36">
+        <v>-9888.2000000000007</v>
+      </c>
+      <c r="D66" s="36">
+        <v>-567679.65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B67" s="36">
+        <v>194.22200000000001</v>
+      </c>
+      <c r="C67" s="36">
+        <v>-6790.74</v>
+      </c>
+      <c r="D67" s="36">
+        <v>-161475.72</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B68" s="36">
+        <v>242.77799999999999</v>
+      </c>
+      <c r="C68" s="36">
+        <v>-3452.53</v>
+      </c>
+      <c r="D68" s="36">
+        <v>87315.47</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B69" s="36">
+        <v>291.33300000000003</v>
+      </c>
+      <c r="C69" s="36">
+        <v>-338.8</v>
+      </c>
+      <c r="D69" s="36">
+        <v>178099.25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B70" s="36">
+        <v>339.88900000000001</v>
+      </c>
+      <c r="C70" s="36">
+        <v>2463.1999999999998</v>
+      </c>
+      <c r="D70" s="36">
+        <v>125262.08</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B71" s="36">
+        <v>388.44400000000002</v>
+      </c>
+      <c r="C71" s="36">
+        <v>4953.4799999999996</v>
+      </c>
+      <c r="D71" s="36">
+        <v>-56059.82</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B72" s="36">
+        <v>437</v>
+      </c>
+      <c r="C72" s="36">
+        <v>7132.02</v>
+      </c>
+      <c r="D72" s="36">
+        <v>-350730.22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B73" s="36">
+        <v>0</v>
+      </c>
+      <c r="C73" s="36">
+        <v>-6811.32</v>
+      </c>
+      <c r="D73" s="36">
+        <v>-350730.22</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B74" s="36">
+        <v>49</v>
+      </c>
+      <c r="C74" s="36">
+        <v>-6195.54</v>
+      </c>
+      <c r="D74" s="36">
+        <v>-28763.79</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B75" s="36">
+        <v>98</v>
+      </c>
+      <c r="C75" s="36">
+        <v>-4772.05</v>
+      </c>
+      <c r="D75" s="36">
+        <v>243240.48</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B76" s="36">
+        <v>147</v>
+      </c>
+      <c r="C76" s="36">
+        <v>-2540.85</v>
+      </c>
+      <c r="D76" s="36">
+        <v>425704.73</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B77" s="36">
+        <v>196</v>
+      </c>
+      <c r="C77" s="36">
+        <v>369.52</v>
+      </c>
+      <c r="D77" s="36">
+        <v>479878.86</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B78" s="36">
+        <v>245</v>
+      </c>
+      <c r="C78" s="36">
+        <v>2729.01</v>
+      </c>
+      <c r="D78" s="36">
+        <v>400457.34</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B79" s="36">
+        <v>294</v>
+      </c>
+      <c r="C79" s="36">
+        <v>4229.47</v>
+      </c>
+      <c r="D79" s="36">
+        <v>226466.96</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B80" s="36">
+        <v>343</v>
+      </c>
+      <c r="C80" s="36">
+        <v>4870.91</v>
+      </c>
+      <c r="D80" s="36">
+        <v>-9.8879999999999999E-11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Planilla de vigas listas
</commit_message>
<xml_diff>
--- a/Tarea 06/Vigas.xlsx
+++ b/Tarea 06/Vigas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ramos Ingenieria\12° Semestre\Proyecto de Hormigón Armado\Tarea 06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53D27C2-B438-4819-AB36-4401B032E87A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA902249-799C-4000-BFAF-7A556FDBD094}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{B94BBB90-C174-4AC8-BDFB-4A9825C26EEC}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="70">
   <si>
     <t>0101</t>
   </si>
@@ -88,6 +88,15 @@
     <t>${q^{+}}_{SC} [kgf/cm]$</t>
   </si>
   <si>
+    <t>PP</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>L [cm]</t>
+  </si>
+  <si>
     <t>posición [cm]</t>
   </si>
   <si>
@@ -139,41 +148,104 @@
     <t>ABS</t>
   </si>
   <si>
-    <t>$[tonf \cdot m]$</t>
-  </si>
-  <si>
-    <t>$[kgf \cdot cm]$</t>
-  </si>
-  <si>
-    <t>Vu</t>
-  </si>
-  <si>
-    <t>$[kgf]$</t>
-  </si>
-  <si>
-    <t>$[tonf]$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mu </t>
-  </si>
-  <si>
     <t>Armadura</t>
   </si>
   <si>
     <t>$2 \phi 32$</t>
   </si>
   <si>
-    <t>$2 \phi 36$</t>
-  </si>
-  <si>
     <t>$E \phi 12 @ 20$</t>
+  </si>
+  <si>
+    <t>Vigas Sísmica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eje C </t>
+  </si>
+  <si>
+    <t>Vu [tonf]</t>
+  </si>
+  <si>
+    <t>$Mu [tonf \cdot m] $</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nivel 2</t>
+  </si>
+  <si>
+    <t>(11-12)</t>
+  </si>
+  <si>
+    <t>$L:1+1\phi 10$</t>
+  </si>
+  <si>
+    <t>Sismo</t>
+  </si>
+  <si>
+    <t>ETABS</t>
+  </si>
+  <si>
+    <t>SAP</t>
+  </si>
+  <si>
+    <t>$M [tonf \cdot m] $</t>
+  </si>
+  <si>
+    <t>$V [tonf]$</t>
+  </si>
+  <si>
+    <t>Esfuerzo</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>F'</t>
+  </si>
+  <si>
+    <t>Estribos</t>
+  </si>
+  <si>
+    <t>Barras laterales</t>
+  </si>
+  <si>
+    <t>Viga Estática</t>
+  </si>
+  <si>
+    <t>Nivel -1</t>
+  </si>
+  <si>
+    <t>$1,2 \dot PP+1 \cdot SC+1,4 \cdot Sismo$</t>
+  </si>
+  <si>
+    <t>$E \phi 10 @ 20$</t>
+  </si>
+  <si>
+    <t>Eje K</t>
+  </si>
+  <si>
+    <t>(10-11)</t>
+  </si>
+  <si>
+    <t>$4 \phi 28$</t>
+  </si>
+  <si>
+    <t>$3 \phi 25$</t>
+  </si>
+  <si>
+    <t>VI25/180 G35</t>
+  </si>
+  <si>
+    <t>VI25/168 G35</t>
+  </si>
+  <si>
+    <t>$1,2 \cdot PP+1,6 \dot SC$</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,8 +267,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,8 +294,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="32">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -515,25 +600,8 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -541,55 +609,8 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="medium">
@@ -601,7 +622,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -703,6 +724,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -734,50 +758,59 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3020,10 +3053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F51FF3-724F-45F5-8F3F-FC55661E6BD0}">
-  <dimension ref="B1:O19"/>
+  <dimension ref="B2:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31:J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -3037,297 +3070,217 @@
     <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:15" s="8" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B2" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="64" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:15" s="8" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="str">
+      <c r="C4" s="4" t="str">
         <f>'[1]-1'!$B$65</f>
         <v>PP_losa [kgf/m2]</v>
       </c>
-      <c r="D2" s="4" t="str">
+      <c r="D4" s="4" t="str">
         <f>'[1]1'!$B$64</f>
         <v>SC [kgf/m2]</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="F4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="4" t="str">
+      <c r="J4" s="4" t="str">
         <f>'[1]-1'!$B$65</f>
         <v>PP_losa [kgf/m2]</v>
       </c>
-      <c r="K2" s="4" t="str">
+      <c r="K4" s="4" t="str">
         <f>'[1]1'!$B$64</f>
         <v>SC [kgf/m2]</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="M4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O4" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10">
-        <f>HLOOKUP($B3,'[1]-1'!$C$46:$AE$69,D$13)</f>
+      <c r="C5" s="10">
+        <f>HLOOKUP($B5,'[1]-1'!$C$46:$AE$69,D$15)</f>
         <v>425.00000000000006</v>
       </c>
-      <c r="D3" s="10">
-        <f>HLOOKUP($B3,'[1]-1'!$C$46:$AE$69,C$13)</f>
+      <c r="D5" s="10">
+        <f>HLOOKUP($B5,'[1]-1'!$C$46:$AE$69,C$15)</f>
         <v>500</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E5" s="10">
         <v>1.77</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F5" s="10">
         <v>178</v>
       </c>
-      <c r="G3" s="11">
-        <f>C3*$E3/100</f>
+      <c r="G5" s="11">
+        <f>C5*$E5/100</f>
         <v>7.5225000000000009</v>
       </c>
-      <c r="H3" s="12">
-        <f>D3*$E3/100</f>
+      <c r="H5" s="12">
+        <f>D5*$E5/100</f>
         <v>8.85</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="10">
-        <f>HLOOKUP($I3,'[1]-1'!$C$46:$AE$69,D$13)</f>
+      <c r="J5" s="10">
+        <f>HLOOKUP($I5,'[1]-1'!$C$46:$AE$69,D$15)</f>
         <v>425.00000000000006</v>
       </c>
-      <c r="K3" s="10">
-        <f>HLOOKUP($I3,'[1]-1'!$C$46:$AE$69,C$13)</f>
+      <c r="K5" s="10">
+        <f>HLOOKUP($I5,'[1]-1'!$C$46:$AE$69,C$15)</f>
         <v>500</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L5" s="10">
         <v>2.77</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M5" s="10">
         <v>176</v>
       </c>
-      <c r="N3" s="11">
-        <f>J3*$L3/100</f>
+      <c r="N5" s="11">
+        <f>J5*$L5/100</f>
         <v>11.772500000000003</v>
       </c>
-      <c r="O3" s="12">
-        <f>K3*$L3/100</f>
+      <c r="O5" s="12">
+        <f>K5*$L5/100</f>
         <v>13.85</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="14">
-        <f>HLOOKUP($B4,'[1]-1'!$C$46:$AE$69,D$13)</f>
+      <c r="C6" s="14">
+        <f>HLOOKUP($B6,'[1]-1'!$C$46:$AE$69,D$15)</f>
         <v>425.00000000000006</v>
       </c>
-      <c r="D4" s="14">
-        <f>HLOOKUP($B4,'[1]-1'!$C$46:$AE$69,C$13)</f>
+      <c r="D6" s="14">
+        <f>HLOOKUP($B6,'[1]-1'!$C$46:$AE$69,C$15)</f>
         <v>500</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E6" s="14">
         <v>2.19</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F6" s="14">
         <v>220</v>
       </c>
-      <c r="G4" s="15">
-        <f>C4*$E4/100</f>
+      <c r="G6" s="15">
+        <f>C6*$E6/100</f>
         <v>9.307500000000001</v>
       </c>
-      <c r="H4" s="16">
-        <f>D4*$E4/100</f>
+      <c r="H6" s="16">
+        <f>D6*$E6/100</f>
         <v>10.95</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="14">
-        <f>HLOOKUP($I4,'[1]-1'!$C$46:$AE$69,D$13)</f>
+      <c r="J6" s="14">
+        <f>HLOOKUP($I6,'[1]-1'!$C$46:$AE$69,D$15)</f>
         <v>425.00000000000006</v>
       </c>
-      <c r="K4" s="14">
-        <f>HLOOKUP($I4,'[1]-1'!$C$46:$AE$69,C$13)</f>
+      <c r="K6" s="14">
+        <f>HLOOKUP($I6,'[1]-1'!$C$46:$AE$69,C$15)</f>
         <v>500</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L6" s="14">
         <v>2.85</v>
       </c>
-      <c r="M4" s="14">
+      <c r="M6" s="14">
         <v>149</v>
       </c>
-      <c r="N4" s="15">
-        <f t="shared" ref="N4:N5" si="0">J4*$L4/100</f>
+      <c r="N6" s="15">
+        <f t="shared" ref="N6:N7" si="0">J6*$L6/100</f>
         <v>12.112500000000002</v>
       </c>
-      <c r="O4" s="16">
-        <f t="shared" ref="O4:O5" si="1">K4*$L4/100</f>
+      <c r="O6" s="16">
+        <f t="shared" ref="O6:O7" si="1">K6*$L6/100</f>
         <v>14.25</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="18">
-        <f>HLOOKUP($B5,'[1]-1'!$C$46:$AE$69,D$13)</f>
-        <v>425.00000000000006</v>
-      </c>
-      <c r="D5" s="18">
-        <f>HLOOKUP($B5,'[1]-1'!$C$46:$AE$69,C$13)</f>
-        <v>500</v>
-      </c>
-      <c r="E5" s="19">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="F5" s="19">
-        <v>498</v>
-      </c>
-      <c r="G5" s="20">
-        <f>C5*$E5/100</f>
-        <v>10.8375</v>
-      </c>
-      <c r="H5" s="21">
-        <f>D5*$E5/100</f>
-        <v>12.75</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="18">
-        <f>HLOOKUP($I5,'[1]-1'!$C$46:$AE$69,D$13)</f>
-        <v>425.00000000000006</v>
-      </c>
-      <c r="K5" s="18">
-        <f>HLOOKUP($I5,'[1]-1'!$C$46:$AE$69,C$13)</f>
-        <v>500</v>
-      </c>
-      <c r="L5" s="19">
-        <v>2.85</v>
-      </c>
-      <c r="M5" s="19">
-        <v>750</v>
-      </c>
-      <c r="N5" s="20">
-        <f t="shared" si="0"/>
-        <v>12.112500000000002</v>
-      </c>
-      <c r="O5" s="21">
-        <f t="shared" si="1"/>
-        <v>14.25</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="22"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24">
-        <v>2.5</v>
-      </c>
-      <c r="F6" s="24">
-        <v>252</v>
-      </c>
-      <c r="G6" s="25">
-        <f>C5*$E6/100</f>
-        <v>10.625000000000002</v>
-      </c>
-      <c r="H6" s="26">
-        <f>D5*$E6/100</f>
-        <v>12.5</v>
-      </c>
-      <c r="I6" s="22"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="24">
-        <v>2.84</v>
-      </c>
-      <c r="M6" s="24">
-        <v>273</v>
-      </c>
-      <c r="N6" s="25">
-        <f>J5*$L6/100</f>
-        <v>12.07</v>
-      </c>
-      <c r="O6" s="26">
-        <f>K5*$L6/100</f>
-        <v>14.2</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" s="18">
-        <f>HLOOKUP($B7,'[1]-1'!$C$46:$AE$69,D$13)</f>
+        <f>HLOOKUP($B7,'[1]-1'!$C$46:$AE$69,D$15)</f>
         <v>425.00000000000006</v>
       </c>
       <c r="D7" s="18">
-        <f>HLOOKUP($B7,'[1]-1'!$C$46:$AE$69,C$13)</f>
+        <f>HLOOKUP($B7,'[1]-1'!$C$46:$AE$69,C$15)</f>
         <v>500</v>
       </c>
       <c r="E7" s="19">
-        <v>2.54</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="F7" s="19">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="G7" s="20">
         <f>C7*$E7/100</f>
-        <v>10.795000000000002</v>
+        <v>10.8375</v>
       </c>
       <c r="H7" s="21">
         <f>D7*$E7/100</f>
-        <v>12.7</v>
+        <v>12.75</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J7" s="18">
-        <f>HLOOKUP($I7,'[1]-1'!$C$46:$AE$69,D$13)</f>
+        <f>HLOOKUP($I7,'[1]-1'!$C$46:$AE$69,D$15)</f>
         <v>425.00000000000006</v>
       </c>
       <c r="K7" s="18">
-        <f>HLOOKUP($I7,'[1]-1'!$C$46:$AE$69,C$13)</f>
+        <f>HLOOKUP($I7,'[1]-1'!$C$46:$AE$69,C$15)</f>
         <v>500</v>
       </c>
       <c r="L7" s="19">
-        <v>3.04</v>
+        <v>2.85</v>
       </c>
       <c r="M7" s="19">
-        <v>442</v>
+        <v>750</v>
       </c>
       <c r="N7" s="20">
-        <f>J7*$L7/100</f>
-        <v>12.920000000000002</v>
+        <f t="shared" si="0"/>
+        <v>12.112500000000002</v>
       </c>
       <c r="O7" s="21">
-        <f>K7*$L7/100</f>
-        <v>15.2</v>
+        <f t="shared" si="1"/>
+        <v>14.25</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
@@ -3335,18 +3288,18 @@
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
       <c r="E8" s="24">
-        <v>2.48</v>
+        <v>2.5</v>
       </c>
       <c r="F8" s="24">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="G8" s="25">
         <f>C7*$E8/100</f>
-        <v>10.540000000000003</v>
+        <v>10.625000000000002</v>
       </c>
       <c r="H8" s="26">
         <f>D7*$E8/100</f>
-        <v>12.4</v>
+        <v>12.5</v>
       </c>
       <c r="I8" s="22"/>
       <c r="J8" s="23"/>
@@ -3355,7 +3308,7 @@
         <v>2.84</v>
       </c>
       <c r="M8" s="24">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="N8" s="25">
         <f>J7*$L8/100</f>
@@ -3368,54 +3321,54 @@
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="17" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="18">
-        <f>HLOOKUP($B9,'[1]-1'!$C$46:$AE$69,D$13)</f>
+        <f>HLOOKUP($B9,'[1]-1'!$C$46:$AE$69,D$15)</f>
         <v>425.00000000000006</v>
       </c>
       <c r="D9" s="18">
-        <f>HLOOKUP($B9,'[1]-1'!$C$46:$AE$69,C$13)</f>
+        <f>HLOOKUP($B9,'[1]-1'!$C$46:$AE$69,C$15)</f>
         <v>500</v>
       </c>
       <c r="E9" s="19">
-        <v>2.5099999999999998</v>
+        <v>2.54</v>
       </c>
       <c r="F9" s="19">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="G9" s="20">
         <f>C9*$E9/100</f>
-        <v>10.6675</v>
+        <v>10.795000000000002</v>
       </c>
       <c r="H9" s="21">
         <f>D9*$E9/100</f>
-        <v>12.55</v>
+        <v>12.7</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J9" s="18">
-        <f>HLOOKUP($I9,'[1]-1'!$C$46:$AE$69,D$13)</f>
+        <f>HLOOKUP($I9,'[1]-1'!$C$46:$AE$69,D$15)</f>
         <v>425.00000000000006</v>
       </c>
       <c r="K9" s="18">
-        <f>HLOOKUP($I9,'[1]-1'!$C$46:$AE$69,C$13)</f>
+        <f>HLOOKUP($I9,'[1]-1'!$C$46:$AE$69,C$15)</f>
         <v>500</v>
       </c>
       <c r="L9" s="19">
-        <v>2.87</v>
+        <v>3.04</v>
       </c>
       <c r="M9" s="19">
-        <v>459</v>
+        <v>442</v>
       </c>
       <c r="N9" s="20">
         <f>J9*$L9/100</f>
-        <v>12.197500000000002</v>
+        <v>12.920000000000002</v>
       </c>
       <c r="O9" s="21">
         <f>K9*$L9/100</f>
-        <v>14.35</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
@@ -3423,203 +3376,696 @@
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
       <c r="E10" s="24">
-        <v>2.4700000000000002</v>
+        <v>2.48</v>
       </c>
       <c r="F10" s="24">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G10" s="25">
         <f>C9*$E10/100</f>
-        <v>10.497500000000002</v>
+        <v>10.540000000000003</v>
       </c>
       <c r="H10" s="26">
         <f>D9*$E10/100</f>
-        <v>12.35</v>
+        <v>12.4</v>
       </c>
       <c r="I10" s="22"/>
       <c r="J10" s="23"/>
       <c r="K10" s="23"/>
       <c r="L10" s="24">
-        <v>2.98</v>
+        <v>2.84</v>
       </c>
       <c r="M10" s="24">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="N10" s="25">
         <f>J9*$L10/100</f>
-        <v>12.665000000000003</v>
+        <v>12.07</v>
       </c>
       <c r="O10" s="26">
         <f>K9*$L10/100</f>
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="18">
+        <f>HLOOKUP($B11,'[1]-1'!$C$46:$AE$69,D$15)</f>
+        <v>425.00000000000006</v>
+      </c>
+      <c r="D11" s="18">
+        <f>HLOOKUP($B11,'[1]-1'!$C$46:$AE$69,C$15)</f>
+        <v>500</v>
+      </c>
+      <c r="E11" s="19">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="F11" s="19">
+        <v>501</v>
+      </c>
+      <c r="G11" s="20">
+        <f>C11*$E11/100</f>
+        <v>10.6675</v>
+      </c>
+      <c r="H11" s="21">
+        <f>D11*$E11/100</f>
+        <v>12.55</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="18">
+        <f>HLOOKUP($I11,'[1]-1'!$C$46:$AE$69,D$15)</f>
+        <v>425.00000000000006</v>
+      </c>
+      <c r="K11" s="18">
+        <f>HLOOKUP($I11,'[1]-1'!$C$46:$AE$69,C$15)</f>
+        <v>500</v>
+      </c>
+      <c r="L11" s="19">
+        <v>2.87</v>
+      </c>
+      <c r="M11" s="19">
+        <v>459</v>
+      </c>
+      <c r="N11" s="20">
+        <f>J11*$L11/100</f>
+        <v>12.197500000000002</v>
+      </c>
+      <c r="O11" s="21">
+        <f>K11*$L11/100</f>
+        <v>14.35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="24">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="F12" s="24">
+        <v>251</v>
+      </c>
+      <c r="G12" s="25">
+        <f>C11*$E12/100</f>
+        <v>10.497500000000002</v>
+      </c>
+      <c r="H12" s="26">
+        <f>D11*$E12/100</f>
+        <v>12.35</v>
+      </c>
+      <c r="I12" s="22"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="24">
+        <v>2.98</v>
+      </c>
+      <c r="M12" s="24">
+        <v>293</v>
+      </c>
+      <c r="N12" s="25">
+        <f>J11*$L12/100</f>
+        <v>12.665000000000003</v>
+      </c>
+      <c r="O12" s="26">
+        <f>K11*$L12/100</f>
         <v>14.9</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="27" t="s">
+    <row r="13" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="28">
-        <f>HLOOKUP($B11,'[1]-1'!$C$46:$AE$69,D$13)</f>
+      <c r="C13" s="28">
+        <f>HLOOKUP($B13,'[1]-1'!$C$46:$AE$69,D$15)</f>
         <v>425.00000000000006</v>
       </c>
-      <c r="D11" s="28">
-        <f>HLOOKUP($B11,'[1]-1'!$C$46:$AE$69,C$13)</f>
+      <c r="D13" s="28">
+        <f>HLOOKUP($B13,'[1]-1'!$C$46:$AE$69,C$15)</f>
         <v>500</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E13" s="28">
         <v>2.4700000000000002</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F13" s="28">
         <v>255</v>
       </c>
-      <c r="G11" s="29">
-        <f>C11*$E11/100</f>
+      <c r="G13" s="29">
+        <f>C13*$E13/100</f>
         <v>10.497500000000002</v>
       </c>
-      <c r="H11" s="30">
-        <f>D11*$E11/100</f>
+      <c r="H13" s="30">
+        <f>D13*$E13/100</f>
         <v>12.35</v>
       </c>
-      <c r="I11" s="27" t="s">
+      <c r="I13" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="28">
-        <f>HLOOKUP($I11,'[1]-1'!$C$46:$AE$69,D$13)</f>
+      <c r="J13" s="28">
+        <f>HLOOKUP($I13,'[1]-1'!$C$46:$AE$69,D$15)</f>
         <v>425.00000000000006</v>
       </c>
-      <c r="K11" s="28">
-        <f>HLOOKUP($I11,'[1]-1'!$C$46:$AE$69,C$13)</f>
+      <c r="K13" s="28">
+        <f>HLOOKUP($I13,'[1]-1'!$C$46:$AE$69,C$15)</f>
         <v>500</v>
       </c>
-      <c r="L11" s="28">
+      <c r="L13" s="28">
         <v>2.5499999999999998</v>
       </c>
-      <c r="M11" s="28">
+      <c r="M13" s="28">
         <v>252</v>
       </c>
-      <c r="N11" s="29">
-        <f>J11*$L11/100</f>
+      <c r="N13" s="29">
+        <f>J13*$L13/100</f>
         <v>10.8375</v>
       </c>
-      <c r="O11" s="30">
-        <f>K11*$L11/100</f>
+      <c r="O13" s="30">
+        <f>K13*$L13/100</f>
         <v>12.75</v>
       </c>
     </row>
-    <row r="12" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="31"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="31"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="32"/>
-    </row>
-    <row r="13" spans="2:15" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="1">
+    <row r="14" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="31"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="31"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+    </row>
+    <row r="15" spans="2:15" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="1">
         <v>19</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D15" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="33" t="s">
+    <row r="16" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="34">
+      <c r="C16" s="34">
         <f>0.3*0.5*'[1]-1'!L$7</f>
         <v>375</v>
       </c>
     </row>
-    <row r="16" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G16" s="2" t="s">
+    <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G17" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="61"/>
+    </row>
+    <row r="18" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="N18" s="2"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="1">
+        <v>7.7839999999999998</v>
+      </c>
+      <c r="D19" s="1">
+        <v>7.96</v>
+      </c>
+      <c r="E19" s="32">
+        <f>C19*1.2+D19*1.6</f>
+        <v>22.076799999999999</v>
+      </c>
+      <c r="F19" s="63"/>
+      <c r="G19" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="H19" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B20" s="57"/>
+      <c r="C20" s="53">
+        <v>-11.079000000000001</v>
+      </c>
+      <c r="D20" s="53">
+        <v>-11.016999999999999</v>
+      </c>
+      <c r="E20" s="58">
+        <f>C20*1.2+D20*1.6</f>
+        <v>-30.921999999999997</v>
+      </c>
+      <c r="F20" s="63"/>
+      <c r="G20" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="H20" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="50">
+        <v>8.048</v>
+      </c>
+      <c r="D21" s="50">
+        <v>7.9409999999999998</v>
+      </c>
+      <c r="E21" s="59">
+        <f>C21*1.2+D21*1.6</f>
+        <v>22.363199999999999</v>
+      </c>
+      <c r="F21" s="63"/>
+      <c r="G21" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G22" s="1"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="26" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B26" s="64" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="58" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="56">
-        <f>MAX('Esfuerzos Viga Estática'!E4:E80)</f>
-        <v>2208015.88</v>
-      </c>
-      <c r="D17" s="49" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="48">
-        <f>C17/100000</f>
-        <v>22.0801588</v>
-      </c>
-      <c r="F17" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="2" t="s">
+      <c r="C26" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="59"/>
-      <c r="C18" s="61">
-        <f>MIN('Esfuerzos Viga Estática'!E4:E80)</f>
-        <v>-3092342.54</v>
-      </c>
-      <c r="D18" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="54">
-        <f>C18/100000</f>
-        <v>-30.923425399999999</v>
-      </c>
-      <c r="F18" s="55" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" s="2" t="s">
+      <c r="C28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="52"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="57">
-        <f>MAX('Esfuerzos Viga Estática'!D4:D80)</f>
-        <v>22365.4</v>
-      </c>
-      <c r="D19" s="50" t="s">
+      <c r="C30" s="32">
+        <v>18.1998</v>
+      </c>
+      <c r="F30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="32">
+        <v>14.436199999999999</v>
+      </c>
+      <c r="F31" s="32"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="1">
+        <v>200</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="J32" s="32"/>
+    </row>
+    <row r="33" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="32"/>
+      <c r="G33" s="1"/>
+      <c r="J33" s="35"/>
+    </row>
+    <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="65"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="62">
-        <f>C19/1000</f>
-        <v>22.365400000000001</v>
-      </c>
-      <c r="F19" s="52" t="s">
+      <c r="I34" s="61"/>
+      <c r="L34" s="2"/>
+      <c r="O34" s="1"/>
+    </row>
+    <row r="35" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="I35" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="L35" s="2"/>
+      <c r="O35" s="1"/>
+    </row>
+    <row r="36" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B36" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="53">
+        <v>11.33</v>
+      </c>
+      <c r="D36" s="53">
+        <v>0.53</v>
+      </c>
+      <c r="E36" s="54">
+        <v>14.436199999999999</v>
+      </c>
+      <c r="F36" s="58">
+        <f>C36*1.2+D36*1+E36*1.4</f>
+        <v>34.336679999999994</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="H36" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="I36" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="L36" s="2"/>
+      <c r="O36" s="1"/>
+    </row>
+    <row r="37" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="50">
+        <v>5.2</v>
+      </c>
+      <c r="D37" s="50">
+        <v>0.312</v>
+      </c>
+      <c r="E37" s="55">
+        <v>18.1998</v>
+      </c>
+      <c r="F37" s="59">
+        <f>C37*1.2+D37*1+E37*1.4</f>
+        <v>32.03172</v>
+      </c>
+      <c r="G37" s="1"/>
+      <c r="H37" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="I37" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="L37" s="2"/>
+      <c r="O37" s="1"/>
+    </row>
+    <row r="38" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="51"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="I38" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="L38" s="2"/>
+      <c r="O38" s="1"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C39" s="53"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="C40" s="53"/>
+      <c r="F40" s="1">
+        <v>1.4098999999999999</v>
+      </c>
+      <c r="G40" s="1">
+        <v>-0.20699999999999999</v>
+      </c>
+      <c r="H40" s="1">
+        <v>14.436199999999999</v>
+      </c>
+      <c r="I40" s="58">
+        <f>F40*1.2+G40*1+H40*1.4</f>
+        <v>21.695559999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="53"/>
+      <c r="F41" s="1">
+        <v>3.2690000000000001</v>
+      </c>
+      <c r="G41" s="2">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="H41" s="1">
+        <v>18.1998</v>
+      </c>
+      <c r="I41" s="59">
+        <f>F41*1.2+G41*1+H41*1.4</f>
+        <v>29.581519999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C42" s="53"/>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C43" s="53"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="66"/>
+      <c r="H43" s="66"/>
+      <c r="I43" s="66"/>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J44" s="32"/>
+    </row>
+    <row r="45" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B45" s="64" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" s="1">
+        <v>184</v>
+      </c>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" s="1">
+        <v>200</v>
+      </c>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G51" s="35"/>
+    </row>
+    <row r="52" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="G52" s="35"/>
+      <c r="H52" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="I52" s="61"/>
+    </row>
+    <row r="53" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" s="53">
+        <v>10.673299999999999</v>
+      </c>
+      <c r="D53" s="53">
+        <v>2.9523000000000001</v>
+      </c>
+      <c r="E53" s="54">
+        <v>5.2817999999999996</v>
+      </c>
+      <c r="F53" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="G53" s="1"/>
+      <c r="H53" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="I53" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>45</v>
+    </row>
+    <row r="54" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" s="50">
+        <v>6.7065000000000001</v>
+      </c>
+      <c r="D54" s="50">
+        <v>1.5425</v>
+      </c>
+      <c r="E54" s="55">
+        <v>2.4342000000000001</v>
+      </c>
+      <c r="F54" s="58">
+        <f>C53*1.2+D53*1+E53*1.4</f>
+        <v>23.154779999999999</v>
+      </c>
+      <c r="G54" s="1"/>
+      <c r="H54" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="I54" s="60" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D55" s="2"/>
+      <c r="F55" s="59">
+        <f>C54*1.2+D54*1+E54*1.4</f>
+        <v>12.998180000000001</v>
+      </c>
+      <c r="G55" s="1"/>
+      <c r="H55" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="I55" s="60" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G56" s="1"/>
+      <c r="H56" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="I56" s="50" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
+  <mergeCells count="25">
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
     <mergeCell ref="B9:B10"/>
+    <mergeCell ref="I9:I10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="J11:J12"/>
     <mergeCell ref="I7:I8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="J7:J8"/>
     <mergeCell ref="K9:K10"/>
     <mergeCell ref="J9:J10"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="J7:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3631,76 +4077,76 @@
   <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4:D80"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.140625" style="35"/>
+    <col min="4" max="4" width="9.140625" style="36"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="A1" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="44" t="s">
+      <c r="A2" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="45"/>
+      <c r="B2" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="48"/>
+      <c r="E2" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="46"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="42" t="s">
+      <c r="A3" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="42" t="s">
-        <v>35</v>
+      <c r="B3" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="43" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="35">
+      <c r="A4" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="36">
         <v>0</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="36">
         <v>-4770.4399999999996</v>
       </c>
-      <c r="D4" s="35">
+      <c r="D4" s="36">
         <f>ABS(C4)</f>
         <v>4770.4399999999996</v>
       </c>
-      <c r="E4" s="43">
+      <c r="E4" s="44">
         <v>1.1640000000000001E-10</v>
       </c>
       <c r="F4">
@@ -3709,1673 +4155,1673 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="35">
+      <c r="A5" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="36">
         <v>50</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="36">
         <v>-4229.8500000000004</v>
       </c>
-      <c r="D5" s="35">
+      <c r="D5" s="36">
         <f t="shared" ref="D5:D68" si="0">ABS(C5)</f>
         <v>4229.8500000000004</v>
       </c>
-      <c r="E5" s="35">
+      <c r="E5" s="36">
         <v>227710.28</v>
       </c>
-      <c r="F5" s="35">
+      <c r="F5" s="36">
         <f t="shared" ref="F5:F68" si="1">ABS(E5)</f>
         <v>227710.28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="35">
+      <c r="A6" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="36">
         <v>100</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="36">
         <v>-3040.58</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="36">
         <f t="shared" si="0"/>
         <v>3040.58</v>
       </c>
-      <c r="E6" s="35">
+      <c r="E6" s="36">
         <v>412173.92</v>
       </c>
-      <c r="F6" s="35">
+      <c r="F6" s="36">
         <f t="shared" si="1"/>
         <v>412173.92</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="35">
+      <c r="A7" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="36">
         <v>150</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="36">
         <v>-1202.6199999999999</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="36">
         <f t="shared" si="0"/>
         <v>1202.6199999999999</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="36">
         <v>520956.74</v>
       </c>
-      <c r="F7" s="35">
+      <c r="F7" s="36">
         <f t="shared" si="1"/>
         <v>520956.74</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="35">
+      <c r="A8" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="36">
         <v>200</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="36">
         <v>1284.02</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="36">
         <f t="shared" si="0"/>
         <v>1284.02</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="36">
         <v>521624.59</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="36">
         <f t="shared" si="1"/>
         <v>521624.59</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="35">
+      <c r="A9" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="36">
         <v>250</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="36">
         <v>4419.3500000000004</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="36">
         <f t="shared" si="0"/>
         <v>4419.3500000000004</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="36">
         <v>381743.27</v>
       </c>
-      <c r="F9" s="35">
+      <c r="F9" s="36">
         <f t="shared" si="1"/>
         <v>381743.27</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="35">
+      <c r="A10" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="36">
         <v>300</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="36">
         <v>7633.23</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="36">
         <f t="shared" si="0"/>
         <v>7633.23</v>
       </c>
-      <c r="E10" s="35">
+      <c r="E10" s="36">
         <v>77738.47</v>
       </c>
-      <c r="F10" s="35">
+      <c r="F10" s="36">
         <f t="shared" si="1"/>
         <v>77738.47</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="35">
+      <c r="A11" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="36">
         <v>350</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="36">
         <v>10183.9</v>
       </c>
-      <c r="D11" s="35">
+      <c r="D11" s="36">
         <f t="shared" si="0"/>
         <v>10183.9</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="36">
         <v>-370468.71</v>
       </c>
-      <c r="F11" s="35">
+      <c r="F11" s="36">
         <f t="shared" si="1"/>
         <v>370468.71</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="35">
+      <c r="A12" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="36">
         <v>400</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="36">
         <v>12067.59</v>
       </c>
-      <c r="D12" s="35">
+      <c r="D12" s="36">
         <f t="shared" si="0"/>
         <v>12067.59</v>
       </c>
-      <c r="E12" s="35">
+      <c r="E12" s="36">
         <v>-929535.09</v>
       </c>
-      <c r="F12" s="35">
+      <c r="F12" s="36">
         <f t="shared" si="1"/>
         <v>929535.09</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="35">
+      <c r="A13" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="36">
         <v>450</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="36">
         <v>13284.31</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="36">
         <f t="shared" si="0"/>
         <v>13284.31</v>
       </c>
-      <c r="E13" s="35">
+      <c r="E13" s="36">
         <v>-1566111.76</v>
       </c>
-      <c r="F13" s="35">
+      <c r="F13" s="36">
         <f t="shared" si="1"/>
         <v>1566111.76</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="35">
+      <c r="A14" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="36">
         <v>500</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="36">
         <v>13834.05</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D14" s="36">
         <f t="shared" si="0"/>
         <v>13834.05</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E14" s="36">
         <v>-2246849.7999999998</v>
       </c>
-      <c r="F14" s="35">
+      <c r="F14" s="36">
         <f t="shared" si="1"/>
         <v>2246849.7999999998</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="35">
+      <c r="A15" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="36">
         <v>0</v>
       </c>
-      <c r="C15" s="35">
+      <c r="C15" s="36">
         <v>-17845.16</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D15" s="36">
         <f t="shared" si="0"/>
         <v>17845.16</v>
       </c>
-      <c r="E15" s="35">
+      <c r="E15" s="36">
         <v>-2246849.7999999998</v>
       </c>
-      <c r="F15" s="35">
+      <c r="F15" s="36">
         <f t="shared" si="1"/>
         <v>2246849.7999999998</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="35">
+      <c r="A16" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="36">
         <v>50</v>
       </c>
-      <c r="C16" s="35">
+      <c r="C16" s="36">
         <v>-17301.189999999999</v>
       </c>
-      <c r="D16" s="35">
+      <c r="D16" s="36">
         <f t="shared" si="0"/>
         <v>17301.189999999999</v>
       </c>
-      <c r="E16" s="35">
+      <c r="E16" s="36">
         <v>-1365460.12</v>
       </c>
-      <c r="F16" s="35">
+      <c r="F16" s="36">
         <f t="shared" si="1"/>
         <v>1365460.12</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="35">
+      <c r="A17" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="36">
         <v>100</v>
       </c>
-      <c r="C17" s="35">
+      <c r="C17" s="36">
         <v>-16101.76</v>
       </c>
-      <c r="D17" s="35">
+      <c r="D17" s="36">
         <f t="shared" si="0"/>
         <v>16101.76</v>
       </c>
-      <c r="E17" s="35">
+      <c r="E17" s="36">
         <v>-527655.43999999994</v>
       </c>
-      <c r="F17" s="35">
+      <c r="F17" s="36">
         <f t="shared" si="1"/>
         <v>527655.43999999994</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="35">
+      <c r="A18" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="36">
         <v>150</v>
       </c>
-      <c r="C18" s="35">
+      <c r="C18" s="36">
         <v>-14246.88</v>
       </c>
-      <c r="D18" s="35">
+      <c r="D18" s="36">
         <f t="shared" si="0"/>
         <v>14246.88</v>
       </c>
-      <c r="E18" s="35">
+      <c r="E18" s="36">
         <v>233791.71</v>
       </c>
-      <c r="F18" s="35">
+      <c r="F18" s="36">
         <f t="shared" si="1"/>
         <v>233791.71</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="35">
+      <c r="A19" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="36">
         <v>200</v>
       </c>
-      <c r="C19" s="35">
+      <c r="C19" s="36">
         <v>-11736.56</v>
       </c>
-      <c r="D19" s="35">
+      <c r="D19" s="36">
         <f t="shared" si="0"/>
         <v>11736.56</v>
       </c>
-      <c r="E19" s="35">
+      <c r="E19" s="36">
         <v>886108.8</v>
       </c>
-      <c r="F19" s="35">
+      <c r="F19" s="36">
         <f t="shared" si="1"/>
         <v>886108.8</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="35">
+      <c r="A20" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="36">
         <v>250</v>
       </c>
-      <c r="C20" s="35">
+      <c r="C20" s="36">
         <v>-8570.7800000000007</v>
       </c>
-      <c r="D20" s="35">
+      <c r="D20" s="36">
         <f t="shared" si="0"/>
         <v>8570.7800000000007</v>
       </c>
-      <c r="E20" s="35">
+      <c r="E20" s="36">
         <v>1396523.28</v>
       </c>
-      <c r="F20" s="35">
+      <c r="F20" s="36">
         <f t="shared" si="1"/>
         <v>1396523.28</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="35">
+      <c r="A21" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="36">
         <v>300</v>
       </c>
-      <c r="C21" s="35">
+      <c r="C21" s="36">
         <v>-4895.6099999999997</v>
       </c>
-      <c r="D21" s="35">
+      <c r="D21" s="36">
         <f t="shared" si="0"/>
         <v>4895.6099999999997</v>
       </c>
-      <c r="E21" s="35">
+      <c r="E21" s="36">
         <v>1734599.49</v>
       </c>
-      <c r="F21" s="35">
+      <c r="F21" s="36">
         <f t="shared" si="1"/>
         <v>1734599.49</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="35">
+      <c r="A22" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="36">
         <v>350</v>
       </c>
-      <c r="C22" s="35">
+      <c r="C22" s="36">
         <v>-1085.48</v>
       </c>
-      <c r="D22" s="35">
+      <c r="D22" s="36">
         <f t="shared" si="0"/>
         <v>1085.48</v>
       </c>
-      <c r="E22" s="35">
+      <c r="E22" s="36">
         <v>1884141.96</v>
       </c>
-      <c r="F22" s="35">
+      <c r="F22" s="36">
         <f t="shared" si="1"/>
         <v>1884141.96</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="35">
+      <c r="A23" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="36">
         <v>400</v>
       </c>
-      <c r="C23" s="35">
+      <c r="C23" s="36">
         <v>2728.29</v>
       </c>
-      <c r="D23" s="35">
+      <c r="D23" s="36">
         <f t="shared" si="0"/>
         <v>2728.29</v>
       </c>
-      <c r="E23" s="35">
+      <c r="E23" s="36">
         <v>1843086.94</v>
       </c>
-      <c r="F23" s="35">
+      <c r="F23" s="36">
         <f t="shared" si="1"/>
         <v>1843086.94</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="35">
+      <c r="A24" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="36">
         <v>450</v>
       </c>
-      <c r="C24" s="35">
+      <c r="C24" s="36">
         <v>6545.72</v>
       </c>
-      <c r="D24" s="35">
+      <c r="D24" s="36">
         <f t="shared" si="0"/>
         <v>6545.72</v>
       </c>
-      <c r="E24" s="35">
+      <c r="E24" s="36">
         <v>1611251.78</v>
       </c>
-      <c r="F24" s="35">
+      <c r="F24" s="36">
         <f t="shared" si="1"/>
         <v>1611251.78</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="35">
+      <c r="A25" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="36">
         <v>500</v>
       </c>
-      <c r="C25" s="35">
+      <c r="C25" s="36">
         <v>10265.52</v>
       </c>
-      <c r="D25" s="35">
+      <c r="D25" s="36">
         <f t="shared" si="0"/>
         <v>10265.52</v>
       </c>
-      <c r="E25" s="35">
+      <c r="E25" s="36">
         <v>1189838.1299999999</v>
       </c>
-      <c r="F25" s="35">
+      <c r="F25" s="36">
         <f t="shared" si="1"/>
         <v>1189838.1299999999</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="35">
+      <c r="A26" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="36">
         <v>550</v>
       </c>
-      <c r="C26" s="35">
+      <c r="C26" s="36">
         <v>13512.1</v>
       </c>
-      <c r="D26" s="35">
+      <c r="D26" s="36">
         <f t="shared" si="0"/>
         <v>13512.1</v>
       </c>
-      <c r="E26" s="35">
+      <c r="E26" s="36">
         <v>592593.55000000005</v>
       </c>
-      <c r="F26" s="35">
+      <c r="F26" s="36">
         <f t="shared" si="1"/>
         <v>592593.55000000005</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="35">
+      <c r="A27" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="36">
         <v>600</v>
       </c>
-      <c r="C27" s="35">
+      <c r="C27" s="36">
         <v>16085.34</v>
       </c>
-      <c r="D27" s="35">
+      <c r="D27" s="36">
         <f t="shared" si="0"/>
         <v>16085.34</v>
       </c>
-      <c r="E27" s="35">
+      <c r="E27" s="36">
         <v>-150148.6</v>
       </c>
-      <c r="F27" s="35">
+      <c r="F27" s="36">
         <f t="shared" si="1"/>
         <v>150148.6</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="35">
+      <c r="A28" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="36">
         <v>650</v>
       </c>
-      <c r="C28" s="35">
+      <c r="C28" s="36">
         <v>17985.16</v>
       </c>
-      <c r="D28" s="35">
+      <c r="D28" s="36">
         <f t="shared" si="0"/>
         <v>17985.16</v>
       </c>
-      <c r="E28" s="35">
+      <c r="E28" s="36">
         <v>-1004717.06</v>
       </c>
-      <c r="F28" s="35">
+      <c r="F28" s="36">
         <f t="shared" si="1"/>
         <v>1004717.06</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="35">
+      <c r="A29" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="36">
         <v>700</v>
       </c>
-      <c r="C29" s="35">
+      <c r="C29" s="36">
         <v>19211.54</v>
       </c>
-      <c r="D29" s="35">
+      <c r="D29" s="36">
         <f t="shared" si="0"/>
         <v>19211.54</v>
       </c>
-      <c r="E29" s="35">
+      <c r="E29" s="36">
         <v>-1937440.55</v>
       </c>
-      <c r="F29" s="35">
+      <c r="F29" s="36">
         <f t="shared" si="1"/>
         <v>1937440.55</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="35">
+      <c r="A30" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="36">
         <v>750</v>
       </c>
-      <c r="C30" s="35">
+      <c r="C30" s="36">
         <v>19764.509999999998</v>
       </c>
-      <c r="D30" s="35">
+      <c r="D30" s="36">
         <f t="shared" si="0"/>
         <v>19764.509999999998</v>
       </c>
-      <c r="E30" s="35">
+      <c r="E30" s="36">
         <v>-2914647.79</v>
       </c>
-      <c r="F30" s="35">
+      <c r="F30" s="36">
         <f t="shared" si="1"/>
         <v>2914647.79</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="35">
+      <c r="A31" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="36">
         <v>0</v>
       </c>
-      <c r="C31" s="35">
+      <c r="C31" s="36">
         <v>-18392.66</v>
       </c>
-      <c r="D31" s="35">
+      <c r="D31" s="36">
         <f t="shared" si="0"/>
         <v>18392.66</v>
       </c>
-      <c r="E31" s="35">
+      <c r="E31" s="36">
         <v>-2914647.79</v>
       </c>
-      <c r="F31" s="35">
+      <c r="F31" s="36">
         <f t="shared" si="1"/>
         <v>2914647.79</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="35">
+      <c r="A32" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="36">
         <v>50</v>
       </c>
-      <c r="C32" s="35">
+      <c r="C32" s="36">
         <v>-17847.88</v>
       </c>
-      <c r="D32" s="35">
+      <c r="D32" s="36">
         <f t="shared" si="0"/>
         <v>17847.88</v>
       </c>
-      <c r="E32" s="35">
+      <c r="E32" s="36">
         <v>-2005896.43</v>
       </c>
-      <c r="F32" s="35">
+      <c r="F32" s="36">
         <f t="shared" si="1"/>
         <v>2005896.43</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="35">
+      <c r="A33" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="36">
         <v>100</v>
       </c>
-      <c r="C33" s="35">
+      <c r="C33" s="36">
         <v>-16646.05</v>
       </c>
-      <c r="D33" s="35">
+      <c r="D33" s="36">
         <f t="shared" si="0"/>
         <v>16646.05</v>
       </c>
-      <c r="E33" s="35">
+      <c r="E33" s="36">
         <v>-1140810.47</v>
       </c>
-      <c r="F33" s="35">
+      <c r="F33" s="36">
         <f t="shared" si="1"/>
         <v>1140810.47</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" s="35">
+      <c r="A34" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="36">
         <v>150</v>
       </c>
-      <c r="C34" s="35">
+      <c r="C34" s="36">
         <v>-14787.15</v>
       </c>
-      <c r="D34" s="35">
+      <c r="D34" s="36">
         <f t="shared" si="0"/>
         <v>14787.15</v>
       </c>
-      <c r="E34" s="35">
+      <c r="E34" s="36">
         <v>-352242.82</v>
       </c>
-      <c r="F34" s="35">
+      <c r="F34" s="36">
         <f t="shared" si="1"/>
         <v>352242.82</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" s="35">
+      <c r="A35" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="36">
         <v>200</v>
       </c>
-      <c r="C35" s="35">
+      <c r="C35" s="36">
         <v>-12271.2</v>
       </c>
-      <c r="D35" s="35">
+      <c r="D35" s="36">
         <f t="shared" si="0"/>
         <v>12271.2</v>
       </c>
-      <c r="E35" s="35">
+      <c r="E35" s="36">
         <v>326953.57</v>
       </c>
-      <c r="F35" s="35">
+      <c r="F35" s="36">
         <f t="shared" si="1"/>
         <v>326953.57</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="35">
+      <c r="A36" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="36">
         <v>250</v>
       </c>
-      <c r="C36" s="35">
+      <c r="C36" s="36">
         <v>-9098.18</v>
       </c>
-      <c r="D36" s="35">
+      <c r="D36" s="36">
         <f t="shared" si="0"/>
         <v>9098.18</v>
       </c>
-      <c r="E36" s="35">
+      <c r="E36" s="36">
         <v>863925.79</v>
       </c>
-      <c r="F36" s="35">
+      <c r="F36" s="36">
         <f t="shared" si="1"/>
         <v>863925.79</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B37" s="35">
+      <c r="A37" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="36">
         <v>300</v>
       </c>
-      <c r="C37" s="35">
+      <c r="C37" s="36">
         <v>-5449.93</v>
       </c>
-      <c r="D37" s="35">
+      <c r="D37" s="36">
         <f t="shared" si="0"/>
         <v>5449.93</v>
       </c>
-      <c r="E37" s="35">
+      <c r="E37" s="36">
         <v>1228617.83</v>
       </c>
-      <c r="F37" s="35">
+      <c r="F37" s="36">
         <f t="shared" si="1"/>
         <v>1228617.83</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B38" s="35">
+      <c r="A38" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="36">
         <v>350</v>
       </c>
-      <c r="C38" s="35">
+      <c r="C38" s="36">
         <v>-1700.81</v>
       </c>
-      <c r="D38" s="35">
+      <c r="D38" s="36">
         <f t="shared" si="0"/>
         <v>1700.81</v>
       </c>
-      <c r="E38" s="35">
+      <c r="E38" s="36">
         <v>1407587.91</v>
       </c>
-      <c r="F38" s="35">
+      <c r="F38" s="36">
         <f t="shared" si="1"/>
         <v>1407587.91</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B39" s="35">
+      <c r="A39" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="36">
         <v>400</v>
       </c>
-      <c r="C39" s="35">
+      <c r="C39" s="36">
         <v>2096.66</v>
       </c>
-      <c r="D39" s="35">
+      <c r="D39" s="36">
         <f t="shared" si="0"/>
         <v>2096.66</v>
       </c>
-      <c r="E39" s="35">
+      <c r="E39" s="36">
         <v>1397893.28</v>
       </c>
-      <c r="F39" s="35">
+      <c r="F39" s="36">
         <f t="shared" si="1"/>
         <v>1397893.28</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B40" s="35">
+      <c r="A40" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="36">
         <v>450</v>
       </c>
-      <c r="C40" s="35">
+      <c r="C40" s="36">
         <v>5937.82</v>
       </c>
-      <c r="D40" s="35">
+      <c r="D40" s="36">
         <f t="shared" si="0"/>
         <v>5937.82</v>
       </c>
-      <c r="E40" s="35">
+      <c r="E40" s="36">
         <v>1197128.75</v>
       </c>
-      <c r="F40" s="35">
+      <c r="F40" s="36">
         <f t="shared" si="1"/>
         <v>1197128.75</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" s="35">
+      <c r="A41" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="36">
         <v>500</v>
       </c>
-      <c r="C41" s="35">
+      <c r="C41" s="36">
         <v>9591.9699999999993</v>
       </c>
-      <c r="D41" s="35">
+      <c r="D41" s="36">
         <f t="shared" si="0"/>
         <v>9591.9699999999993</v>
       </c>
-      <c r="E41" s="35">
+      <c r="E41" s="36">
         <v>807570.01</v>
       </c>
-      <c r="F41" s="35">
+      <c r="F41" s="36">
         <f t="shared" si="1"/>
         <v>807570.01</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B42" s="35">
+      <c r="A42" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="36">
         <v>550</v>
       </c>
-      <c r="C42" s="35">
+      <c r="C42" s="36">
         <v>12760.43</v>
       </c>
-      <c r="D42" s="35">
+      <c r="D42" s="36">
         <f t="shared" si="0"/>
         <v>12760.43</v>
       </c>
-      <c r="E42" s="35">
+      <c r="E42" s="36">
         <v>246026.46</v>
       </c>
-      <c r="F42" s="35">
+      <c r="F42" s="36">
         <f t="shared" si="1"/>
         <v>246026.46</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B43" s="35">
+      <c r="A43" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" s="36">
         <v>600</v>
       </c>
-      <c r="C43" s="35">
+      <c r="C43" s="36">
         <v>15272.84</v>
       </c>
-      <c r="D43" s="35">
+      <c r="D43" s="36">
         <f t="shared" si="0"/>
         <v>15272.84</v>
       </c>
-      <c r="E43" s="35">
+      <c r="E43" s="36">
         <v>-457538.92</v>
       </c>
-      <c r="F43" s="35">
+      <c r="F43" s="36">
         <f t="shared" si="1"/>
         <v>457538.92</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B44" s="35">
+      <c r="A44" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" s="36">
         <v>650</v>
       </c>
-      <c r="C44" s="35">
+      <c r="C44" s="36">
         <v>17129.21</v>
       </c>
-      <c r="D44" s="35">
+      <c r="D44" s="36">
         <f t="shared" si="0"/>
         <v>17129.21</v>
       </c>
-      <c r="E44" s="35">
+      <c r="E44" s="36">
         <v>-1270323.76</v>
       </c>
-      <c r="F44" s="35">
+      <c r="F44" s="36">
         <f t="shared" si="1"/>
         <v>1270323.76</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B45" s="35">
+      <c r="A45" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="36">
         <v>700</v>
       </c>
-      <c r="C45" s="35">
+      <c r="C45" s="36">
         <v>18329.53</v>
       </c>
-      <c r="D45" s="35">
+      <c r="D45" s="36">
         <f t="shared" si="0"/>
         <v>18329.53</v>
       </c>
-      <c r="E45" s="35">
+      <c r="E45" s="36">
         <v>-2159525.75</v>
       </c>
-      <c r="F45" s="35">
+      <c r="F45" s="36">
         <f t="shared" si="1"/>
         <v>2159525.75</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B46" s="35">
+      <c r="A46" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="36">
         <v>750</v>
       </c>
-      <c r="C46" s="35">
+      <c r="C46" s="36">
         <v>18873.8</v>
       </c>
-      <c r="D46" s="35">
+      <c r="D46" s="36">
         <f t="shared" si="0"/>
         <v>18873.8</v>
       </c>
-      <c r="E46" s="35">
+      <c r="E46" s="36">
         <v>-3092342.54</v>
       </c>
-      <c r="F46" s="35">
+      <c r="F46" s="36">
         <f t="shared" si="1"/>
         <v>3092342.54</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B47" s="35">
+      <c r="A47" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="36">
         <v>0</v>
       </c>
-      <c r="C47" s="35">
+      <c r="C47" s="36">
         <v>-20219.28</v>
       </c>
-      <c r="D47" s="35">
+      <c r="D47" s="36">
         <f t="shared" si="0"/>
         <v>20219.28</v>
       </c>
-      <c r="E47" s="35">
+      <c r="E47" s="36">
         <v>-3092342.54</v>
       </c>
-      <c r="F47" s="35">
+      <c r="F47" s="36">
         <f t="shared" si="1"/>
         <v>3092342.54</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B48" s="35">
+      <c r="A48" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" s="36">
         <v>50</v>
       </c>
-      <c r="C48" s="35">
+      <c r="C48" s="36">
         <v>-19750.099999999999</v>
       </c>
-      <c r="D48" s="35">
+      <c r="D48" s="36">
         <f t="shared" si="0"/>
         <v>19750.099999999999</v>
       </c>
-      <c r="E48" s="35">
+      <c r="E48" s="36">
         <v>-2091000.44</v>
       </c>
-      <c r="F48" s="35">
+      <c r="F48" s="36">
         <f t="shared" si="1"/>
         <v>2091000.44</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B49" s="35">
+      <c r="A49" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" s="36">
         <v>100</v>
       </c>
-      <c r="C49" s="35">
+      <c r="C49" s="36">
         <v>-18775.05</v>
       </c>
-      <c r="D49" s="35">
+      <c r="D49" s="36">
         <f t="shared" si="0"/>
         <v>18775.05</v>
       </c>
-      <c r="E49" s="35">
+      <c r="E49" s="36">
         <v>-1125764.1200000001</v>
       </c>
-      <c r="F49" s="35">
+      <c r="F49" s="36">
         <f t="shared" si="1"/>
         <v>1125764.1200000001</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B50" s="35">
+      <c r="A50" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B50" s="36">
         <v>150</v>
       </c>
-      <c r="C50" s="35">
+      <c r="C50" s="36">
         <v>-17294.13</v>
       </c>
-      <c r="D50" s="35">
+      <c r="D50" s="36">
         <f t="shared" si="0"/>
         <v>17294.13</v>
       </c>
-      <c r="E50" s="35">
+      <c r="E50" s="36">
         <v>-221926.9</v>
       </c>
-      <c r="F50" s="35">
+      <c r="F50" s="36">
         <f t="shared" si="1"/>
         <v>221926.9</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B51" s="35">
+      <c r="A51" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51" s="36">
         <v>200</v>
       </c>
-      <c r="C51" s="35">
+      <c r="C51" s="36">
         <v>-15307.35</v>
       </c>
-      <c r="D51" s="35">
+      <c r="D51" s="36">
         <f t="shared" si="0"/>
         <v>15307.35</v>
       </c>
-      <c r="E51" s="35">
+      <c r="E51" s="36">
         <v>595217.92000000004</v>
       </c>
-      <c r="F51" s="35">
+      <c r="F51" s="36">
         <f t="shared" si="1"/>
         <v>595217.92000000004</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B52" s="35">
+      <c r="A52" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="36">
         <v>250</v>
       </c>
-      <c r="C52" s="35">
+      <c r="C52" s="36">
         <v>-12814.7</v>
       </c>
-      <c r="D52" s="35">
+      <c r="D52" s="36">
         <f t="shared" si="0"/>
         <v>12814.7</v>
       </c>
-      <c r="E52" s="35">
+      <c r="E52" s="36">
         <v>1300377</v>
       </c>
-      <c r="F52" s="35">
+      <c r="F52" s="36">
         <f t="shared" si="1"/>
         <v>1300377</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B53" s="35">
+      <c r="A53" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" s="36">
         <v>300</v>
       </c>
-      <c r="C53" s="35">
+      <c r="C53" s="36">
         <v>-8339.69</v>
       </c>
-      <c r="D53" s="35">
+      <c r="D53" s="36">
         <f t="shared" si="0"/>
         <v>8339.69</v>
       </c>
-      <c r="E53" s="35">
+      <c r="E53" s="36">
         <v>1831455.76</v>
       </c>
-      <c r="F53" s="35">
+      <c r="F53" s="36">
         <f t="shared" si="1"/>
         <v>1831455.76</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B54" s="35">
+      <c r="A54" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="36">
         <v>350</v>
       </c>
-      <c r="C54" s="35">
+      <c r="C54" s="36">
         <v>-3765.03</v>
       </c>
-      <c r="D54" s="35">
+      <c r="D54" s="36">
         <f t="shared" si="0"/>
         <v>3765.03</v>
       </c>
-      <c r="E54" s="35">
+      <c r="E54" s="36">
         <v>2134059.37</v>
       </c>
-      <c r="F54" s="35">
+      <c r="F54" s="36">
         <f t="shared" si="1"/>
         <v>2134059.37</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B55" s="35">
+      <c r="A55" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B55" s="36">
         <v>400</v>
       </c>
-      <c r="C55" s="35">
+      <c r="C55" s="36">
         <v>806.19</v>
       </c>
-      <c r="D55" s="35">
+      <c r="D55" s="36">
         <f t="shared" si="0"/>
         <v>806.19</v>
       </c>
-      <c r="E55" s="35">
+      <c r="E55" s="36">
         <v>2208015.88</v>
       </c>
-      <c r="F55" s="35">
+      <c r="F55" s="36">
         <f t="shared" si="1"/>
         <v>2208015.88</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B56" s="35">
+      <c r="A56" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B56" s="36">
         <v>450</v>
       </c>
-      <c r="C56" s="35">
+      <c r="C56" s="36">
         <v>5373.97</v>
       </c>
-      <c r="D56" s="35">
+      <c r="D56" s="36">
         <f t="shared" si="0"/>
         <v>5373.97</v>
       </c>
-      <c r="E56" s="35">
+      <c r="E56" s="36">
         <v>2053497.33</v>
       </c>
-      <c r="F56" s="35">
+      <c r="F56" s="36">
         <f t="shared" si="1"/>
         <v>2053497.33</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B57" s="35">
+      <c r="A57" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B57" s="36">
         <v>500</v>
       </c>
-      <c r="C57" s="35">
+      <c r="C57" s="36">
         <v>9872.67</v>
       </c>
-      <c r="D57" s="35">
+      <c r="D57" s="36">
         <f t="shared" si="0"/>
         <v>9872.67</v>
       </c>
-      <c r="E57" s="35">
+      <c r="E57" s="36">
         <v>1670741.37</v>
       </c>
-      <c r="F57" s="35">
+      <c r="F57" s="36">
         <f t="shared" si="1"/>
         <v>1670741.37</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B58" s="35">
+      <c r="A58" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B58" s="36">
         <v>550</v>
       </c>
-      <c r="C58" s="35">
+      <c r="C58" s="36">
         <v>12706.97</v>
       </c>
-      <c r="D58" s="35">
+      <c r="D58" s="36">
         <f t="shared" si="0"/>
         <v>12706.97</v>
       </c>
-      <c r="E58" s="35">
+      <c r="E58" s="36">
         <v>1105550.75</v>
       </c>
-      <c r="F58" s="35">
+      <c r="F58" s="36">
         <f t="shared" si="1"/>
         <v>1105550.75</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B59" s="35">
+      <c r="A59" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59" s="36">
         <v>600</v>
       </c>
-      <c r="C59" s="35">
+      <c r="C59" s="36">
         <v>15373.4</v>
       </c>
-      <c r="D59" s="35">
+      <c r="D59" s="36">
         <f t="shared" si="0"/>
         <v>15373.4</v>
       </c>
-      <c r="E59" s="35">
+      <c r="E59" s="36">
         <v>402841.96</v>
       </c>
-      <c r="F59" s="35">
+      <c r="F59" s="36">
         <f t="shared" si="1"/>
         <v>402841.96</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B60" s="35">
+      <c r="A60" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B60" s="36">
         <v>650</v>
       </c>
-      <c r="C60" s="35">
+      <c r="C60" s="36">
         <v>17871.939999999999</v>
       </c>
-      <c r="D60" s="35">
+      <c r="D60" s="36">
         <f t="shared" si="0"/>
         <v>17871.939999999999</v>
       </c>
-      <c r="E60" s="35">
+      <c r="E60" s="36">
         <v>-428991.08</v>
       </c>
-      <c r="F60" s="35">
+      <c r="F60" s="36">
         <f t="shared" si="1"/>
         <v>428991.08</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B61" s="35">
+      <c r="A61" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61" s="36">
         <v>700</v>
       </c>
-      <c r="C61" s="35">
+      <c r="C61" s="36">
         <v>20202.61</v>
       </c>
-      <c r="D61" s="35">
+      <c r="D61" s="36">
         <f t="shared" si="0"/>
         <v>20202.61</v>
       </c>
-      <c r="E61" s="35">
+      <c r="E61" s="36">
         <v>-1381554.44</v>
       </c>
-      <c r="F61" s="35">
+      <c r="F61" s="36">
         <f t="shared" si="1"/>
         <v>1381554.44</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B62" s="35">
+      <c r="A62" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B62" s="36">
         <v>750</v>
       </c>
-      <c r="C62" s="35">
+      <c r="C62" s="36">
         <v>22365.4</v>
       </c>
-      <c r="D62" s="35">
+      <c r="D62" s="36">
         <f t="shared" si="0"/>
         <v>22365.4</v>
       </c>
-      <c r="E62" s="35">
+      <c r="E62" s="36">
         <v>-2446454.19</v>
       </c>
-      <c r="F62" s="35">
+      <c r="F62" s="36">
         <f t="shared" si="1"/>
         <v>2446454.19</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="B63" s="35">
+      <c r="A63" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B63" s="36">
         <v>0</v>
       </c>
-      <c r="C63" s="35">
+      <c r="C63" s="36">
         <v>-14560.05</v>
       </c>
-      <c r="D63" s="35">
+      <c r="D63" s="36">
         <f t="shared" si="0"/>
         <v>14560.05</v>
       </c>
-      <c r="E63" s="35">
+      <c r="E63" s="36">
         <v>-2446454.19</v>
       </c>
-      <c r="F63" s="35">
+      <c r="F63" s="36">
         <f t="shared" si="1"/>
         <v>2446454.19</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="B64" s="35">
+      <c r="A64" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B64" s="36">
         <v>48.555999999999997</v>
       </c>
-      <c r="C64" s="35">
+      <c r="C64" s="36">
         <v>-13900.95</v>
       </c>
-      <c r="D64" s="35">
+      <c r="D64" s="36">
         <f t="shared" si="0"/>
         <v>13900.95</v>
       </c>
-      <c r="E64" s="35">
+      <c r="E64" s="36">
         <v>-1751849.93</v>
       </c>
-      <c r="F64" s="35">
+      <c r="F64" s="36">
         <f t="shared" si="1"/>
         <v>1751849.93</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="B65" s="35">
+      <c r="A65" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B65" s="36">
         <v>97.111000000000004</v>
       </c>
-      <c r="C65" s="35">
+      <c r="C65" s="36">
         <v>-12343.67</v>
       </c>
-      <c r="D65" s="35">
+      <c r="D65" s="36">
         <f t="shared" si="0"/>
         <v>12343.67</v>
       </c>
-      <c r="E65" s="35">
+      <c r="E65" s="36">
         <v>-1111054.42</v>
       </c>
-      <c r="F65" s="35">
+      <c r="F65" s="36">
         <f t="shared" si="1"/>
         <v>1111054.42</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="B66" s="35">
+      <c r="A66" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B66" s="36">
         <v>145.667</v>
       </c>
-      <c r="C66" s="35">
+      <c r="C66" s="36">
         <v>-9888.2000000000007</v>
       </c>
-      <c r="D66" s="35">
+      <c r="D66" s="36">
         <f t="shared" si="0"/>
         <v>9888.2000000000007</v>
       </c>
-      <c r="E66" s="35">
+      <c r="E66" s="36">
         <v>-567679.65</v>
       </c>
-      <c r="F66" s="35">
+      <c r="F66" s="36">
         <f t="shared" si="1"/>
         <v>567679.65</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="B67" s="35">
+      <c r="A67" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B67" s="36">
         <v>194.22200000000001</v>
       </c>
-      <c r="C67" s="35">
+      <c r="C67" s="36">
         <v>-6790.74</v>
       </c>
-      <c r="D67" s="35">
+      <c r="D67" s="36">
         <f t="shared" si="0"/>
         <v>6790.74</v>
       </c>
-      <c r="E67" s="35">
+      <c r="E67" s="36">
         <v>-161475.72</v>
       </c>
-      <c r="F67" s="35">
+      <c r="F67" s="36">
         <f t="shared" si="1"/>
         <v>161475.72</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="B68" s="35">
+      <c r="A68" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B68" s="36">
         <v>242.77799999999999</v>
       </c>
-      <c r="C68" s="35">
+      <c r="C68" s="36">
         <v>-3452.53</v>
       </c>
-      <c r="D68" s="35">
+      <c r="D68" s="36">
         <f t="shared" si="0"/>
         <v>3452.53</v>
       </c>
-      <c r="E68" s="35">
+      <c r="E68" s="36">
         <v>87315.47</v>
       </c>
-      <c r="F68" s="35">
+      <c r="F68" s="36">
         <f t="shared" si="1"/>
         <v>87315.47</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="B69" s="35">
+      <c r="A69" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B69" s="36">
         <v>291.33300000000003</v>
       </c>
-      <c r="C69" s="35">
+      <c r="C69" s="36">
         <v>-338.8</v>
       </c>
-      <c r="D69" s="35">
+      <c r="D69" s="36">
         <f t="shared" ref="D69:D80" si="2">ABS(C69)</f>
         <v>338.8</v>
       </c>
-      <c r="E69" s="35">
+      <c r="E69" s="36">
         <v>178099.25</v>
       </c>
-      <c r="F69" s="35">
+      <c r="F69" s="36">
         <f t="shared" ref="F69:F80" si="3">ABS(E69)</f>
         <v>178099.25</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="B70" s="35">
+      <c r="A70" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B70" s="36">
         <v>339.88900000000001</v>
       </c>
-      <c r="C70" s="35">
+      <c r="C70" s="36">
         <v>2463.1999999999998</v>
       </c>
-      <c r="D70" s="35">
+      <c r="D70" s="36">
         <f t="shared" si="2"/>
         <v>2463.1999999999998</v>
       </c>
-      <c r="E70" s="35">
+      <c r="E70" s="36">
         <v>125262.08</v>
       </c>
-      <c r="F70" s="35">
+      <c r="F70" s="36">
         <f t="shared" si="3"/>
         <v>125262.08</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="B71" s="35">
+      <c r="A71" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B71" s="36">
         <v>388.44400000000002</v>
       </c>
-      <c r="C71" s="35">
+      <c r="C71" s="36">
         <v>4953.4799999999996</v>
       </c>
-      <c r="D71" s="35">
+      <c r="D71" s="36">
         <f t="shared" si="2"/>
         <v>4953.4799999999996</v>
       </c>
-      <c r="E71" s="35">
+      <c r="E71" s="36">
         <v>-56059.82</v>
       </c>
-      <c r="F71" s="35">
+      <c r="F71" s="36">
         <f t="shared" si="3"/>
         <v>56059.82</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="B72" s="35">
+      <c r="A72" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B72" s="36">
         <v>437</v>
       </c>
-      <c r="C72" s="35">
+      <c r="C72" s="36">
         <v>7132.02</v>
       </c>
-      <c r="D72" s="35">
+      <c r="D72" s="36">
         <f t="shared" si="2"/>
         <v>7132.02</v>
       </c>
-      <c r="E72" s="35">
+      <c r="E72" s="36">
         <v>-350730.22</v>
       </c>
-      <c r="F72" s="35">
+      <c r="F72" s="36">
         <f t="shared" si="3"/>
         <v>350730.22</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B73" s="35">
+      <c r="A73" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B73" s="36">
         <v>0</v>
       </c>
-      <c r="C73" s="35">
+      <c r="C73" s="36">
         <v>-6811.32</v>
       </c>
-      <c r="D73" s="35">
+      <c r="D73" s="36">
         <f t="shared" si="2"/>
         <v>6811.32</v>
       </c>
-      <c r="E73" s="35">
+      <c r="E73" s="36">
         <v>-350730.22</v>
       </c>
-      <c r="F73" s="35">
+      <c r="F73" s="36">
         <f t="shared" si="3"/>
         <v>350730.22</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B74" s="35">
+      <c r="A74" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B74" s="36">
         <v>49</v>
       </c>
-      <c r="C74" s="35">
+      <c r="C74" s="36">
         <v>-6195.54</v>
       </c>
-      <c r="D74" s="35">
+      <c r="D74" s="36">
         <f t="shared" si="2"/>
         <v>6195.54</v>
       </c>
-      <c r="E74" s="35">
+      <c r="E74" s="36">
         <v>-28763.79</v>
       </c>
-      <c r="F74" s="35">
+      <c r="F74" s="36">
         <f t="shared" si="3"/>
         <v>28763.79</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B75" s="35">
+      <c r="A75" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B75" s="36">
         <v>98</v>
       </c>
-      <c r="C75" s="35">
+      <c r="C75" s="36">
         <v>-4772.05</v>
       </c>
-      <c r="D75" s="35">
+      <c r="D75" s="36">
         <f t="shared" si="2"/>
         <v>4772.05</v>
       </c>
-      <c r="E75" s="35">
+      <c r="E75" s="36">
         <v>243240.48</v>
       </c>
-      <c r="F75" s="35">
+      <c r="F75" s="36">
         <f t="shared" si="3"/>
         <v>243240.48</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B76" s="35">
+      <c r="A76" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B76" s="36">
         <v>147</v>
       </c>
-      <c r="C76" s="35">
+      <c r="C76" s="36">
         <v>-2540.85</v>
       </c>
-      <c r="D76" s="35">
+      <c r="D76" s="36">
         <f t="shared" si="2"/>
         <v>2540.85</v>
       </c>
-      <c r="E76" s="35">
+      <c r="E76" s="36">
         <v>425704.73</v>
       </c>
-      <c r="F76" s="35">
+      <c r="F76" s="36">
         <f t="shared" si="3"/>
         <v>425704.73</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B77" s="35">
+      <c r="A77" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B77" s="36">
         <v>196</v>
       </c>
-      <c r="C77" s="35">
+      <c r="C77" s="36">
         <v>369.52</v>
       </c>
-      <c r="D77" s="35">
+      <c r="D77" s="36">
         <f t="shared" si="2"/>
         <v>369.52</v>
       </c>
-      <c r="E77" s="35">
+      <c r="E77" s="36">
         <v>479878.86</v>
       </c>
-      <c r="F77" s="35">
+      <c r="F77" s="36">
         <f t="shared" si="3"/>
         <v>479878.86</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B78" s="35">
+      <c r="A78" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B78" s="36">
         <v>245</v>
       </c>
-      <c r="C78" s="35">
+      <c r="C78" s="36">
         <v>2729.01</v>
       </c>
-      <c r="D78" s="35">
+      <c r="D78" s="36">
         <f t="shared" si="2"/>
         <v>2729.01</v>
       </c>
-      <c r="E78" s="35">
+      <c r="E78" s="36">
         <v>400457.34</v>
       </c>
-      <c r="F78" s="35">
+      <c r="F78" s="36">
         <f t="shared" si="3"/>
         <v>400457.34</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B79" s="35">
+      <c r="A79" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B79" s="36">
         <v>294</v>
       </c>
-      <c r="C79" s="35">
+      <c r="C79" s="36">
         <v>4229.47</v>
       </c>
-      <c r="D79" s="35">
+      <c r="D79" s="36">
         <f t="shared" si="2"/>
         <v>4229.47</v>
       </c>
-      <c r="E79" s="35">
+      <c r="E79" s="36">
         <v>226466.96</v>
       </c>
-      <c r="F79" s="35">
+      <c r="F79" s="36">
         <f t="shared" si="3"/>
         <v>226466.96</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B80" s="35">
+      <c r="A80" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B80" s="36">
         <v>343</v>
       </c>
-      <c r="C80" s="35">
+      <c r="C80" s="36">
         <v>4870.91</v>
       </c>
-      <c r="D80" s="35">
+      <c r="D80" s="36">
         <f t="shared" si="2"/>
         <v>4870.91</v>
       </c>
-      <c r="E80" s="35">
+      <c r="E80" s="36">
         <v>-9.8879999999999999E-11</v>
       </c>
-      <c r="F80" s="35">
+      <c r="F80" s="36">
         <f t="shared" si="3"/>
         <v>9.8879999999999999E-11</v>
       </c>

</xml_diff>

<commit_message>
Tablas listas para pegar al informe
</commit_message>
<xml_diff>
--- a/Tarea 06/Vigas.xlsx
+++ b/Tarea 06/Vigas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ramos Ingenieria\12° Semestre\Proyecto de Hormigón Armado\Tarea 06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA902249-799C-4000-BFAF-7A556FDBD094}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED35D8F4-B2C6-4BD1-B18D-E88096EC4BF0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{B94BBB90-C174-4AC8-BDFB-4A9825C26EEC}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="68">
   <si>
     <t>0101</t>
   </si>
@@ -181,12 +181,6 @@
     <t>Sismo</t>
   </si>
   <si>
-    <t>ETABS</t>
-  </si>
-  <si>
-    <t>SAP</t>
-  </si>
-  <si>
     <t>$M [tonf \cdot m] $</t>
   </si>
   <si>
@@ -217,9 +211,6 @@
     <t>$1,2 \dot PP+1 \cdot SC+1,4 \cdot Sismo$</t>
   </si>
   <si>
-    <t>$E \phi 10 @ 20$</t>
-  </si>
-  <si>
     <t>Eje K</t>
   </si>
   <si>
@@ -239,6 +230,9 @@
   </si>
   <si>
     <t>$1,2 \cdot PP+1,6 \dot SC$</t>
+  </si>
+  <si>
+    <t>$A_{s.min} [cm^2]$</t>
   </si>
 </sst>
 </file>
@@ -622,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -672,12 +666,6 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -685,12 +673,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -746,6 +728,75 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -759,58 +810,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -851,7 +869,7 @@
       <sheetName val="Deformaciones"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="7">
           <cell r="L7">
@@ -947,6 +965,37 @@
             <v>0129</v>
           </cell>
         </row>
+        <row r="47">
+          <cell r="C47"/>
+          <cell r="D47"/>
+          <cell r="E47"/>
+          <cell r="F47"/>
+          <cell r="G47"/>
+          <cell r="H47"/>
+          <cell r="I47"/>
+          <cell r="J47"/>
+          <cell r="K47"/>
+          <cell r="L47"/>
+          <cell r="M47"/>
+          <cell r="N47"/>
+          <cell r="O47"/>
+          <cell r="P47"/>
+          <cell r="Q47"/>
+          <cell r="R47"/>
+          <cell r="S47"/>
+          <cell r="T47"/>
+          <cell r="U47"/>
+          <cell r="V47"/>
+          <cell r="W47"/>
+          <cell r="X47"/>
+          <cell r="Y47"/>
+          <cell r="Z47"/>
+          <cell r="AA47"/>
+          <cell r="AB47"/>
+          <cell r="AC47"/>
+          <cell r="AD47"/>
+          <cell r="AE47"/>
+        </row>
         <row r="48">
           <cell r="C48">
             <v>5</v>
@@ -1303,6 +1352,37 @@
             <v>6</v>
           </cell>
         </row>
+        <row r="52">
+          <cell r="C52"/>
+          <cell r="D52"/>
+          <cell r="E52"/>
+          <cell r="F52"/>
+          <cell r="G52"/>
+          <cell r="H52"/>
+          <cell r="I52"/>
+          <cell r="J52"/>
+          <cell r="K52"/>
+          <cell r="L52"/>
+          <cell r="M52"/>
+          <cell r="N52"/>
+          <cell r="O52"/>
+          <cell r="P52"/>
+          <cell r="Q52"/>
+          <cell r="R52"/>
+          <cell r="S52"/>
+          <cell r="T52"/>
+          <cell r="U52"/>
+          <cell r="V52"/>
+          <cell r="W52"/>
+          <cell r="X52"/>
+          <cell r="Y52"/>
+          <cell r="Z52"/>
+          <cell r="AA52"/>
+          <cell r="AB52"/>
+          <cell r="AC52"/>
+          <cell r="AD52"/>
+          <cell r="AE52"/>
+        </row>
         <row r="53">
           <cell r="C53">
             <v>1.1000000000000001</v>
@@ -2193,6 +2273,37 @@
             <v>1.39</v>
           </cell>
         </row>
+        <row r="63">
+          <cell r="C63"/>
+          <cell r="D63"/>
+          <cell r="E63"/>
+          <cell r="F63"/>
+          <cell r="G63"/>
+          <cell r="H63"/>
+          <cell r="I63"/>
+          <cell r="J63"/>
+          <cell r="K63"/>
+          <cell r="L63"/>
+          <cell r="M63"/>
+          <cell r="N63"/>
+          <cell r="O63"/>
+          <cell r="P63"/>
+          <cell r="Q63"/>
+          <cell r="R63"/>
+          <cell r="S63"/>
+          <cell r="T63"/>
+          <cell r="U63"/>
+          <cell r="V63"/>
+          <cell r="W63"/>
+          <cell r="X63"/>
+          <cell r="Y63"/>
+          <cell r="Z63"/>
+          <cell r="AA63"/>
+          <cell r="AB63"/>
+          <cell r="AC63"/>
+          <cell r="AD63"/>
+          <cell r="AE63"/>
+        </row>
         <row r="64">
           <cell r="C64">
             <v>500</v>
@@ -2731,7 +2842,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="64">
           <cell r="B64" t="str">
@@ -2739,18 +2850,18 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3053,10 +3164,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F51FF3-724F-45F5-8F3F-FC55661E6BD0}">
-  <dimension ref="B2:O56"/>
+  <dimension ref="B2:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31:J32"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -3071,11 +3182,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="64" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="64" t="s">
-        <v>60</v>
+      <c r="B2" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3146,11 +3257,11 @@
         <v>178</v>
       </c>
       <c r="G5" s="11">
-        <f>C5*$E5/100</f>
+        <f t="shared" ref="G5:H7" si="0">C5*$E5/100</f>
         <v>7.5225000000000009</v>
       </c>
       <c r="H5" s="12">
-        <f>D5*$E5/100</f>
+        <f t="shared" si="0"/>
         <v>8.85</v>
       </c>
       <c r="I5" s="9" t="s">
@@ -3198,11 +3309,11 @@
         <v>220</v>
       </c>
       <c r="G6" s="15">
-        <f>C6*$E6/100</f>
+        <f t="shared" si="0"/>
         <v>9.307500000000001</v>
       </c>
       <c r="H6" s="16">
-        <f>D6*$E6/100</f>
+        <f t="shared" si="0"/>
         <v>10.95</v>
       </c>
       <c r="I6" s="13" t="s">
@@ -3223,336 +3334,336 @@
         <v>149</v>
       </c>
       <c r="N6" s="15">
-        <f t="shared" ref="N6:N7" si="0">J6*$L6/100</f>
+        <f t="shared" ref="N6:N7" si="1">J6*$L6/100</f>
         <v>12.112500000000002</v>
       </c>
       <c r="O6" s="16">
-        <f t="shared" ref="O6:O7" si="1">K6*$L6/100</f>
+        <f t="shared" ref="O6:O7" si="2">K6*$L6/100</f>
         <v>14.25</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="62">
         <f>HLOOKUP($B7,'[1]-1'!$C$46:$AE$69,D$15)</f>
         <v>425.00000000000006</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="62">
         <f>HLOOKUP($B7,'[1]-1'!$C$46:$AE$69,C$15)</f>
         <v>500</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="17">
         <v>2.5499999999999998</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="17">
         <v>498</v>
       </c>
-      <c r="G7" s="20">
-        <f>C7*$E7/100</f>
+      <c r="G7" s="18">
+        <f t="shared" si="0"/>
         <v>10.8375</v>
       </c>
-      <c r="H7" s="21">
-        <f>D7*$E7/100</f>
+      <c r="H7" s="19">
+        <f t="shared" si="0"/>
         <v>12.75</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="62">
         <f>HLOOKUP($I7,'[1]-1'!$C$46:$AE$69,D$15)</f>
         <v>425.00000000000006</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="62">
         <f>HLOOKUP($I7,'[1]-1'!$C$46:$AE$69,C$15)</f>
         <v>500</v>
       </c>
-      <c r="L7" s="19">
+      <c r="L7" s="17">
         <v>2.85</v>
       </c>
-      <c r="M7" s="19">
+      <c r="M7" s="17">
         <v>750</v>
       </c>
-      <c r="N7" s="20">
-        <f t="shared" si="0"/>
+      <c r="N7" s="18">
+        <f t="shared" si="1"/>
         <v>12.112500000000002</v>
       </c>
-      <c r="O7" s="21">
-        <f t="shared" si="1"/>
+      <c r="O7" s="19">
+        <f t="shared" si="2"/>
         <v>14.25</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="22"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="24">
+      <c r="B8" s="61"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="20">
         <v>2.5</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="20">
         <v>252</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="21">
         <f>C7*$E8/100</f>
         <v>10.625000000000002</v>
       </c>
-      <c r="H8" s="26">
+      <c r="H8" s="22">
         <f>D7*$E8/100</f>
         <v>12.5</v>
       </c>
-      <c r="I8" s="22"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="24">
+      <c r="I8" s="61"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="20">
         <v>2.84</v>
       </c>
-      <c r="M8" s="24">
+      <c r="M8" s="20">
         <v>273</v>
       </c>
-      <c r="N8" s="25">
+      <c r="N8" s="21">
         <f>J7*$L8/100</f>
         <v>12.07</v>
       </c>
-      <c r="O8" s="26">
+      <c r="O8" s="22">
         <f>K7*$L8/100</f>
         <v>14.2</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="62">
         <f>HLOOKUP($B9,'[1]-1'!$C$46:$AE$69,D$15)</f>
         <v>425.00000000000006</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="62">
         <f>HLOOKUP($B9,'[1]-1'!$C$46:$AE$69,C$15)</f>
         <v>500</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="17">
         <v>2.54</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="17">
         <v>500</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="18">
         <f>C9*$E9/100</f>
         <v>10.795000000000002</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="19">
         <f>D9*$E9/100</f>
         <v>12.7</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="62">
         <f>HLOOKUP($I9,'[1]-1'!$C$46:$AE$69,D$15)</f>
         <v>425.00000000000006</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="62">
         <f>HLOOKUP($I9,'[1]-1'!$C$46:$AE$69,C$15)</f>
         <v>500</v>
       </c>
-      <c r="L9" s="19">
+      <c r="L9" s="17">
         <v>3.04</v>
       </c>
-      <c r="M9" s="19">
+      <c r="M9" s="17">
         <v>442</v>
       </c>
-      <c r="N9" s="20">
+      <c r="N9" s="18">
         <f>J9*$L9/100</f>
         <v>12.920000000000002</v>
       </c>
-      <c r="O9" s="21">
+      <c r="O9" s="19">
         <f>K9*$L9/100</f>
         <v>15.2</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="22"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24">
+      <c r="B10" s="61"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="20">
         <v>2.48</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="20">
         <v>250</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="21">
         <f>C9*$E10/100</f>
         <v>10.540000000000003</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10" s="22">
         <f>D9*$E10/100</f>
         <v>12.4</v>
       </c>
-      <c r="I10" s="22"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="24">
+      <c r="I10" s="61"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="20">
         <v>2.84</v>
       </c>
-      <c r="M10" s="24">
+      <c r="M10" s="20">
         <v>280</v>
       </c>
-      <c r="N10" s="25">
+      <c r="N10" s="21">
         <f>J9*$L10/100</f>
         <v>12.07</v>
       </c>
-      <c r="O10" s="26">
+      <c r="O10" s="22">
         <f>K9*$L10/100</f>
         <v>14.2</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="62">
         <f>HLOOKUP($B11,'[1]-1'!$C$46:$AE$69,D$15)</f>
         <v>425.00000000000006</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="62">
         <f>HLOOKUP($B11,'[1]-1'!$C$46:$AE$69,C$15)</f>
         <v>500</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="17">
         <v>2.5099999999999998</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="17">
         <v>501</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="18">
         <f>C11*$E11/100</f>
         <v>10.6675</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="19">
         <f>D11*$E11/100</f>
         <v>12.55</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="62">
         <f>HLOOKUP($I11,'[1]-1'!$C$46:$AE$69,D$15)</f>
         <v>425.00000000000006</v>
       </c>
-      <c r="K11" s="18">
+      <c r="K11" s="62">
         <f>HLOOKUP($I11,'[1]-1'!$C$46:$AE$69,C$15)</f>
         <v>500</v>
       </c>
-      <c r="L11" s="19">
+      <c r="L11" s="17">
         <v>2.87</v>
       </c>
-      <c r="M11" s="19">
+      <c r="M11" s="17">
         <v>459</v>
       </c>
-      <c r="N11" s="20">
+      <c r="N11" s="18">
         <f>J11*$L11/100</f>
         <v>12.197500000000002</v>
       </c>
-      <c r="O11" s="21">
+      <c r="O11" s="19">
         <f>K11*$L11/100</f>
         <v>14.35</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="22"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="24">
+      <c r="B12" s="61"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="20">
         <v>2.4700000000000002</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="20">
         <v>251</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="21">
         <f>C11*$E12/100</f>
         <v>10.497500000000002</v>
       </c>
-      <c r="H12" s="26">
+      <c r="H12" s="22">
         <f>D11*$E12/100</f>
         <v>12.35</v>
       </c>
-      <c r="I12" s="22"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="24">
+      <c r="I12" s="61"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="20">
         <v>2.98</v>
       </c>
-      <c r="M12" s="24">
+      <c r="M12" s="20">
         <v>293</v>
       </c>
-      <c r="N12" s="25">
+      <c r="N12" s="21">
         <f>J11*$L12/100</f>
         <v>12.665000000000003</v>
       </c>
-      <c r="O12" s="26">
+      <c r="O12" s="22">
         <f>K11*$L12/100</f>
         <v>14.9</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="28">
+      <c r="C13" s="24">
         <f>HLOOKUP($B13,'[1]-1'!$C$46:$AE$69,D$15)</f>
         <v>425.00000000000006</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="24">
         <f>HLOOKUP($B13,'[1]-1'!$C$46:$AE$69,C$15)</f>
         <v>500</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E13" s="24">
         <v>2.4700000000000002</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="24">
         <v>255</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G13" s="25">
         <f>C13*$E13/100</f>
         <v>10.497500000000002</v>
       </c>
-      <c r="H13" s="30">
+      <c r="H13" s="26">
         <f>D13*$E13/100</f>
         <v>12.35</v>
       </c>
-      <c r="I13" s="27" t="s">
+      <c r="I13" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="J13" s="28">
+      <c r="J13" s="24">
         <f>HLOOKUP($I13,'[1]-1'!$C$46:$AE$69,D$15)</f>
         <v>425.00000000000006</v>
       </c>
-      <c r="K13" s="28">
+      <c r="K13" s="24">
         <f>HLOOKUP($I13,'[1]-1'!$C$46:$AE$69,C$15)</f>
         <v>500</v>
       </c>
-      <c r="L13" s="28">
+      <c r="L13" s="24">
         <v>2.5499999999999998</v>
       </c>
-      <c r="M13" s="28">
+      <c r="M13" s="24">
         <v>252</v>
       </c>
-      <c r="N13" s="29">
+      <c r="N13" s="25">
         <f>J13*$L13/100</f>
         <v>10.8375</v>
       </c>
-      <c r="O13" s="30">
+      <c r="O13" s="26">
         <f>K13*$L13/100</f>
         <v>12.75</v>
       </c>
     </row>
     <row r="14" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="31"/>
+      <c r="B14" s="27"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="31"/>
-      <c r="N14" s="32"/>
-      <c r="O14" s="32"/>
+      <c r="I14" s="27"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
     </row>
     <row r="15" spans="2:15" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="1">
@@ -3563,45 +3674,65 @@
       </c>
     </row>
     <row r="16" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="34">
+      <c r="C16" s="30">
         <f>0.3*0.5*'[1]-1'!L$7</f>
         <v>375</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G17" s="61" t="s">
+    <row r="17" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="43"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="61"/>
-    </row>
-    <row r="18" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="56" t="s">
+      <c r="I17" s="57"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="2"/>
+    </row>
+    <row r="18" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="70"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="I18" s="52">
+        <f>1.53</f>
+        <v>1.53</v>
+      </c>
+      <c r="K18" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="L18" s="74" t="s">
+        <v>53</v>
+      </c>
+      <c r="M18" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="G18" s="49" t="s">
+      <c r="N18" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="H18" s="62" t="s">
-        <v>66</v>
-      </c>
-      <c r="N18" s="2"/>
-      <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="51" t="s">
-        <v>52</v>
+      <c r="O18" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="58" t="s">
+        <v>50</v>
       </c>
       <c r="C19" s="1">
         <v>7.7839999999999998</v>
@@ -3609,125 +3740,169 @@
       <c r="D19" s="1">
         <v>7.96</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="28">
         <f>C19*1.2+D19*1.6</f>
         <v>22.076799999999999</v>
       </c>
-      <c r="F19" s="63"/>
-      <c r="G19" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19" s="60" t="s">
-        <v>65</v>
-      </c>
-      <c r="M19" s="2"/>
-      <c r="O19" s="1"/>
-    </row>
-    <row r="20" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" s="57"/>
-      <c r="C20" s="53">
+      <c r="F19" s="28"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="K19" s="71">
+        <f>1.53</f>
+        <v>1.53</v>
+      </c>
+      <c r="L19" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="M19" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="N19" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="O19" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="B20" s="59"/>
+      <c r="C20" s="44">
         <v>-11.079000000000001</v>
       </c>
-      <c r="D20" s="53">
+      <c r="D20" s="44">
         <v>-11.016999999999999</v>
       </c>
-      <c r="E20" s="58">
+      <c r="E20" s="49">
         <f>C20*1.2+D20*1.6</f>
         <v>-30.921999999999997</v>
       </c>
-      <c r="F20" s="63"/>
-      <c r="G20" s="53" t="s">
-        <v>57</v>
-      </c>
-      <c r="H20" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="M20" s="2"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="N20" s="2"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="50">
+    <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="41">
         <v>8.048</v>
       </c>
-      <c r="D21" s="50">
+      <c r="D21" s="41">
         <v>7.9409999999999998</v>
       </c>
-      <c r="E21" s="59">
+      <c r="E21" s="50">
         <f>C21*1.2+D21*1.6</f>
         <v>22.363199999999999</v>
       </c>
-      <c r="F21" s="63"/>
-      <c r="G21" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="H21" s="50" t="s">
+      <c r="F21" s="49"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="N21" s="2"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="43"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="M21" s="2"/>
-      <c r="O21" s="1"/>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="G22" s="1"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="1"/>
-    </row>
-    <row r="26" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B26" s="64" t="s">
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+    </row>
+    <row r="26" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="B26" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="64" t="s">
+      <c r="C26" s="54" t="s">
         <v>46</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F28" s="52"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="52"/>
-      <c r="I28" s="52"/>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C29" s="1">
         <v>90</v>
       </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="32">
+      <c r="C30" s="28">
         <v>18.1998</v>
       </c>
-      <c r="F30" s="32"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="32"/>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F30" s="28"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="32">
+      <c r="C31" s="28">
         <v>14.436199999999999</v>
       </c>
-      <c r="F31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="32"/>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F31" s="28"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>20</v>
       </c>
@@ -3735,194 +3910,249 @@
         <v>200</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="J32" s="32"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="48"/>
+      <c r="L32" s="48"/>
+      <c r="M32" s="48"/>
+      <c r="N32" s="48"/>
+      <c r="O32" s="51"/>
     </row>
     <row r="33" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="32"/>
+      <c r="C33" s="28"/>
       <c r="G33" s="1"/>
-      <c r="J33" s="35"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="72"/>
+      <c r="K33" s="48"/>
+      <c r="L33" s="48"/>
+      <c r="M33" s="48"/>
+      <c r="N33" s="48"/>
+      <c r="O33" s="51"/>
     </row>
     <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="65" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" s="65"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="61" t="s">
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="I34" s="61"/>
-      <c r="L34" s="2"/>
-      <c r="O34" s="1"/>
+      <c r="I34" s="57"/>
+      <c r="K34" s="51"/>
+      <c r="L34" s="48"/>
+      <c r="M34" s="48"/>
+      <c r="N34" s="48"/>
+      <c r="O34" s="48"/>
     </row>
     <row r="35" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="56" t="s">
+      <c r="B35" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="I35" s="52">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="K35" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="L35" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="M35" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" s="56" t="s">
-        <v>49</v>
-      </c>
-      <c r="F35" s="56" t="s">
-        <v>61</v>
-      </c>
-      <c r="G35" s="1"/>
-      <c r="H35" s="49" t="s">
+      <c r="N35" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="I35" s="62" t="s">
-        <v>66</v>
-      </c>
-      <c r="L35" s="2"/>
-      <c r="O35" s="1"/>
+      <c r="O35" s="74" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="36" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B36" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="53">
+      <c r="B36" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="44">
         <v>11.33</v>
       </c>
-      <c r="D36" s="53">
+      <c r="D36" s="44">
         <v>0.53</v>
       </c>
-      <c r="E36" s="54">
+      <c r="E36" s="45">
         <v>14.436199999999999</v>
       </c>
-      <c r="F36" s="58">
+      <c r="F36" s="49">
         <f>C36*1.2+D36*1+E36*1.4</f>
         <v>34.336679999999994</v>
       </c>
       <c r="G36" s="1"/>
-      <c r="H36" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="I36" s="60" t="s">
-        <v>66</v>
-      </c>
-      <c r="L36" s="2"/>
-      <c r="O36" s="1"/>
+      <c r="H36" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="I36" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="K36" s="71">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="L36" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="M36" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="N36" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="O36" s="14" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="37" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="C37" s="50">
+      <c r="B37" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="41">
         <v>5.2</v>
       </c>
-      <c r="D37" s="50">
+      <c r="D37" s="41">
         <v>0.312</v>
       </c>
-      <c r="E37" s="55">
+      <c r="E37" s="46">
         <v>18.1998</v>
       </c>
-      <c r="F37" s="59">
+      <c r="F37" s="50">
         <f>C37*1.2+D37*1+E37*1.4</f>
         <v>32.03172</v>
       </c>
       <c r="G37" s="1"/>
-      <c r="H37" s="53" t="s">
-        <v>57</v>
-      </c>
-      <c r="I37" s="60" t="s">
-        <v>62</v>
+      <c r="H37" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="I37" s="51" t="s">
+        <v>63</v>
       </c>
       <c r="L37" s="2"/>
       <c r="O37" s="1"/>
     </row>
-    <row r="38" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="D38" s="51"/>
-      <c r="F38" s="58"/>
+    <row r="38" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="C38" s="68"/>
+      <c r="D38" s="68"/>
+      <c r="F38" s="49"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="I38" s="50" t="s">
-        <v>48</v>
+      <c r="H38" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="I38" s="51" t="s">
+        <v>41</v>
       </c>
       <c r="L38" s="2"/>
       <c r="O38" s="1"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C39" s="53"/>
+    <row r="39" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="44"/>
       <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="C40" s="53"/>
-      <c r="F40" s="1">
+      <c r="H39" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="I39" s="55" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C40" s="44"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+    </row>
+    <row r="41" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="C41" s="44"/>
+      <c r="F41" s="1">
         <v>1.4098999999999999</v>
       </c>
-      <c r="G40" s="1">
+      <c r="G41" s="1">
         <v>-0.20699999999999999</v>
       </c>
-      <c r="H40" s="1">
+      <c r="H41" s="43">
         <v>14.436199999999999</v>
       </c>
-      <c r="I40" s="58">
-        <f>F40*1.2+G40*1+H40*1.4</f>
+      <c r="I41" s="49">
+        <f>F41*1.2+G41*1+H41*1.4</f>
         <v>21.695559999999997</v>
       </c>
     </row>
-    <row r="41" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="53"/>
-      <c r="F41" s="1">
+    <row r="42" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="44"/>
+      <c r="F42" s="1">
         <v>3.2690000000000001</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G42" s="2">
         <v>0.17899999999999999</v>
       </c>
-      <c r="H41" s="1">
+      <c r="H42" s="43">
         <v>18.1998</v>
       </c>
-      <c r="I41" s="59">
-        <f>F41*1.2+G41*1+H41*1.4</f>
+      <c r="I42" s="50">
+        <f>F42*1.2+G42*1+H42*1.4</f>
         <v>29.581519999999998</v>
       </c>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C42" s="53"/>
-    </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C43" s="53"/>
-      <c r="F43" s="66"/>
-      <c r="G43" s="66"/>
-      <c r="H43" s="66"/>
-      <c r="I43" s="66"/>
+      <c r="C43" s="44"/>
+      <c r="F43" s="56"/>
+      <c r="G43" s="56"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="J44" s="32"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="28"/>
     </row>
     <row r="45" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B45" s="64" t="s">
+      <c r="B45" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="64" t="s">
+      <c r="C45" s="54" t="s">
         <v>46</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G45" s="1"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="G46" s="1"/>
+      <c r="H46" s="43"/>
+      <c r="I46" s="43"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G47" s="1"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="43"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
@@ -3932,8 +4162,10 @@
         <v>184</v>
       </c>
       <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H48" s="43"/>
+      <c r="I48" s="43"/>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>20</v>
       </c>
@@ -3941,113 +4173,163 @@
         <v>200</v>
       </c>
       <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H49" s="43"/>
+      <c r="I49" s="43"/>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G51" s="35"/>
-    </row>
-    <row r="52" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="C52" s="56" t="s">
+      <c r="H50" s="43"/>
+      <c r="I50" s="43"/>
+    </row>
+    <row r="51" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G51" s="31"/>
+      <c r="H51" s="43"/>
+      <c r="I51" s="43"/>
+    </row>
+    <row r="52" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="D52" s="56" t="s">
+      <c r="D52" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="E52" s="56" t="s">
+      <c r="E52" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="G52" s="35"/>
-      <c r="H52" s="61" t="s">
+      <c r="F52" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="G52" s="31"/>
+      <c r="H52" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="I52" s="61"/>
-    </row>
-    <row r="53" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="C53" s="53">
+      <c r="I52" s="57"/>
+    </row>
+    <row r="53" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C53" s="44">
         <v>10.673299999999999</v>
       </c>
-      <c r="D53" s="53">
+      <c r="D53" s="44">
         <v>2.9523000000000001</v>
       </c>
-      <c r="E53" s="54">
+      <c r="E53" s="45">
         <v>5.2817999999999996</v>
       </c>
-      <c r="F53" s="56" t="s">
-        <v>61</v>
-      </c>
-      <c r="G53" s="1"/>
-      <c r="H53" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="I53" s="62" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="54" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="C54" s="50">
-        <v>6.7065000000000001</v>
-      </c>
-      <c r="D54" s="50">
-        <v>1.5425</v>
-      </c>
-      <c r="E54" s="55">
-        <v>2.4342000000000001</v>
-      </c>
-      <c r="F54" s="58">
+      <c r="F53" s="49">
         <f>C53*1.2+D53*1+E53*1.4</f>
         <v>23.154779999999999</v>
       </c>
-      <c r="G54" s="1"/>
-      <c r="H54" s="53" t="s">
+      <c r="G53" s="1"/>
+      <c r="H53" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="I53" s="52">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="K53" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="L53" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="M53" s="73" t="s">
+        <v>54</v>
+      </c>
+      <c r="N53" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="O53" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="I54" s="60" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="55" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="2"/>
-      <c r="F55" s="59">
+    </row>
+    <row r="54" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C54" s="41">
+        <v>6.7065000000000001</v>
+      </c>
+      <c r="D54" s="41">
+        <v>1.5425</v>
+      </c>
+      <c r="E54" s="46">
+        <v>2.4342000000000001</v>
+      </c>
+      <c r="F54" s="50">
         <f>C54*1.2+D54*1+E54*1.4</f>
         <v>12.998180000000001</v>
       </c>
+      <c r="G54" s="1"/>
+      <c r="H54" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="I54" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="K54" s="71">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="L54" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="M54" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="N54" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="O54" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D55" s="2"/>
       <c r="G55" s="1"/>
-      <c r="H55" s="53" t="s">
-        <v>57</v>
-      </c>
-      <c r="I55" s="60" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="56" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H55" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="I55" s="51" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="G56" s="1"/>
-      <c r="H56" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="I56" s="50" t="s">
+      <c r="H56" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="I56" s="51" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H57" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="I57" s="55" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="F28:I28"/>
+  <mergeCells count="22">
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="J11:J12"/>
     <mergeCell ref="B19:B20"/>
-    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="H17:I17"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="C7:C8"/>
@@ -4055,17 +4337,8 @@
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="B9:B10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H52:I52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4083,70 +4356,70 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.140625" style="36"/>
+    <col min="4" max="4" width="9.140625" style="32"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="48"/>
-      <c r="E2" s="45" t="s">
+      <c r="D2" s="67"/>
+      <c r="E2" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="46"/>
+      <c r="F2" s="65"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="39" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="36">
+      <c r="B4" s="32">
         <v>0</v>
       </c>
-      <c r="C4" s="36">
+      <c r="C4" s="32">
         <v>-4770.4399999999996</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="32">
         <f>ABS(C4)</f>
         <v>4770.4399999999996</v>
       </c>
-      <c r="E4" s="44">
+      <c r="E4" s="40">
         <v>1.1640000000000001E-10</v>
       </c>
       <c r="F4">
@@ -4155,1673 +4428,1673 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="36">
+      <c r="B5" s="32">
         <v>50</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="32">
         <v>-4229.8500000000004</v>
       </c>
-      <c r="D5" s="36">
+      <c r="D5" s="32">
         <f t="shared" ref="D5:D68" si="0">ABS(C5)</f>
         <v>4229.8500000000004</v>
       </c>
-      <c r="E5" s="36">
+      <c r="E5" s="32">
         <v>227710.28</v>
       </c>
-      <c r="F5" s="36">
+      <c r="F5" s="32">
         <f t="shared" ref="F5:F68" si="1">ABS(E5)</f>
         <v>227710.28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="36">
+      <c r="B6" s="32">
         <v>100</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="32">
         <v>-3040.58</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D6" s="32">
         <f t="shared" si="0"/>
         <v>3040.58</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="32">
         <v>412173.92</v>
       </c>
-      <c r="F6" s="36">
+      <c r="F6" s="32">
         <f t="shared" si="1"/>
         <v>412173.92</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="36">
+      <c r="B7" s="32">
         <v>150</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="32">
         <v>-1202.6199999999999</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="32">
         <f t="shared" si="0"/>
         <v>1202.6199999999999</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="32">
         <v>520956.74</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="32">
         <f t="shared" si="1"/>
         <v>520956.74</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="36">
+      <c r="B8" s="32">
         <v>200</v>
       </c>
-      <c r="C8" s="36">
+      <c r="C8" s="32">
         <v>1284.02</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="32">
         <f t="shared" si="0"/>
         <v>1284.02</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="32">
         <v>521624.59</v>
       </c>
-      <c r="F8" s="36">
+      <c r="F8" s="32">
         <f t="shared" si="1"/>
         <v>521624.59</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="36">
+      <c r="B9" s="32">
         <v>250</v>
       </c>
-      <c r="C9" s="36">
+      <c r="C9" s="32">
         <v>4419.3500000000004</v>
       </c>
-      <c r="D9" s="36">
+      <c r="D9" s="32">
         <f t="shared" si="0"/>
         <v>4419.3500000000004</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="32">
         <v>381743.27</v>
       </c>
-      <c r="F9" s="36">
+      <c r="F9" s="32">
         <f t="shared" si="1"/>
         <v>381743.27</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="36">
+      <c r="B10" s="32">
         <v>300</v>
       </c>
-      <c r="C10" s="36">
+      <c r="C10" s="32">
         <v>7633.23</v>
       </c>
-      <c r="D10" s="36">
+      <c r="D10" s="32">
         <f t="shared" si="0"/>
         <v>7633.23</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="32">
         <v>77738.47</v>
       </c>
-      <c r="F10" s="36">
+      <c r="F10" s="32">
         <f t="shared" si="1"/>
         <v>77738.47</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="36">
+      <c r="B11" s="32">
         <v>350</v>
       </c>
-      <c r="C11" s="36">
+      <c r="C11" s="32">
         <v>10183.9</v>
       </c>
-      <c r="D11" s="36">
+      <c r="D11" s="32">
         <f t="shared" si="0"/>
         <v>10183.9</v>
       </c>
-      <c r="E11" s="36">
+      <c r="E11" s="32">
         <v>-370468.71</v>
       </c>
-      <c r="F11" s="36">
+      <c r="F11" s="32">
         <f t="shared" si="1"/>
         <v>370468.71</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="36">
+      <c r="B12" s="32">
         <v>400</v>
       </c>
-      <c r="C12" s="36">
+      <c r="C12" s="32">
         <v>12067.59</v>
       </c>
-      <c r="D12" s="36">
+      <c r="D12" s="32">
         <f t="shared" si="0"/>
         <v>12067.59</v>
       </c>
-      <c r="E12" s="36">
+      <c r="E12" s="32">
         <v>-929535.09</v>
       </c>
-      <c r="F12" s="36">
+      <c r="F12" s="32">
         <f t="shared" si="1"/>
         <v>929535.09</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="36">
+      <c r="B13" s="32">
         <v>450</v>
       </c>
-      <c r="C13" s="36">
+      <c r="C13" s="32">
         <v>13284.31</v>
       </c>
-      <c r="D13" s="36">
+      <c r="D13" s="32">
         <f t="shared" si="0"/>
         <v>13284.31</v>
       </c>
-      <c r="E13" s="36">
+      <c r="E13" s="32">
         <v>-1566111.76</v>
       </c>
-      <c r="F13" s="36">
+      <c r="F13" s="32">
         <f t="shared" si="1"/>
         <v>1566111.76</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="36">
+      <c r="B14" s="32">
         <v>500</v>
       </c>
-      <c r="C14" s="36">
+      <c r="C14" s="32">
         <v>13834.05</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D14" s="32">
         <f t="shared" si="0"/>
         <v>13834.05</v>
       </c>
-      <c r="E14" s="36">
+      <c r="E14" s="32">
         <v>-2246849.7999999998</v>
       </c>
-      <c r="F14" s="36">
+      <c r="F14" s="32">
         <f t="shared" si="1"/>
         <v>2246849.7999999998</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="36">
+      <c r="B15" s="32">
         <v>0</v>
       </c>
-      <c r="C15" s="36">
+      <c r="C15" s="32">
         <v>-17845.16</v>
       </c>
-      <c r="D15" s="36">
+      <c r="D15" s="32">
         <f t="shared" si="0"/>
         <v>17845.16</v>
       </c>
-      <c r="E15" s="36">
+      <c r="E15" s="32">
         <v>-2246849.7999999998</v>
       </c>
-      <c r="F15" s="36">
+      <c r="F15" s="32">
         <f t="shared" si="1"/>
         <v>2246849.7999999998</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="36">
+      <c r="B16" s="32">
         <v>50</v>
       </c>
-      <c r="C16" s="36">
+      <c r="C16" s="32">
         <v>-17301.189999999999</v>
       </c>
-      <c r="D16" s="36">
+      <c r="D16" s="32">
         <f t="shared" si="0"/>
         <v>17301.189999999999</v>
       </c>
-      <c r="E16" s="36">
+      <c r="E16" s="32">
         <v>-1365460.12</v>
       </c>
-      <c r="F16" s="36">
+      <c r="F16" s="32">
         <f t="shared" si="1"/>
         <v>1365460.12</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="36">
+      <c r="B17" s="32">
         <v>100</v>
       </c>
-      <c r="C17" s="36">
+      <c r="C17" s="32">
         <v>-16101.76</v>
       </c>
-      <c r="D17" s="36">
+      <c r="D17" s="32">
         <f t="shared" si="0"/>
         <v>16101.76</v>
       </c>
-      <c r="E17" s="36">
+      <c r="E17" s="32">
         <v>-527655.43999999994</v>
       </c>
-      <c r="F17" s="36">
+      <c r="F17" s="32">
         <f t="shared" si="1"/>
         <v>527655.43999999994</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="36">
+      <c r="B18" s="32">
         <v>150</v>
       </c>
-      <c r="C18" s="36">
+      <c r="C18" s="32">
         <v>-14246.88</v>
       </c>
-      <c r="D18" s="36">
+      <c r="D18" s="32">
         <f t="shared" si="0"/>
         <v>14246.88</v>
       </c>
-      <c r="E18" s="36">
+      <c r="E18" s="32">
         <v>233791.71</v>
       </c>
-      <c r="F18" s="36">
+      <c r="F18" s="32">
         <f t="shared" si="1"/>
         <v>233791.71</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="36">
+      <c r="B19" s="32">
         <v>200</v>
       </c>
-      <c r="C19" s="36">
+      <c r="C19" s="32">
         <v>-11736.56</v>
       </c>
-      <c r="D19" s="36">
+      <c r="D19" s="32">
         <f t="shared" si="0"/>
         <v>11736.56</v>
       </c>
-      <c r="E19" s="36">
+      <c r="E19" s="32">
         <v>886108.8</v>
       </c>
-      <c r="F19" s="36">
+      <c r="F19" s="32">
         <f t="shared" si="1"/>
         <v>886108.8</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="36">
+      <c r="B20" s="32">
         <v>250</v>
       </c>
-      <c r="C20" s="36">
+      <c r="C20" s="32">
         <v>-8570.7800000000007</v>
       </c>
-      <c r="D20" s="36">
+      <c r="D20" s="32">
         <f t="shared" si="0"/>
         <v>8570.7800000000007</v>
       </c>
-      <c r="E20" s="36">
+      <c r="E20" s="32">
         <v>1396523.28</v>
       </c>
-      <c r="F20" s="36">
+      <c r="F20" s="32">
         <f t="shared" si="1"/>
         <v>1396523.28</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="36">
+      <c r="B21" s="32">
         <v>300</v>
       </c>
-      <c r="C21" s="36">
+      <c r="C21" s="32">
         <v>-4895.6099999999997</v>
       </c>
-      <c r="D21" s="36">
+      <c r="D21" s="32">
         <f t="shared" si="0"/>
         <v>4895.6099999999997</v>
       </c>
-      <c r="E21" s="36">
+      <c r="E21" s="32">
         <v>1734599.49</v>
       </c>
-      <c r="F21" s="36">
+      <c r="F21" s="32">
         <f t="shared" si="1"/>
         <v>1734599.49</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="36">
+      <c r="B22" s="32">
         <v>350</v>
       </c>
-      <c r="C22" s="36">
+      <c r="C22" s="32">
         <v>-1085.48</v>
       </c>
-      <c r="D22" s="36">
+      <c r="D22" s="32">
         <f t="shared" si="0"/>
         <v>1085.48</v>
       </c>
-      <c r="E22" s="36">
+      <c r="E22" s="32">
         <v>1884141.96</v>
       </c>
-      <c r="F22" s="36">
+      <c r="F22" s="32">
         <f t="shared" si="1"/>
         <v>1884141.96</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="36">
+      <c r="B23" s="32">
         <v>400</v>
       </c>
-      <c r="C23" s="36">
+      <c r="C23" s="32">
         <v>2728.29</v>
       </c>
-      <c r="D23" s="36">
+      <c r="D23" s="32">
         <f t="shared" si="0"/>
         <v>2728.29</v>
       </c>
-      <c r="E23" s="36">
+      <c r="E23" s="32">
         <v>1843086.94</v>
       </c>
-      <c r="F23" s="36">
+      <c r="F23" s="32">
         <f t="shared" si="1"/>
         <v>1843086.94</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="36">
+      <c r="B24" s="32">
         <v>450</v>
       </c>
-      <c r="C24" s="36">
+      <c r="C24" s="32">
         <v>6545.72</v>
       </c>
-      <c r="D24" s="36">
+      <c r="D24" s="32">
         <f t="shared" si="0"/>
         <v>6545.72</v>
       </c>
-      <c r="E24" s="36">
+      <c r="E24" s="32">
         <v>1611251.78</v>
       </c>
-      <c r="F24" s="36">
+      <c r="F24" s="32">
         <f t="shared" si="1"/>
         <v>1611251.78</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="36">
+      <c r="B25" s="32">
         <v>500</v>
       </c>
-      <c r="C25" s="36">
+      <c r="C25" s="32">
         <v>10265.52</v>
       </c>
-      <c r="D25" s="36">
+      <c r="D25" s="32">
         <f t="shared" si="0"/>
         <v>10265.52</v>
       </c>
-      <c r="E25" s="36">
+      <c r="E25" s="32">
         <v>1189838.1299999999</v>
       </c>
-      <c r="F25" s="36">
+      <c r="F25" s="32">
         <f t="shared" si="1"/>
         <v>1189838.1299999999</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="36">
+      <c r="B26" s="32">
         <v>550</v>
       </c>
-      <c r="C26" s="36">
+      <c r="C26" s="32">
         <v>13512.1</v>
       </c>
-      <c r="D26" s="36">
+      <c r="D26" s="32">
         <f t="shared" si="0"/>
         <v>13512.1</v>
       </c>
-      <c r="E26" s="36">
+      <c r="E26" s="32">
         <v>592593.55000000005</v>
       </c>
-      <c r="F26" s="36">
+      <c r="F26" s="32">
         <f t="shared" si="1"/>
         <v>592593.55000000005</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="36">
+      <c r="B27" s="32">
         <v>600</v>
       </c>
-      <c r="C27" s="36">
+      <c r="C27" s="32">
         <v>16085.34</v>
       </c>
-      <c r="D27" s="36">
+      <c r="D27" s="32">
         <f t="shared" si="0"/>
         <v>16085.34</v>
       </c>
-      <c r="E27" s="36">
+      <c r="E27" s="32">
         <v>-150148.6</v>
       </c>
-      <c r="F27" s="36">
+      <c r="F27" s="32">
         <f t="shared" si="1"/>
         <v>150148.6</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="36">
+      <c r="B28" s="32">
         <v>650</v>
       </c>
-      <c r="C28" s="36">
+      <c r="C28" s="32">
         <v>17985.16</v>
       </c>
-      <c r="D28" s="36">
+      <c r="D28" s="32">
         <f t="shared" si="0"/>
         <v>17985.16</v>
       </c>
-      <c r="E28" s="36">
+      <c r="E28" s="32">
         <v>-1004717.06</v>
       </c>
-      <c r="F28" s="36">
+      <c r="F28" s="32">
         <f t="shared" si="1"/>
         <v>1004717.06</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="36">
+      <c r="B29" s="32">
         <v>700</v>
       </c>
-      <c r="C29" s="36">
+      <c r="C29" s="32">
         <v>19211.54</v>
       </c>
-      <c r="D29" s="36">
+      <c r="D29" s="32">
         <f t="shared" si="0"/>
         <v>19211.54</v>
       </c>
-      <c r="E29" s="36">
+      <c r="E29" s="32">
         <v>-1937440.55</v>
       </c>
-      <c r="F29" s="36">
+      <c r="F29" s="32">
         <f t="shared" si="1"/>
         <v>1937440.55</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="36">
+      <c r="B30" s="32">
         <v>750</v>
       </c>
-      <c r="C30" s="36">
+      <c r="C30" s="32">
         <v>19764.509999999998</v>
       </c>
-      <c r="D30" s="36">
+      <c r="D30" s="32">
         <f t="shared" si="0"/>
         <v>19764.509999999998</v>
       </c>
-      <c r="E30" s="36">
+      <c r="E30" s="32">
         <v>-2914647.79</v>
       </c>
-      <c r="F30" s="36">
+      <c r="F30" s="32">
         <f t="shared" si="1"/>
         <v>2914647.79</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="36">
+      <c r="B31" s="32">
         <v>0</v>
       </c>
-      <c r="C31" s="36">
+      <c r="C31" s="32">
         <v>-18392.66</v>
       </c>
-      <c r="D31" s="36">
+      <c r="D31" s="32">
         <f t="shared" si="0"/>
         <v>18392.66</v>
       </c>
-      <c r="E31" s="36">
+      <c r="E31" s="32">
         <v>-2914647.79</v>
       </c>
-      <c r="F31" s="36">
+      <c r="F31" s="32">
         <f t="shared" si="1"/>
         <v>2914647.79</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="36">
+      <c r="B32" s="32">
         <v>50</v>
       </c>
-      <c r="C32" s="36">
+      <c r="C32" s="32">
         <v>-17847.88</v>
       </c>
-      <c r="D32" s="36">
+      <c r="D32" s="32">
         <f t="shared" si="0"/>
         <v>17847.88</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="32">
         <v>-2005896.43</v>
       </c>
-      <c r="F32" s="36">
+      <c r="F32" s="32">
         <f t="shared" si="1"/>
         <v>2005896.43</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="39" t="s">
+      <c r="A33" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="36">
+      <c r="B33" s="32">
         <v>100</v>
       </c>
-      <c r="C33" s="36">
+      <c r="C33" s="32">
         <v>-16646.05</v>
       </c>
-      <c r="D33" s="36">
+      <c r="D33" s="32">
         <f t="shared" si="0"/>
         <v>16646.05</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="32">
         <v>-1140810.47</v>
       </c>
-      <c r="F33" s="36">
+      <c r="F33" s="32">
         <f t="shared" si="1"/>
         <v>1140810.47</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="36">
+      <c r="B34" s="32">
         <v>150</v>
       </c>
-      <c r="C34" s="36">
+      <c r="C34" s="32">
         <v>-14787.15</v>
       </c>
-      <c r="D34" s="36">
+      <c r="D34" s="32">
         <f t="shared" si="0"/>
         <v>14787.15</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="32">
         <v>-352242.82</v>
       </c>
-      <c r="F34" s="36">
+      <c r="F34" s="32">
         <f t="shared" si="1"/>
         <v>352242.82</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="39" t="s">
+      <c r="A35" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="36">
+      <c r="B35" s="32">
         <v>200</v>
       </c>
-      <c r="C35" s="36">
+      <c r="C35" s="32">
         <v>-12271.2</v>
       </c>
-      <c r="D35" s="36">
+      <c r="D35" s="32">
         <f t="shared" si="0"/>
         <v>12271.2</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="32">
         <v>326953.57</v>
       </c>
-      <c r="F35" s="36">
+      <c r="F35" s="32">
         <f t="shared" si="1"/>
         <v>326953.57</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="36">
+      <c r="B36" s="32">
         <v>250</v>
       </c>
-      <c r="C36" s="36">
+      <c r="C36" s="32">
         <v>-9098.18</v>
       </c>
-      <c r="D36" s="36">
+      <c r="D36" s="32">
         <f t="shared" si="0"/>
         <v>9098.18</v>
       </c>
-      <c r="E36" s="36">
+      <c r="E36" s="32">
         <v>863925.79</v>
       </c>
-      <c r="F36" s="36">
+      <c r="F36" s="32">
         <f t="shared" si="1"/>
         <v>863925.79</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="36">
+      <c r="B37" s="32">
         <v>300</v>
       </c>
-      <c r="C37" s="36">
+      <c r="C37" s="32">
         <v>-5449.93</v>
       </c>
-      <c r="D37" s="36">
+      <c r="D37" s="32">
         <f t="shared" si="0"/>
         <v>5449.93</v>
       </c>
-      <c r="E37" s="36">
+      <c r="E37" s="32">
         <v>1228617.83</v>
       </c>
-      <c r="F37" s="36">
+      <c r="F37" s="32">
         <f t="shared" si="1"/>
         <v>1228617.83</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="39" t="s">
+      <c r="A38" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="36">
+      <c r="B38" s="32">
         <v>350</v>
       </c>
-      <c r="C38" s="36">
+      <c r="C38" s="32">
         <v>-1700.81</v>
       </c>
-      <c r="D38" s="36">
+      <c r="D38" s="32">
         <f t="shared" si="0"/>
         <v>1700.81</v>
       </c>
-      <c r="E38" s="36">
+      <c r="E38" s="32">
         <v>1407587.91</v>
       </c>
-      <c r="F38" s="36">
+      <c r="F38" s="32">
         <f t="shared" si="1"/>
         <v>1407587.91</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="36">
+      <c r="B39" s="32">
         <v>400</v>
       </c>
-      <c r="C39" s="36">
+      <c r="C39" s="32">
         <v>2096.66</v>
       </c>
-      <c r="D39" s="36">
+      <c r="D39" s="32">
         <f t="shared" si="0"/>
         <v>2096.66</v>
       </c>
-      <c r="E39" s="36">
+      <c r="E39" s="32">
         <v>1397893.28</v>
       </c>
-      <c r="F39" s="36">
+      <c r="F39" s="32">
         <f t="shared" si="1"/>
         <v>1397893.28</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="39" t="s">
+      <c r="A40" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="36">
+      <c r="B40" s="32">
         <v>450</v>
       </c>
-      <c r="C40" s="36">
+      <c r="C40" s="32">
         <v>5937.82</v>
       </c>
-      <c r="D40" s="36">
+      <c r="D40" s="32">
         <f t="shared" si="0"/>
         <v>5937.82</v>
       </c>
-      <c r="E40" s="36">
+      <c r="E40" s="32">
         <v>1197128.75</v>
       </c>
-      <c r="F40" s="36">
+      <c r="F40" s="32">
         <f t="shared" si="1"/>
         <v>1197128.75</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B41" s="36">
+      <c r="B41" s="32">
         <v>500</v>
       </c>
-      <c r="C41" s="36">
+      <c r="C41" s="32">
         <v>9591.9699999999993</v>
       </c>
-      <c r="D41" s="36">
+      <c r="D41" s="32">
         <f t="shared" si="0"/>
         <v>9591.9699999999993</v>
       </c>
-      <c r="E41" s="36">
+      <c r="E41" s="32">
         <v>807570.01</v>
       </c>
-      <c r="F41" s="36">
+      <c r="F41" s="32">
         <f t="shared" si="1"/>
         <v>807570.01</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="36">
+      <c r="B42" s="32">
         <v>550</v>
       </c>
-      <c r="C42" s="36">
+      <c r="C42" s="32">
         <v>12760.43</v>
       </c>
-      <c r="D42" s="36">
+      <c r="D42" s="32">
         <f t="shared" si="0"/>
         <v>12760.43</v>
       </c>
-      <c r="E42" s="36">
+      <c r="E42" s="32">
         <v>246026.46</v>
       </c>
-      <c r="F42" s="36">
+      <c r="F42" s="32">
         <f t="shared" si="1"/>
         <v>246026.46</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="36">
+      <c r="B43" s="32">
         <v>600</v>
       </c>
-      <c r="C43" s="36">
+      <c r="C43" s="32">
         <v>15272.84</v>
       </c>
-      <c r="D43" s="36">
+      <c r="D43" s="32">
         <f t="shared" si="0"/>
         <v>15272.84</v>
       </c>
-      <c r="E43" s="36">
+      <c r="E43" s="32">
         <v>-457538.92</v>
       </c>
-      <c r="F43" s="36">
+      <c r="F43" s="32">
         <f t="shared" si="1"/>
         <v>457538.92</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="39" t="s">
+      <c r="A44" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B44" s="36">
+      <c r="B44" s="32">
         <v>650</v>
       </c>
-      <c r="C44" s="36">
+      <c r="C44" s="32">
         <v>17129.21</v>
       </c>
-      <c r="D44" s="36">
+      <c r="D44" s="32">
         <f t="shared" si="0"/>
         <v>17129.21</v>
       </c>
-      <c r="E44" s="36">
+      <c r="E44" s="32">
         <v>-1270323.76</v>
       </c>
-      <c r="F44" s="36">
+      <c r="F44" s="32">
         <f t="shared" si="1"/>
         <v>1270323.76</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="39" t="s">
+      <c r="A45" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="36">
+      <c r="B45" s="32">
         <v>700</v>
       </c>
-      <c r="C45" s="36">
+      <c r="C45" s="32">
         <v>18329.53</v>
       </c>
-      <c r="D45" s="36">
+      <c r="D45" s="32">
         <f t="shared" si="0"/>
         <v>18329.53</v>
       </c>
-      <c r="E45" s="36">
+      <c r="E45" s="32">
         <v>-2159525.75</v>
       </c>
-      <c r="F45" s="36">
+      <c r="F45" s="32">
         <f t="shared" si="1"/>
         <v>2159525.75</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="39" t="s">
+      <c r="A46" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B46" s="36">
+      <c r="B46" s="32">
         <v>750</v>
       </c>
-      <c r="C46" s="36">
+      <c r="C46" s="32">
         <v>18873.8</v>
       </c>
-      <c r="D46" s="36">
+      <c r="D46" s="32">
         <f t="shared" si="0"/>
         <v>18873.8</v>
       </c>
-      <c r="E46" s="36">
+      <c r="E46" s="32">
         <v>-3092342.54</v>
       </c>
-      <c r="F46" s="36">
+      <c r="F46" s="32">
         <f t="shared" si="1"/>
         <v>3092342.54</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="39" t="s">
+      <c r="A47" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B47" s="36">
+      <c r="B47" s="32">
         <v>0</v>
       </c>
-      <c r="C47" s="36">
+      <c r="C47" s="32">
         <v>-20219.28</v>
       </c>
-      <c r="D47" s="36">
+      <c r="D47" s="32">
         <f t="shared" si="0"/>
         <v>20219.28</v>
       </c>
-      <c r="E47" s="36">
+      <c r="E47" s="32">
         <v>-3092342.54</v>
       </c>
-      <c r="F47" s="36">
+      <c r="F47" s="32">
         <f t="shared" si="1"/>
         <v>3092342.54</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="39" t="s">
+      <c r="A48" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B48" s="36">
+      <c r="B48" s="32">
         <v>50</v>
       </c>
-      <c r="C48" s="36">
+      <c r="C48" s="32">
         <v>-19750.099999999999</v>
       </c>
-      <c r="D48" s="36">
+      <c r="D48" s="32">
         <f t="shared" si="0"/>
         <v>19750.099999999999</v>
       </c>
-      <c r="E48" s="36">
+      <c r="E48" s="32">
         <v>-2091000.44</v>
       </c>
-      <c r="F48" s="36">
+      <c r="F48" s="32">
         <f t="shared" si="1"/>
         <v>2091000.44</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="39" t="s">
+      <c r="A49" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B49" s="36">
+      <c r="B49" s="32">
         <v>100</v>
       </c>
-      <c r="C49" s="36">
+      <c r="C49" s="32">
         <v>-18775.05</v>
       </c>
-      <c r="D49" s="36">
+      <c r="D49" s="32">
         <f t="shared" si="0"/>
         <v>18775.05</v>
       </c>
-      <c r="E49" s="36">
+      <c r="E49" s="32">
         <v>-1125764.1200000001</v>
       </c>
-      <c r="F49" s="36">
+      <c r="F49" s="32">
         <f t="shared" si="1"/>
         <v>1125764.1200000001</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="39" t="s">
+      <c r="A50" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B50" s="36">
+      <c r="B50" s="32">
         <v>150</v>
       </c>
-      <c r="C50" s="36">
+      <c r="C50" s="32">
         <v>-17294.13</v>
       </c>
-      <c r="D50" s="36">
+      <c r="D50" s="32">
         <f t="shared" si="0"/>
         <v>17294.13</v>
       </c>
-      <c r="E50" s="36">
+      <c r="E50" s="32">
         <v>-221926.9</v>
       </c>
-      <c r="F50" s="36">
+      <c r="F50" s="32">
         <f t="shared" si="1"/>
         <v>221926.9</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="39" t="s">
+      <c r="A51" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B51" s="36">
+      <c r="B51" s="32">
         <v>200</v>
       </c>
-      <c r="C51" s="36">
+      <c r="C51" s="32">
         <v>-15307.35</v>
       </c>
-      <c r="D51" s="36">
+      <c r="D51" s="32">
         <f t="shared" si="0"/>
         <v>15307.35</v>
       </c>
-      <c r="E51" s="36">
+      <c r="E51" s="32">
         <v>595217.92000000004</v>
       </c>
-      <c r="F51" s="36">
+      <c r="F51" s="32">
         <f t="shared" si="1"/>
         <v>595217.92000000004</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="39" t="s">
+      <c r="A52" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B52" s="36">
+      <c r="B52" s="32">
         <v>250</v>
       </c>
-      <c r="C52" s="36">
+      <c r="C52" s="32">
         <v>-12814.7</v>
       </c>
-      <c r="D52" s="36">
+      <c r="D52" s="32">
         <f t="shared" si="0"/>
         <v>12814.7</v>
       </c>
-      <c r="E52" s="36">
+      <c r="E52" s="32">
         <v>1300377</v>
       </c>
-      <c r="F52" s="36">
+      <c r="F52" s="32">
         <f t="shared" si="1"/>
         <v>1300377</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="39" t="s">
+      <c r="A53" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B53" s="36">
+      <c r="B53" s="32">
         <v>300</v>
       </c>
-      <c r="C53" s="36">
+      <c r="C53" s="32">
         <v>-8339.69</v>
       </c>
-      <c r="D53" s="36">
+      <c r="D53" s="32">
         <f t="shared" si="0"/>
         <v>8339.69</v>
       </c>
-      <c r="E53" s="36">
+      <c r="E53" s="32">
         <v>1831455.76</v>
       </c>
-      <c r="F53" s="36">
+      <c r="F53" s="32">
         <f t="shared" si="1"/>
         <v>1831455.76</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="39" t="s">
+      <c r="A54" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B54" s="36">
+      <c r="B54" s="32">
         <v>350</v>
       </c>
-      <c r="C54" s="36">
+      <c r="C54" s="32">
         <v>-3765.03</v>
       </c>
-      <c r="D54" s="36">
+      <c r="D54" s="32">
         <f t="shared" si="0"/>
         <v>3765.03</v>
       </c>
-      <c r="E54" s="36">
+      <c r="E54" s="32">
         <v>2134059.37</v>
       </c>
-      <c r="F54" s="36">
+      <c r="F54" s="32">
         <f t="shared" si="1"/>
         <v>2134059.37</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="39" t="s">
+      <c r="A55" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B55" s="36">
+      <c r="B55" s="32">
         <v>400</v>
       </c>
-      <c r="C55" s="36">
+      <c r="C55" s="32">
         <v>806.19</v>
       </c>
-      <c r="D55" s="36">
+      <c r="D55" s="32">
         <f t="shared" si="0"/>
         <v>806.19</v>
       </c>
-      <c r="E55" s="36">
+      <c r="E55" s="32">
         <v>2208015.88</v>
       </c>
-      <c r="F55" s="36">
+      <c r="F55" s="32">
         <f t="shared" si="1"/>
         <v>2208015.88</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="39" t="s">
+      <c r="A56" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B56" s="36">
+      <c r="B56" s="32">
         <v>450</v>
       </c>
-      <c r="C56" s="36">
+      <c r="C56" s="32">
         <v>5373.97</v>
       </c>
-      <c r="D56" s="36">
+      <c r="D56" s="32">
         <f t="shared" si="0"/>
         <v>5373.97</v>
       </c>
-      <c r="E56" s="36">
+      <c r="E56" s="32">
         <v>2053497.33</v>
       </c>
-      <c r="F56" s="36">
+      <c r="F56" s="32">
         <f t="shared" si="1"/>
         <v>2053497.33</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="39" t="s">
+      <c r="A57" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B57" s="36">
+      <c r="B57" s="32">
         <v>500</v>
       </c>
-      <c r="C57" s="36">
+      <c r="C57" s="32">
         <v>9872.67</v>
       </c>
-      <c r="D57" s="36">
+      <c r="D57" s="32">
         <f t="shared" si="0"/>
         <v>9872.67</v>
       </c>
-      <c r="E57" s="36">
+      <c r="E57" s="32">
         <v>1670741.37</v>
       </c>
-      <c r="F57" s="36">
+      <c r="F57" s="32">
         <f t="shared" si="1"/>
         <v>1670741.37</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="39" t="s">
+      <c r="A58" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B58" s="36">
+      <c r="B58" s="32">
         <v>550</v>
       </c>
-      <c r="C58" s="36">
+      <c r="C58" s="32">
         <v>12706.97</v>
       </c>
-      <c r="D58" s="36">
+      <c r="D58" s="32">
         <f t="shared" si="0"/>
         <v>12706.97</v>
       </c>
-      <c r="E58" s="36">
+      <c r="E58" s="32">
         <v>1105550.75</v>
       </c>
-      <c r="F58" s="36">
+      <c r="F58" s="32">
         <f t="shared" si="1"/>
         <v>1105550.75</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="39" t="s">
+      <c r="A59" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B59" s="36">
+      <c r="B59" s="32">
         <v>600</v>
       </c>
-      <c r="C59" s="36">
+      <c r="C59" s="32">
         <v>15373.4</v>
       </c>
-      <c r="D59" s="36">
+      <c r="D59" s="32">
         <f t="shared" si="0"/>
         <v>15373.4</v>
       </c>
-      <c r="E59" s="36">
+      <c r="E59" s="32">
         <v>402841.96</v>
       </c>
-      <c r="F59" s="36">
+      <c r="F59" s="32">
         <f t="shared" si="1"/>
         <v>402841.96</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="39" t="s">
+      <c r="A60" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B60" s="36">
+      <c r="B60" s="32">
         <v>650</v>
       </c>
-      <c r="C60" s="36">
+      <c r="C60" s="32">
         <v>17871.939999999999</v>
       </c>
-      <c r="D60" s="36">
+      <c r="D60" s="32">
         <f t="shared" si="0"/>
         <v>17871.939999999999</v>
       </c>
-      <c r="E60" s="36">
+      <c r="E60" s="32">
         <v>-428991.08</v>
       </c>
-      <c r="F60" s="36">
+      <c r="F60" s="32">
         <f t="shared" si="1"/>
         <v>428991.08</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="39" t="s">
+      <c r="A61" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B61" s="36">
+      <c r="B61" s="32">
         <v>700</v>
       </c>
-      <c r="C61" s="36">
+      <c r="C61" s="32">
         <v>20202.61</v>
       </c>
-      <c r="D61" s="36">
+      <c r="D61" s="32">
         <f t="shared" si="0"/>
         <v>20202.61</v>
       </c>
-      <c r="E61" s="36">
+      <c r="E61" s="32">
         <v>-1381554.44</v>
       </c>
-      <c r="F61" s="36">
+      <c r="F61" s="32">
         <f t="shared" si="1"/>
         <v>1381554.44</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="39" t="s">
+      <c r="A62" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B62" s="36">
+      <c r="B62" s="32">
         <v>750</v>
       </c>
-      <c r="C62" s="36">
+      <c r="C62" s="32">
         <v>22365.4</v>
       </c>
-      <c r="D62" s="36">
+      <c r="D62" s="32">
         <f t="shared" si="0"/>
         <v>22365.4</v>
       </c>
-      <c r="E62" s="36">
+      <c r="E62" s="32">
         <v>-2446454.19</v>
       </c>
-      <c r="F62" s="36">
+      <c r="F62" s="32">
         <f t="shared" si="1"/>
         <v>2446454.19</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="39" t="s">
+      <c r="A63" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B63" s="36">
+      <c r="B63" s="32">
         <v>0</v>
       </c>
-      <c r="C63" s="36">
+      <c r="C63" s="32">
         <v>-14560.05</v>
       </c>
-      <c r="D63" s="36">
+      <c r="D63" s="32">
         <f t="shared" si="0"/>
         <v>14560.05</v>
       </c>
-      <c r="E63" s="36">
+      <c r="E63" s="32">
         <v>-2446454.19</v>
       </c>
-      <c r="F63" s="36">
+      <c r="F63" s="32">
         <f t="shared" si="1"/>
         <v>2446454.19</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="39" t="s">
+      <c r="A64" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="36">
+      <c r="B64" s="32">
         <v>48.555999999999997</v>
       </c>
-      <c r="C64" s="36">
+      <c r="C64" s="32">
         <v>-13900.95</v>
       </c>
-      <c r="D64" s="36">
+      <c r="D64" s="32">
         <f t="shared" si="0"/>
         <v>13900.95</v>
       </c>
-      <c r="E64" s="36">
+      <c r="E64" s="32">
         <v>-1751849.93</v>
       </c>
-      <c r="F64" s="36">
+      <c r="F64" s="32">
         <f t="shared" si="1"/>
         <v>1751849.93</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="39" t="s">
+      <c r="A65" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B65" s="36">
+      <c r="B65" s="32">
         <v>97.111000000000004</v>
       </c>
-      <c r="C65" s="36">
+      <c r="C65" s="32">
         <v>-12343.67</v>
       </c>
-      <c r="D65" s="36">
+      <c r="D65" s="32">
         <f t="shared" si="0"/>
         <v>12343.67</v>
       </c>
-      <c r="E65" s="36">
+      <c r="E65" s="32">
         <v>-1111054.42</v>
       </c>
-      <c r="F65" s="36">
+      <c r="F65" s="32">
         <f t="shared" si="1"/>
         <v>1111054.42</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="39" t="s">
+      <c r="A66" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B66" s="36">
+      <c r="B66" s="32">
         <v>145.667</v>
       </c>
-      <c r="C66" s="36">
+      <c r="C66" s="32">
         <v>-9888.2000000000007</v>
       </c>
-      <c r="D66" s="36">
+      <c r="D66" s="32">
         <f t="shared" si="0"/>
         <v>9888.2000000000007</v>
       </c>
-      <c r="E66" s="36">
+      <c r="E66" s="32">
         <v>-567679.65</v>
       </c>
-      <c r="F66" s="36">
+      <c r="F66" s="32">
         <f t="shared" si="1"/>
         <v>567679.65</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="39" t="s">
+      <c r="A67" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B67" s="36">
+      <c r="B67" s="32">
         <v>194.22200000000001</v>
       </c>
-      <c r="C67" s="36">
+      <c r="C67" s="32">
         <v>-6790.74</v>
       </c>
-      <c r="D67" s="36">
+      <c r="D67" s="32">
         <f t="shared" si="0"/>
         <v>6790.74</v>
       </c>
-      <c r="E67" s="36">
+      <c r="E67" s="32">
         <v>-161475.72</v>
       </c>
-      <c r="F67" s="36">
+      <c r="F67" s="32">
         <f t="shared" si="1"/>
         <v>161475.72</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="39" t="s">
+      <c r="A68" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B68" s="36">
+      <c r="B68" s="32">
         <v>242.77799999999999</v>
       </c>
-      <c r="C68" s="36">
+      <c r="C68" s="32">
         <v>-3452.53</v>
       </c>
-      <c r="D68" s="36">
+      <c r="D68" s="32">
         <f t="shared" si="0"/>
         <v>3452.53</v>
       </c>
-      <c r="E68" s="36">
+      <c r="E68" s="32">
         <v>87315.47</v>
       </c>
-      <c r="F68" s="36">
+      <c r="F68" s="32">
         <f t="shared" si="1"/>
         <v>87315.47</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="39" t="s">
+      <c r="A69" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B69" s="36">
+      <c r="B69" s="32">
         <v>291.33300000000003</v>
       </c>
-      <c r="C69" s="36">
+      <c r="C69" s="32">
         <v>-338.8</v>
       </c>
-      <c r="D69" s="36">
+      <c r="D69" s="32">
         <f t="shared" ref="D69:D80" si="2">ABS(C69)</f>
         <v>338.8</v>
       </c>
-      <c r="E69" s="36">
+      <c r="E69" s="32">
         <v>178099.25</v>
       </c>
-      <c r="F69" s="36">
+      <c r="F69" s="32">
         <f t="shared" ref="F69:F80" si="3">ABS(E69)</f>
         <v>178099.25</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="39" t="s">
+      <c r="A70" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B70" s="36">
+      <c r="B70" s="32">
         <v>339.88900000000001</v>
       </c>
-      <c r="C70" s="36">
+      <c r="C70" s="32">
         <v>2463.1999999999998</v>
       </c>
-      <c r="D70" s="36">
+      <c r="D70" s="32">
         <f t="shared" si="2"/>
         <v>2463.1999999999998</v>
       </c>
-      <c r="E70" s="36">
+      <c r="E70" s="32">
         <v>125262.08</v>
       </c>
-      <c r="F70" s="36">
+      <c r="F70" s="32">
         <f t="shared" si="3"/>
         <v>125262.08</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="39" t="s">
+      <c r="A71" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B71" s="36">
+      <c r="B71" s="32">
         <v>388.44400000000002</v>
       </c>
-      <c r="C71" s="36">
+      <c r="C71" s="32">
         <v>4953.4799999999996</v>
       </c>
-      <c r="D71" s="36">
+      <c r="D71" s="32">
         <f t="shared" si="2"/>
         <v>4953.4799999999996</v>
       </c>
-      <c r="E71" s="36">
+      <c r="E71" s="32">
         <v>-56059.82</v>
       </c>
-      <c r="F71" s="36">
+      <c r="F71" s="32">
         <f t="shared" si="3"/>
         <v>56059.82</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="39" t="s">
+      <c r="A72" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B72" s="36">
+      <c r="B72" s="32">
         <v>437</v>
       </c>
-      <c r="C72" s="36">
+      <c r="C72" s="32">
         <v>7132.02</v>
       </c>
-      <c r="D72" s="36">
+      <c r="D72" s="32">
         <f t="shared" si="2"/>
         <v>7132.02</v>
       </c>
-      <c r="E72" s="36">
+      <c r="E72" s="32">
         <v>-350730.22</v>
       </c>
-      <c r="F72" s="36">
+      <c r="F72" s="32">
         <f t="shared" si="3"/>
         <v>350730.22</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="39" t="s">
+      <c r="A73" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B73" s="36">
+      <c r="B73" s="32">
         <v>0</v>
       </c>
-      <c r="C73" s="36">
+      <c r="C73" s="32">
         <v>-6811.32</v>
       </c>
-      <c r="D73" s="36">
+      <c r="D73" s="32">
         <f t="shared" si="2"/>
         <v>6811.32</v>
       </c>
-      <c r="E73" s="36">
+      <c r="E73" s="32">
         <v>-350730.22</v>
       </c>
-      <c r="F73" s="36">
+      <c r="F73" s="32">
         <f t="shared" si="3"/>
         <v>350730.22</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="39" t="s">
+      <c r="A74" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B74" s="36">
+      <c r="B74" s="32">
         <v>49</v>
       </c>
-      <c r="C74" s="36">
+      <c r="C74" s="32">
         <v>-6195.54</v>
       </c>
-      <c r="D74" s="36">
+      <c r="D74" s="32">
         <f t="shared" si="2"/>
         <v>6195.54</v>
       </c>
-      <c r="E74" s="36">
+      <c r="E74" s="32">
         <v>-28763.79</v>
       </c>
-      <c r="F74" s="36">
+      <c r="F74" s="32">
         <f t="shared" si="3"/>
         <v>28763.79</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="39" t="s">
+      <c r="A75" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B75" s="36">
+      <c r="B75" s="32">
         <v>98</v>
       </c>
-      <c r="C75" s="36">
+      <c r="C75" s="32">
         <v>-4772.05</v>
       </c>
-      <c r="D75" s="36">
+      <c r="D75" s="32">
         <f t="shared" si="2"/>
         <v>4772.05</v>
       </c>
-      <c r="E75" s="36">
+      <c r="E75" s="32">
         <v>243240.48</v>
       </c>
-      <c r="F75" s="36">
+      <c r="F75" s="32">
         <f t="shared" si="3"/>
         <v>243240.48</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="39" t="s">
+      <c r="A76" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B76" s="36">
+      <c r="B76" s="32">
         <v>147</v>
       </c>
-      <c r="C76" s="36">
+      <c r="C76" s="32">
         <v>-2540.85</v>
       </c>
-      <c r="D76" s="36">
+      <c r="D76" s="32">
         <f t="shared" si="2"/>
         <v>2540.85</v>
       </c>
-      <c r="E76" s="36">
+      <c r="E76" s="32">
         <v>425704.73</v>
       </c>
-      <c r="F76" s="36">
+      <c r="F76" s="32">
         <f t="shared" si="3"/>
         <v>425704.73</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="39" t="s">
+      <c r="A77" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B77" s="36">
+      <c r="B77" s="32">
         <v>196</v>
       </c>
-      <c r="C77" s="36">
+      <c r="C77" s="32">
         <v>369.52</v>
       </c>
-      <c r="D77" s="36">
+      <c r="D77" s="32">
         <f t="shared" si="2"/>
         <v>369.52</v>
       </c>
-      <c r="E77" s="36">
+      <c r="E77" s="32">
         <v>479878.86</v>
       </c>
-      <c r="F77" s="36">
+      <c r="F77" s="32">
         <f t="shared" si="3"/>
         <v>479878.86</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="39" t="s">
+      <c r="A78" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B78" s="36">
+      <c r="B78" s="32">
         <v>245</v>
       </c>
-      <c r="C78" s="36">
+      <c r="C78" s="32">
         <v>2729.01</v>
       </c>
-      <c r="D78" s="36">
+      <c r="D78" s="32">
         <f t="shared" si="2"/>
         <v>2729.01</v>
       </c>
-      <c r="E78" s="36">
+      <c r="E78" s="32">
         <v>400457.34</v>
       </c>
-      <c r="F78" s="36">
+      <c r="F78" s="32">
         <f t="shared" si="3"/>
         <v>400457.34</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="39" t="s">
+      <c r="A79" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B79" s="36">
+      <c r="B79" s="32">
         <v>294</v>
       </c>
-      <c r="C79" s="36">
+      <c r="C79" s="32">
         <v>4229.47</v>
       </c>
-      <c r="D79" s="36">
+      <c r="D79" s="32">
         <f t="shared" si="2"/>
         <v>4229.47</v>
       </c>
-      <c r="E79" s="36">
+      <c r="E79" s="32">
         <v>226466.96</v>
       </c>
-      <c r="F79" s="36">
+      <c r="F79" s="32">
         <f t="shared" si="3"/>
         <v>226466.96</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="39" t="s">
+      <c r="A80" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B80" s="36">
+      <c r="B80" s="32">
         <v>343</v>
       </c>
-      <c r="C80" s="36">
+      <c r="C80" s="32">
         <v>4870.91</v>
       </c>
-      <c r="D80" s="36">
+      <c r="D80" s="32">
         <f t="shared" si="2"/>
         <v>4870.91</v>
       </c>
-      <c r="E80" s="36">
+      <c r="E80" s="32">
         <v>-9.8879999999999999E-11</v>
       </c>
-      <c r="F80" s="36">
+      <c r="F80" s="32">
         <f t="shared" si="3"/>
         <v>9.8879999999999999E-11</v>
       </c>

</xml_diff>

<commit_message>
Acomodo tablas para informe
</commit_message>
<xml_diff>
--- a/Tarea 06/Vigas.xlsx
+++ b/Tarea 06/Vigas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ramos Ingenieria\12° Semestre\Proyecto de Hormigón Armado\Tarea 06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED35D8F4-B2C6-4BD1-B18D-E88096EC4BF0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA456E69-7238-4B11-B70A-EAB6CD42A421}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{B94BBB90-C174-4AC8-BDFB-4A9825C26EEC}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="75">
   <si>
     <t>0101</t>
   </si>
@@ -233,6 +233,27 @@
   </si>
   <si>
     <t>$A_{s.min} [cm^2]$</t>
+  </si>
+  <si>
+    <t>Flexión</t>
+  </si>
+  <si>
+    <t>Corte</t>
+  </si>
+  <si>
+    <t>Viga C</t>
+  </si>
+  <si>
+    <t>Viga K</t>
+  </si>
+  <si>
+    <t>$A_{req} [cm^2]$</t>
+  </si>
+  <si>
+    <t>$\phi \cdot Vn [tonf]$</t>
+  </si>
+  <si>
+    <t>$\phi Mn [tonf \cdot m]$</t>
   </si>
 </sst>
 </file>
@@ -616,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -828,6 +849,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -869,7 +902,7 @@
       <sheetName val="Deformaciones"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
         <row r="7">
           <cell r="L7">
@@ -965,37 +998,6 @@
             <v>0129</v>
           </cell>
         </row>
-        <row r="47">
-          <cell r="C47"/>
-          <cell r="D47"/>
-          <cell r="E47"/>
-          <cell r="F47"/>
-          <cell r="G47"/>
-          <cell r="H47"/>
-          <cell r="I47"/>
-          <cell r="J47"/>
-          <cell r="K47"/>
-          <cell r="L47"/>
-          <cell r="M47"/>
-          <cell r="N47"/>
-          <cell r="O47"/>
-          <cell r="P47"/>
-          <cell r="Q47"/>
-          <cell r="R47"/>
-          <cell r="S47"/>
-          <cell r="T47"/>
-          <cell r="U47"/>
-          <cell r="V47"/>
-          <cell r="W47"/>
-          <cell r="X47"/>
-          <cell r="Y47"/>
-          <cell r="Z47"/>
-          <cell r="AA47"/>
-          <cell r="AB47"/>
-          <cell r="AC47"/>
-          <cell r="AD47"/>
-          <cell r="AE47"/>
-        </row>
         <row r="48">
           <cell r="C48">
             <v>5</v>
@@ -1352,37 +1354,6 @@
             <v>6</v>
           </cell>
         </row>
-        <row r="52">
-          <cell r="C52"/>
-          <cell r="D52"/>
-          <cell r="E52"/>
-          <cell r="F52"/>
-          <cell r="G52"/>
-          <cell r="H52"/>
-          <cell r="I52"/>
-          <cell r="J52"/>
-          <cell r="K52"/>
-          <cell r="L52"/>
-          <cell r="M52"/>
-          <cell r="N52"/>
-          <cell r="O52"/>
-          <cell r="P52"/>
-          <cell r="Q52"/>
-          <cell r="R52"/>
-          <cell r="S52"/>
-          <cell r="T52"/>
-          <cell r="U52"/>
-          <cell r="V52"/>
-          <cell r="W52"/>
-          <cell r="X52"/>
-          <cell r="Y52"/>
-          <cell r="Z52"/>
-          <cell r="AA52"/>
-          <cell r="AB52"/>
-          <cell r="AC52"/>
-          <cell r="AD52"/>
-          <cell r="AE52"/>
-        </row>
         <row r="53">
           <cell r="C53">
             <v>1.1000000000000001</v>
@@ -2273,37 +2244,6 @@
             <v>1.39</v>
           </cell>
         </row>
-        <row r="63">
-          <cell r="C63"/>
-          <cell r="D63"/>
-          <cell r="E63"/>
-          <cell r="F63"/>
-          <cell r="G63"/>
-          <cell r="H63"/>
-          <cell r="I63"/>
-          <cell r="J63"/>
-          <cell r="K63"/>
-          <cell r="L63"/>
-          <cell r="M63"/>
-          <cell r="N63"/>
-          <cell r="O63"/>
-          <cell r="P63"/>
-          <cell r="Q63"/>
-          <cell r="R63"/>
-          <cell r="S63"/>
-          <cell r="T63"/>
-          <cell r="U63"/>
-          <cell r="V63"/>
-          <cell r="W63"/>
-          <cell r="X63"/>
-          <cell r="Y63"/>
-          <cell r="Z63"/>
-          <cell r="AA63"/>
-          <cell r="AB63"/>
-          <cell r="AC63"/>
-          <cell r="AD63"/>
-          <cell r="AE63"/>
-        </row>
         <row r="64">
           <cell r="C64">
             <v>500</v>
@@ -2842,7 +2782,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
       <sheetData sheetId="3">
         <row r="64">
           <cell r="B64" t="str">
@@ -2850,18 +2790,18 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3166,8 +3106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F51FF3-724F-45F5-8F3F-FC55661E6BD0}">
   <dimension ref="B2:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" topLeftCell="J31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M47" sqref="M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -3919,7 +3859,7 @@
       <c r="N32" s="48"/>
       <c r="O32" s="51"/>
     </row>
-    <row r="33" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="28"/>
       <c r="G33" s="1"/>
       <c r="H33" s="43"/>
@@ -3939,9 +3879,11 @@
         <v>39</v>
       </c>
       <c r="I34" s="57"/>
-      <c r="K34" s="51"/>
-      <c r="L34" s="48"/>
-      <c r="M34" s="48"/>
+      <c r="K34" s="78" t="s">
+        <v>68</v>
+      </c>
+      <c r="L34" s="78"/>
+      <c r="M34" s="78"/>
       <c r="N34" s="48"/>
       <c r="O34" s="48"/>
     </row>
@@ -3963,14 +3905,12 @@
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="52" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="I35" s="52">
         <v>4.5599999999999996</v>
       </c>
-      <c r="K35" s="73" t="s">
-        <v>67</v>
-      </c>
+      <c r="K35" s="73"/>
       <c r="L35" s="73" t="s">
         <v>53</v>
       </c>
@@ -3978,28 +3918,26 @@
         <v>54</v>
       </c>
       <c r="N35" s="73" t="s">
-        <v>55</v>
-      </c>
-      <c r="O35" s="74" t="s">
-        <v>56</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="O35" s="70"/>
     </row>
     <row r="36" spans="2:15" ht="15" x14ac:dyDescent="0.25">
       <c r="B36" s="44" t="s">
         <v>50</v>
       </c>
       <c r="C36" s="44">
-        <v>11.33</v>
+        <v>1.4</v>
       </c>
       <c r="D36" s="44">
-        <v>0.53</v>
+        <v>-0.2</v>
       </c>
       <c r="E36" s="45">
         <v>14.436199999999999</v>
       </c>
       <c r="F36" s="49">
         <f>C36*1.2+D36*1+E36*1.4</f>
-        <v>34.336679999999994</v>
+        <v>21.690679999999997</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="42" t="s">
@@ -4008,38 +3946,34 @@
       <c r="I36" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="K36" s="71">
-        <v>4.5599999999999996</v>
-      </c>
+      <c r="K36" s="71"/>
       <c r="L36" s="14" t="s">
         <v>63</v>
       </c>
       <c r="M36" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="N36" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="O36" s="14" t="s">
-        <v>48</v>
-      </c>
+      <c r="N36" s="14">
+        <v>33.42</v>
+      </c>
+      <c r="O36" s="48"/>
     </row>
     <row r="37" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="41" t="s">
         <v>51</v>
       </c>
       <c r="C37" s="41">
-        <v>5.2</v>
+        <v>3.26</v>
       </c>
       <c r="D37" s="41">
-        <v>0.312</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="E37" s="46">
         <v>18.1998</v>
       </c>
       <c r="F37" s="50">
         <f>C37*1.2+D37*1+E37*1.4</f>
-        <v>32.03172</v>
+        <v>29.570719999999994</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="48" t="s">
@@ -4049,7 +3983,7 @@
         <v>63</v>
       </c>
       <c r="L37" s="2"/>
-      <c r="O37" s="1"/>
+      <c r="O37" s="73"/>
     </row>
     <row r="38" spans="2:15" ht="15" x14ac:dyDescent="0.25">
       <c r="C38" s="68"/>
@@ -4063,7 +3997,12 @@
         <v>41</v>
       </c>
       <c r="L38" s="2"/>
-      <c r="O38" s="1"/>
+      <c r="N38" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="O38" s="73" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="39" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="44"/>
@@ -4074,13 +4013,19 @@
       <c r="I39" s="55" t="s">
         <v>48</v>
       </c>
+      <c r="N39" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="O39" s="14">
+        <v>45.09</v>
+      </c>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C40" s="44"/>
       <c r="H40" s="43"/>
       <c r="I40" s="43"/>
     </row>
-    <row r="41" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="44"/>
       <c r="F41" s="1">
         <v>1.4098999999999999</v>
@@ -4111,20 +4056,38 @@
         <f>F42*1.2+G42*1+H42*1.4</f>
         <v>29.581519999999998</v>
       </c>
-    </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K42" s="75" t="s">
+        <v>67</v>
+      </c>
+      <c r="L42" s="75"/>
+    </row>
+    <row r="43" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="44"/>
       <c r="F43" s="56"/>
       <c r="G43" s="56"/>
       <c r="H43" s="43"/>
       <c r="I43" s="43"/>
+      <c r="K43" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="L43" s="42" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H44" s="43"/>
       <c r="I44" s="43"/>
-      <c r="J44" s="28"/>
-    </row>
-    <row r="45" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="J44" s="76" t="s">
+        <v>70</v>
+      </c>
+      <c r="K44" s="52">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="L44" s="42">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="54" t="s">
         <v>42</v>
       </c>
@@ -4137,6 +4100,15 @@
       <c r="G45" s="1"/>
       <c r="H45" s="43"/>
       <c r="I45" s="43"/>
+      <c r="J45" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="K45" s="77">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="L45" s="55">
+        <v>1.58</v>
+      </c>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="G46" s="1"/>
@@ -4176,15 +4148,27 @@
       <c r="H49" s="43"/>
       <c r="I49" s="43"/>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:15" ht="15" x14ac:dyDescent="0.25">
       <c r="G50" s="1"/>
       <c r="H50" s="43"/>
       <c r="I50" s="43"/>
+      <c r="N50" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="O50" s="73" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="51" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G51" s="31"/>
       <c r="H51" s="43"/>
       <c r="I51" s="43"/>
+      <c r="N51" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="O51" s="14">
+        <v>45.09</v>
+      </c>
     </row>
     <row r="52" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="47" t="s">
@@ -4242,7 +4226,7 @@
         <v>54</v>
       </c>
       <c r="N53" s="73" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="O53" s="74" t="s">
         <v>56</v>
@@ -4276,13 +4260,13 @@
         <v>4.5599999999999996</v>
       </c>
       <c r="L54" s="14" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="M54" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="N54" s="14" t="s">
-        <v>41</v>
+      <c r="N54" s="14">
+        <v>40.1</v>
       </c>
       <c r="O54" s="14" t="s">
         <v>48</v>
@@ -4316,7 +4300,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="24">
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="K34:M34"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="J7:J8"/>

</xml_diff>

<commit_message>
Cambios chicos para acomodar tablas
</commit_message>
<xml_diff>
--- a/Tarea 06/Vigas.xlsx
+++ b/Tarea 06/Vigas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ramos Ingenieria\12° Semestre\Proyecto de Hormigón Armado\Tarea 06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA456E69-7238-4B11-B70A-EAB6CD42A421}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16725AF5-0FAD-4322-BF84-360E6E927CC3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{B94BBB90-C174-4AC8-BDFB-4A9825C26EEC}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="79">
   <si>
     <t>0101</t>
   </si>
@@ -254,6 +254,18 @@
   </si>
   <si>
     <t>$\phi Mn [tonf \cdot m]$</t>
+  </si>
+  <si>
+    <t>Viga estática</t>
+  </si>
+  <si>
+    <t>$A'_{req} [cm^2]$</t>
+  </si>
+  <si>
+    <t>$\rho_{req}$</t>
+  </si>
+  <si>
+    <t>$\rho_{min}$</t>
   </si>
 </sst>
 </file>
@@ -637,7 +649,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -854,6 +866,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -861,6 +876,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3106,8 +3124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F51FF3-724F-45F5-8F3F-FC55661E6BD0}">
   <dimension ref="B2:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M47" sqref="M47"/>
+    <sheetView tabSelected="1" topLeftCell="C31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43:M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -3613,7 +3631,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="29" t="s">
         <v>12</v>
       </c>
@@ -3623,7 +3641,6 @@
       </c>
     </row>
     <row r="17" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F17" s="43"/>
       <c r="G17" s="1"/>
       <c r="H17" s="57" t="s">
         <v>39</v>
@@ -3633,9 +3650,6 @@
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="47" t="s">
-        <v>52</v>
-      </c>
       <c r="C18" s="47" t="s">
         <v>19</v>
       </c>
@@ -3643,48 +3657,39 @@
         <v>20</v>
       </c>
       <c r="E18" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="70"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="I18" s="52">
-        <f>1.53</f>
-        <v>1.53</v>
-      </c>
       <c r="K18" s="73" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="L18" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="M18" s="74" t="s">
-        <v>54</v>
-      </c>
-      <c r="N18" s="74" t="s">
+      <c r="O18" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="O18" s="74" t="s">
+      <c r="P18" s="74" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="58" t="s">
-        <v>50</v>
-      </c>
       <c r="C19" s="1">
         <v>7.7839999999999998</v>
       </c>
       <c r="D19" s="1">
         <v>7.96</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E19" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="28">
         <f>C19*1.2+D19*1.6</f>
         <v>22.076799999999999</v>
       </c>
-      <c r="F19" s="28"/>
       <c r="G19" s="53"/>
       <c r="H19" s="42" t="s">
         <v>53</v>
@@ -3693,35 +3698,30 @@
         <v>63</v>
       </c>
       <c r="K19" s="71">
-        <f>1.53</f>
-        <v>1.53</v>
+        <v>13.65</v>
       </c>
       <c r="L19" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="M19" s="71" t="s">
-        <v>62</v>
-      </c>
-      <c r="N19" s="71" t="s">
+      <c r="O19" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="O19" s="14" t="s">
+      <c r="P19" s="14" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" s="59"/>
       <c r="C20" s="44">
         <v>-11.079000000000001</v>
       </c>
       <c r="D20" s="44">
         <v>-11.016999999999999</v>
       </c>
-      <c r="E20" s="49">
+      <c r="E20" s="59"/>
+      <c r="F20" s="49">
         <f>C20*1.2+D20*1.6</f>
         <v>-30.921999999999997</v>
       </c>
-      <c r="F20" s="49"/>
       <c r="G20" s="53"/>
       <c r="H20" s="48" t="s">
         <v>54</v>
@@ -3733,20 +3733,19 @@
       <c r="O20" s="1"/>
     </row>
     <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="41" t="s">
-        <v>51</v>
-      </c>
       <c r="C21" s="41">
         <v>8.048</v>
       </c>
       <c r="D21" s="41">
         <v>7.9409999999999998</v>
       </c>
-      <c r="E21" s="50">
+      <c r="E21" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="50">
         <f>C21*1.2+D21*1.6</f>
         <v>22.363199999999999</v>
       </c>
-      <c r="F21" s="49"/>
       <c r="G21" s="53"/>
       <c r="H21" s="48" t="s">
         <v>55</v>
@@ -3754,11 +3753,16 @@
       <c r="I21" s="51" t="s">
         <v>41</v>
       </c>
+      <c r="K21" s="73" t="s">
+        <v>76</v>
+      </c>
+      <c r="L21" s="74" t="s">
+        <v>54</v>
+      </c>
       <c r="N21" s="2"/>
       <c r="O21" s="1"/>
     </row>
     <row r="22" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="43"/>
       <c r="G22" s="1"/>
       <c r="H22" s="55" t="s">
         <v>56</v>
@@ -3766,6 +3770,12 @@
       <c r="I22" s="55" t="s">
         <v>48</v>
       </c>
+      <c r="K22" s="71">
+        <v>19.78</v>
+      </c>
+      <c r="L22" s="71" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H23" s="43"/>
@@ -3775,11 +3785,11 @@
       <c r="H24" s="43"/>
       <c r="I24" s="43"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H25" s="43"/>
       <c r="I25" s="43"/>
     </row>
-    <row r="26" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="54" t="s">
         <v>42</v>
       </c>
@@ -3789,14 +3799,20 @@
       <c r="D26" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H26" s="43"/>
+      <c r="H26" s="52" t="s">
+        <v>67</v>
+      </c>
       <c r="I26" s="43"/>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H27" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="I27" s="42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>43</v>
       </c>
@@ -3804,9 +3820,15 @@
         <v>47</v>
       </c>
       <c r="F28" s="56"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
+      <c r="G28" s="80" t="s">
+        <v>75</v>
+      </c>
+      <c r="H28" s="80">
+        <v>1.5369999999999999</v>
+      </c>
+      <c r="I28" s="76">
+        <v>0.47599999999999998</v>
+      </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
@@ -3859,7 +3881,7 @@
       <c r="N32" s="48"/>
       <c r="O32" s="51"/>
     </row>
-    <row r="33" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="28"/>
       <c r="G33" s="1"/>
       <c r="H33" s="43"/>
@@ -3871,7 +3893,7 @@
       <c r="N33" s="48"/>
       <c r="O33" s="51"/>
     </row>
-    <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="69"/>
       <c r="D34" s="69"/>
       <c r="G34" s="31"/>
@@ -3879,15 +3901,15 @@
         <v>39</v>
       </c>
       <c r="I34" s="57"/>
-      <c r="K34" s="78" t="s">
+      <c r="K34" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="L34" s="78"/>
-      <c r="M34" s="78"/>
+      <c r="L34" s="79"/>
+      <c r="M34" s="79"/>
       <c r="N34" s="48"/>
       <c r="O34" s="48"/>
     </row>
-    <row r="35" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="47" t="s">
         <v>52</v>
       </c>
@@ -3910,19 +3932,25 @@
       <c r="I35" s="52">
         <v>4.5599999999999996</v>
       </c>
-      <c r="K35" s="73"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="73" t="s">
+        <v>77</v>
+      </c>
       <c r="L35" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="M35" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="M35" s="73" t="s">
+      <c r="N35" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="N35" s="73" t="s">
+      <c r="O35" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="O35" s="70"/>
-    </row>
-    <row r="36" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="P35" s="70"/>
+    </row>
+    <row r="36" spans="2:16" ht="15" x14ac:dyDescent="0.25">
       <c r="B36" s="44" t="s">
         <v>50</v>
       </c>
@@ -3946,19 +3974,25 @@
       <c r="I36" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="K36" s="71"/>
-      <c r="L36" s="14" t="s">
-        <v>63</v>
+      <c r="J36" s="51"/>
+      <c r="K36" s="71">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L36" s="71">
+        <v>16.66</v>
       </c>
       <c r="M36" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="N36" s="14">
-        <v>33.42</v>
-      </c>
-      <c r="O36" s="48"/>
-    </row>
-    <row r="37" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N36" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="O36" s="14">
+        <v>88.97</v>
+      </c>
+      <c r="P36" s="48"/>
+    </row>
+    <row r="37" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="41" t="s">
         <v>51</v>
       </c>
@@ -3985,7 +4019,7 @@
       <c r="L37" s="2"/>
       <c r="O37" s="73"/>
     </row>
-    <row r="38" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" ht="15" x14ac:dyDescent="0.25">
       <c r="C38" s="68"/>
       <c r="D38" s="68"/>
       <c r="F38" s="49"/>
@@ -4004,7 +4038,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="44"/>
       <c r="G39" s="1"/>
       <c r="H39" s="55" t="s">
@@ -4020,12 +4054,12 @@
         <v>45.09</v>
       </c>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C40" s="44"/>
       <c r="H40" s="43"/>
       <c r="I40" s="43"/>
     </row>
-    <row r="41" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="44"/>
       <c r="F41" s="1">
         <v>1.4098999999999999</v>
@@ -4041,7 +4075,7 @@
         <v>21.695559999999997</v>
       </c>
     </row>
-    <row r="42" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="44"/>
       <c r="F42" s="1">
         <v>3.2690000000000001</v>
@@ -4061,7 +4095,7 @@
       </c>
       <c r="L42" s="75"/>
     </row>
-    <row r="43" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="44"/>
       <c r="F43" s="56"/>
       <c r="G43" s="56"/>
@@ -4073,11 +4107,14 @@
       <c r="L43" s="42" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M43" s="42" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H44" s="43"/>
       <c r="I44" s="43"/>
-      <c r="J44" s="76" t="s">
+      <c r="J44" s="77" t="s">
         <v>70</v>
       </c>
       <c r="K44" s="52">
@@ -4086,8 +4123,11 @@
       <c r="L44" s="42">
         <v>1.58</v>
       </c>
-    </row>
-    <row r="45" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M44" s="42">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="54" t="s">
         <v>42</v>
       </c>
@@ -4103,19 +4143,22 @@
       <c r="J45" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="K45" s="77">
-        <v>4.5599999999999996</v>
+      <c r="K45" s="78">
+        <v>4.9000000000000004</v>
       </c>
       <c r="L45" s="55">
-        <v>1.58</v>
-      </c>
-    </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1.68</v>
+      </c>
+      <c r="M45" s="55">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="G46" s="1"/>
       <c r="H46" s="43"/>
       <c r="I46" s="43"/>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>60</v>
       </c>
@@ -4126,7 +4169,7 @@
       <c r="H47" s="43"/>
       <c r="I47" s="43"/>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>21</v>
       </c>
@@ -4137,7 +4180,7 @@
       <c r="H48" s="43"/>
       <c r="I48" s="43"/>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>20</v>
       </c>
@@ -4148,7 +4191,7 @@
       <c r="H49" s="43"/>
       <c r="I49" s="43"/>
     </row>
-    <row r="50" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:16" ht="15" x14ac:dyDescent="0.25">
       <c r="G50" s="1"/>
       <c r="H50" s="43"/>
       <c r="I50" s="43"/>
@@ -4159,7 +4202,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G51" s="31"/>
       <c r="H51" s="43"/>
       <c r="I51" s="43"/>
@@ -4170,7 +4213,7 @@
         <v>45.09</v>
       </c>
     </row>
-    <row r="52" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="47" t="s">
         <v>52</v>
       </c>
@@ -4192,7 +4235,7 @@
       </c>
       <c r="I52" s="57"/>
     </row>
-    <row r="53" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="44" t="s">
         <v>50</v>
       </c>
@@ -4217,22 +4260,25 @@
         <v>4.5599999999999996</v>
       </c>
       <c r="K53" s="73" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="L53" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="M53" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="M53" s="73" t="s">
+      <c r="N53" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="N53" s="73" t="s">
+      <c r="O53" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="O53" s="74" t="s">
+      <c r="P53" s="74" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="41" t="s">
         <v>51</v>
       </c>
@@ -4257,22 +4303,25 @@
         <v>40</v>
       </c>
       <c r="K54" s="71">
-        <v>4.5599999999999996</v>
-      </c>
-      <c r="L54" s="14" t="s">
-        <v>63</v>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L54" s="71">
+        <v>14.66</v>
       </c>
       <c r="M54" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="N54" s="14">
-        <v>40.1</v>
-      </c>
-      <c r="O54" s="14" t="s">
+      <c r="N54" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="O54" s="14">
+        <v>95.65</v>
+      </c>
+      <c r="P54" s="14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D55" s="2"/>
       <c r="G55" s="1"/>
       <c r="H55" s="48" t="s">
@@ -4282,7 +4331,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
       <c r="G56" s="1"/>
       <c r="H56" s="48" t="s">
         <v>55</v>
@@ -4291,7 +4340,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H57" s="55" t="s">
         <v>56</v>
       </c>
@@ -4314,7 +4363,7 @@
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="J11:J12"/>
-    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="E19:E20"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="D7:D8"/>

</xml_diff>

<commit_message>
Me da pajita hacer todos los comits jeje
</commit_message>
<xml_diff>
--- a/Tarea 06/Vigas.xlsx
+++ b/Tarea 06/Vigas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ramos Ingenieria\12° Semestre\Proyecto de Hormigón Armado\Tarea 06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16725AF5-0FAD-4322-BF84-360E6E927CC3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF69467-C737-470F-B2C4-27F5A8F980D4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{B94BBB90-C174-4AC8-BDFB-4A9825C26EEC}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="79">
   <si>
     <t>0101</t>
   </si>
@@ -272,7 +272,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,6 +300,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -646,10 +653,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -881,9 +889,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3122,10 +3134,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F51FF3-724F-45F5-8F3F-FC55661E6BD0}">
-  <dimension ref="B2:P57"/>
+  <dimension ref="B2:Q57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43:M45"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -3136,7 +3148,9 @@
     <col min="7" max="7" width="18.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="14" width="16.42578125" style="1" customWidth="1"/>
     <col min="15" max="15" width="16.42578125" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="1"/>
+    <col min="16" max="16" width="9.140625" style="1"/>
+    <col min="17" max="17" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="15" x14ac:dyDescent="0.25">
@@ -3640,7 +3654,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="17" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G17" s="1"/>
       <c r="H17" s="57" t="s">
         <v>39</v>
@@ -3649,7 +3663,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="2"/>
     </row>
-    <row r="18" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="47" t="s">
         <v>19</v>
       </c>
@@ -3669,14 +3683,17 @@
       <c r="L18" s="74" t="s">
         <v>53</v>
       </c>
+      <c r="M18" s="73" t="s">
+        <v>74</v>
+      </c>
       <c r="O18" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="P18" s="74" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P18" s="73" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
         <v>7.7839999999999998</v>
       </c>
@@ -3703,14 +3720,25 @@
       <c r="L19" s="71" t="s">
         <v>63</v>
       </c>
+      <c r="M19" s="14">
+        <v>23.67</v>
+      </c>
+      <c r="N19" s="81">
+        <f>(M19-F19)/F19</f>
+        <v>7.2166255979127555E-2</v>
+      </c>
       <c r="O19" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="P19" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="P19" s="14">
+        <v>26.65</v>
+      </c>
+      <c r="Q19" s="81">
+        <f>(P19-F21)/F21</f>
+        <v>0.19168991915289402</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" ht="15" x14ac:dyDescent="0.25">
       <c r="C20" s="44">
         <v>-11.079000000000001</v>
       </c>
@@ -3732,7 +3760,7 @@
       <c r="N20" s="2"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="41">
         <v>8.048</v>
       </c>
@@ -3759,10 +3787,13 @@
       <c r="L21" s="74" t="s">
         <v>54</v>
       </c>
+      <c r="M21" s="73" t="s">
+        <v>74</v>
+      </c>
       <c r="N21" s="2"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G22" s="1"/>
       <c r="H22" s="55" t="s">
         <v>56</v>
@@ -3776,20 +3807,27 @@
       <c r="L22" s="71" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="M22" s="14">
+        <v>37.43</v>
+      </c>
+      <c r="N22" s="81">
+        <f>(-F20-M22)/F20</f>
+        <v>0.21046504107108219</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="H23" s="43"/>
       <c r="I23" s="43"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="H24" s="43"/>
       <c r="I24" s="43"/>
     </row>
-    <row r="25" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H25" s="43"/>
       <c r="I25" s="43"/>
     </row>
-    <row r="26" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="54" t="s">
         <v>42</v>
       </c>
@@ -3804,7 +3842,7 @@
       </c>
       <c r="I26" s="43"/>
     </row>
-    <row r="27" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H27" s="42" t="s">
         <v>68</v>
       </c>
@@ -3812,7 +3850,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>43</v>
       </c>
@@ -3830,7 +3868,7 @@
         <v>0.47599999999999998</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>21</v>
       </c>
@@ -3840,7 +3878,7 @@
       <c r="H29" s="43"/>
       <c r="I29" s="43"/>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>44</v>
       </c>
@@ -3852,7 +3890,7 @@
       <c r="I30" s="28"/>
       <c r="J30" s="28"/>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>45</v>
       </c>
@@ -3864,7 +3902,7 @@
       <c r="I31" s="28"/>
       <c r="J31" s="28"/>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>20</v>
       </c>
@@ -3881,7 +3919,7 @@
       <c r="N32" s="48"/>
       <c r="O32" s="51"/>
     </row>
-    <row r="33" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="28"/>
       <c r="G33" s="1"/>
       <c r="H33" s="43"/>
@@ -3893,7 +3931,7 @@
       <c r="N33" s="48"/>
       <c r="O33" s="51"/>
     </row>
-    <row r="34" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="69"/>
       <c r="D34" s="69"/>
       <c r="G34" s="31"/>
@@ -3909,7 +3947,7 @@
       <c r="N34" s="48"/>
       <c r="O34" s="48"/>
     </row>
-    <row r="35" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="47" t="s">
         <v>52</v>
       </c>
@@ -3950,7 +3988,7 @@
       </c>
       <c r="P35" s="70"/>
     </row>
-    <row r="36" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:17" ht="15" x14ac:dyDescent="0.25">
       <c r="B36" s="44" t="s">
         <v>50</v>
       </c>
@@ -3991,8 +4029,12 @@
         <v>88.97</v>
       </c>
       <c r="P36" s="48"/>
-    </row>
-    <row r="37" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q36" s="81">
+        <f>(O36-F36)/F36</f>
+        <v>3.1017616782876334</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="41" t="s">
         <v>51</v>
       </c>
@@ -4019,7 +4061,7 @@
       <c r="L37" s="2"/>
       <c r="O37" s="73"/>
     </row>
-    <row r="38" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:17" ht="15" x14ac:dyDescent="0.25">
       <c r="C38" s="68"/>
       <c r="D38" s="68"/>
       <c r="F38" s="49"/>
@@ -4038,7 +4080,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="44"/>
       <c r="G39" s="1"/>
       <c r="H39" s="55" t="s">
@@ -4053,13 +4095,17 @@
       <c r="O39" s="14">
         <v>45.09</v>
       </c>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q39" s="81">
+        <f>(O39-F37)/F37</f>
+        <v>0.52481914542493424</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C40" s="44"/>
       <c r="H40" s="43"/>
       <c r="I40" s="43"/>
     </row>
-    <row r="41" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="44"/>
       <c r="F41" s="1">
         <v>1.4098999999999999</v>
@@ -4075,7 +4121,7 @@
         <v>21.695559999999997</v>
       </c>
     </row>
-    <row r="42" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="44"/>
       <c r="F42" s="1">
         <v>3.2690000000000001</v>
@@ -4095,7 +4141,7 @@
       </c>
       <c r="L42" s="75"/>
     </row>
-    <row r="43" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="44"/>
       <c r="F43" s="56"/>
       <c r="G43" s="56"/>
@@ -4111,7 +4157,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="H44" s="43"/>
       <c r="I44" s="43"/>
       <c r="J44" s="77" t="s">
@@ -4127,7 +4173,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="45" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="54" t="s">
         <v>42</v>
       </c>
@@ -4153,12 +4199,12 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
       <c r="G46" s="1"/>
       <c r="H46" s="43"/>
       <c r="I46" s="43"/>
     </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>60</v>
       </c>
@@ -4169,7 +4215,7 @@
       <c r="H47" s="43"/>
       <c r="I47" s="43"/>
     </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>21</v>
       </c>
@@ -4180,7 +4226,7 @@
       <c r="H48" s="43"/>
       <c r="I48" s="43"/>
     </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>20</v>
       </c>
@@ -4191,7 +4237,7 @@
       <c r="H49" s="43"/>
       <c r="I49" s="43"/>
     </row>
-    <row r="50" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:17" ht="15" x14ac:dyDescent="0.25">
       <c r="G50" s="1"/>
       <c r="H50" s="43"/>
       <c r="I50" s="43"/>
@@ -4202,7 +4248,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G51" s="31"/>
       <c r="H51" s="43"/>
       <c r="I51" s="43"/>
@@ -4212,8 +4258,12 @@
       <c r="O51" s="14">
         <v>45.09</v>
       </c>
-    </row>
-    <row r="52" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q51" s="81">
+        <f>(O51-F54)/F54</f>
+        <v>2.4689471910682874</v>
+      </c>
+    </row>
+    <row r="52" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="47" t="s">
         <v>52</v>
       </c>
@@ -4235,7 +4285,7 @@
       </c>
       <c r="I52" s="57"/>
     </row>
-    <row r="53" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="44" t="s">
         <v>50</v>
       </c>
@@ -4274,11 +4324,9 @@
       <c r="O53" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="P53" s="74" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P53" s="74"/>
+    </row>
+    <row r="54" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="41" t="s">
         <v>51</v>
       </c>
@@ -4317,11 +4365,13 @@
       <c r="O54" s="14">
         <v>95.65</v>
       </c>
-      <c r="P54" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P54" s="14"/>
+      <c r="Q54" s="81">
+        <f>(O54-F53)/F53</f>
+        <v>3.1308965146721328</v>
+      </c>
+    </row>
+    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D55" s="2"/>
       <c r="G55" s="1"/>
       <c r="H55" s="48" t="s">
@@ -4331,7 +4381,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
       <c r="G56" s="1"/>
       <c r="H56" s="48" t="s">
         <v>55</v>
@@ -4340,7 +4390,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H57" s="55" t="s">
         <v>56</v>
       </c>

</xml_diff>